<commit_message>
Updated 2025 tab to include 'By Artist' column for top tracks:
</commit_message>
<xml_diff>
--- a/excel/spotify_listening_report_2025.xlsx
+++ b/excel/spotify_listening_report_2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermitchell/Documents/projects/projects_2025/analytics_projects/Spotify_Sandbox/spotify_sandbox_github/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C201B7E-A7AF-B64B-8B8B-F53F9C11B385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360F54A3-D90D-B748-A0FB-B20AA74B958A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39360" yWindow="220" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{02962024-D185-E646-89C4-A67A4B8F8E62}"/>
+    <workbookView xWindow="30240" yWindow="-1960" windowWidth="38400" windowHeight="21600" xr2:uid="{02962024-D185-E646-89C4-A67A4B8F8E62}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Overview" sheetId="13" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="526">
   <si>
     <t>Based on Spotify Extended Streaming History Time Listened (Music Only)</t>
   </si>
@@ -2368,12 +2368,12 @@
   <sheetPr>
     <tabColor rgb="FFCFC7FF"/>
   </sheetPr>
-  <dimension ref="A1:N106"/>
+  <dimension ref="A1:O106"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G32" sqref="G32"/>
-      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomLeft" activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2383,15 +2383,16 @@
     <col min="3" max="3" width="13.83203125" customWidth="1"/>
     <col min="4" max="4" width="3" customWidth="1"/>
     <col min="5" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="57.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" style="51" customWidth="1"/>
-    <col min="8" max="8" width="3" customWidth="1"/>
-    <col min="9" max="9" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="51.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.83203125" style="51" customWidth="1"/>
+    <col min="6" max="6" width="38.5" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" style="51" customWidth="1"/>
+    <col min="9" max="9" width="3" customWidth="1"/>
+    <col min="10" max="10" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="51.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.83203125" style="51" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="52" t="s">
         <v>295</v>
       </c>
@@ -2405,8 +2406,9 @@
       <c r="I1" s="52"/>
       <c r="J1" s="52"/>
       <c r="K1" s="52"/>
-    </row>
-    <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L1" s="52"/>
+    </row>
+    <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
@@ -2420,8 +2422,9 @@
       <c r="I2" s="53"/>
       <c r="J2" s="53"/>
       <c r="K2" s="53"/>
-    </row>
-    <row r="3" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L2" s="53"/>
+    </row>
+    <row r="3" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="54" t="s">
         <v>1</v>
       </c>
@@ -2435,21 +2438,23 @@
       <c r="I3" s="54"/>
       <c r="J3" s="54"/>
       <c r="K3" s="54"/>
-    </row>
-    <row r="4" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L3" s="54"/>
+    </row>
+    <row r="4" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="22"/>
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
       <c r="F4" s="23"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
       <c r="I4" s="23"/>
       <c r="J4" s="23"/>
-      <c r="K4" s="24"/>
-    </row>
-    <row r="5" spans="1:14" s="25" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="23"/>
+      <c r="L4" s="24"/>
+    </row>
+    <row r="5" spans="1:15" s="25" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="55" t="s">
         <v>196</v>
       </c>
@@ -2460,13 +2465,14 @@
       </c>
       <c r="F5" s="55"/>
       <c r="G5" s="55"/>
-      <c r="I5" s="55" t="s">
+      <c r="H5" s="55"/>
+      <c r="J5" s="55" t="s">
         <v>297</v>
       </c>
-      <c r="J5" s="55"/>
       <c r="K5" s="55"/>
-    </row>
-    <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L5" s="55"/>
+    </row>
+    <row r="6" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
         <v>2</v>
       </c>
@@ -2482,20 +2488,23 @@
       <c r="F6" s="4" t="s">
         <v>488</v>
       </c>
-      <c r="G6" s="28" t="s">
+      <c r="G6" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="H6" s="28" t="s">
         <v>197</v>
       </c>
-      <c r="I6" s="26" t="s">
+      <c r="J6" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>489</v>
       </c>
-      <c r="K6" s="28" t="s">
+      <c r="L6" s="28" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="29">
         <v>1</v>
       </c>
@@ -2512,21 +2521,22 @@
       <c r="F7" s="30" t="s">
         <v>298</v>
       </c>
-      <c r="G7" s="33">
+      <c r="G7" s="30"/>
+      <c r="H7" s="33">
         <v>162.39576666666667</v>
       </c>
-      <c r="H7" s="32"/>
-      <c r="I7" s="29">
+      <c r="I7" s="32"/>
+      <c r="J7" s="29">
         <v>1</v>
       </c>
-      <c r="J7" s="30" t="s">
+      <c r="K7" s="30" t="s">
         <v>298</v>
       </c>
-      <c r="K7" s="33">
+      <c r="L7" s="33">
         <v>756.05693333333329</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="34">
         <v>2</v>
       </c>
@@ -2543,21 +2553,22 @@
       <c r="F8" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="G8" s="36">
+      <c r="G8" s="10"/>
+      <c r="H8" s="36">
         <v>136.98431666666667</v>
       </c>
-      <c r="H8" s="32"/>
-      <c r="I8" s="34">
+      <c r="I8" s="32"/>
+      <c r="J8" s="34">
         <v>2</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="K8" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="K8" s="36">
+      <c r="L8" s="36">
         <v>646.74423333333334</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="34">
         <v>3</v>
       </c>
@@ -2574,21 +2585,22 @@
       <c r="F9" s="10" t="s">
         <v>301</v>
       </c>
-      <c r="G9" s="36">
+      <c r="G9" s="10"/>
+      <c r="H9" s="36">
         <v>129.39758333333333</v>
       </c>
-      <c r="H9" s="32"/>
-      <c r="I9" s="34">
+      <c r="I9" s="32"/>
+      <c r="J9" s="34">
         <v>3</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="K9" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="K9" s="36">
+      <c r="L9" s="36">
         <v>534.33128333333332</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="34">
         <v>4</v>
       </c>
@@ -2605,21 +2617,22 @@
       <c r="F10" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="G10" s="36">
+      <c r="G10" s="10"/>
+      <c r="H10" s="36">
         <v>120.67485000000001</v>
       </c>
-      <c r="H10" s="32"/>
-      <c r="I10" s="34">
+      <c r="I10" s="32"/>
+      <c r="J10" s="34">
         <v>4</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="K10" s="10" t="s">
         <v>304</v>
       </c>
-      <c r="K10" s="36">
+      <c r="L10" s="36">
         <v>510.32485000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="34">
         <v>5</v>
       </c>
@@ -2636,22 +2649,23 @@
       <c r="F11" s="10" t="s">
         <v>305</v>
       </c>
-      <c r="G11" s="36">
+      <c r="G11" s="10"/>
+      <c r="H11" s="36">
         <v>116.45350000000001</v>
       </c>
-      <c r="H11" s="32"/>
-      <c r="I11" s="34">
+      <c r="I11" s="32"/>
+      <c r="J11" s="34">
         <v>5</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="K11" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="K11" s="36">
+      <c r="L11" s="36">
         <v>453.36713333333336</v>
       </c>
-      <c r="N11" s="37"/>
-    </row>
-    <row r="12" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O11" s="37"/>
+    </row>
+    <row r="12" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="38">
         <v>6</v>
       </c>
@@ -2668,21 +2682,22 @@
       <c r="F12" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="G12" s="40">
+      <c r="G12" s="16"/>
+      <c r="H12" s="40">
         <v>110.51224999999999</v>
       </c>
-      <c r="H12" s="32"/>
-      <c r="I12" s="38">
+      <c r="I12" s="32"/>
+      <c r="J12" s="38">
         <v>6</v>
       </c>
-      <c r="J12" s="16" t="s">
+      <c r="K12" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="K12" s="40">
+      <c r="L12" s="40">
         <v>428.76588333333331</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="38">
         <v>7</v>
       </c>
@@ -2699,21 +2714,22 @@
       <c r="F13" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="G13" s="40">
+      <c r="G13" s="16"/>
+      <c r="H13" s="40">
         <v>110.18210000000001</v>
       </c>
-      <c r="H13" s="32"/>
-      <c r="I13" s="38">
+      <c r="I13" s="32"/>
+      <c r="J13" s="38">
         <v>7</v>
       </c>
-      <c r="J13" s="16" t="s">
+      <c r="K13" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="K13" s="40">
+      <c r="L13" s="40">
         <v>370.43581666666665</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="38">
         <v>8</v>
       </c>
@@ -2730,21 +2746,22 @@
       <c r="F14" s="16" t="s">
         <v>311</v>
       </c>
-      <c r="G14" s="40">
+      <c r="G14" s="16"/>
+      <c r="H14" s="40">
         <v>101.7728</v>
       </c>
-      <c r="H14" s="32"/>
-      <c r="I14" s="38">
+      <c r="I14" s="32"/>
+      <c r="J14" s="38">
         <v>8</v>
       </c>
-      <c r="J14" s="16" t="s">
+      <c r="K14" s="16" t="s">
         <v>312</v>
       </c>
-      <c r="K14" s="40">
+      <c r="L14" s="40">
         <v>345.12774999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="38">
         <v>9</v>
       </c>
@@ -2761,21 +2778,22 @@
       <c r="F15" s="16" t="s">
         <v>313</v>
       </c>
-      <c r="G15" s="40">
+      <c r="G15" s="16"/>
+      <c r="H15" s="40">
         <v>88.796733333333336</v>
       </c>
-      <c r="H15" s="32"/>
-      <c r="I15" s="38">
+      <c r="I15" s="32"/>
+      <c r="J15" s="38">
         <v>9</v>
       </c>
-      <c r="J15" s="16" t="s">
+      <c r="K15" s="16" t="s">
         <v>314</v>
       </c>
-      <c r="K15" s="40">
+      <c r="L15" s="40">
         <v>340.55865</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="38">
         <v>10</v>
       </c>
@@ -2792,21 +2810,22 @@
       <c r="F16" s="16" t="s">
         <v>315</v>
       </c>
-      <c r="G16" s="40">
+      <c r="G16" s="16"/>
+      <c r="H16" s="40">
         <v>87.560916666666671</v>
       </c>
-      <c r="H16" s="32"/>
-      <c r="I16" s="38">
+      <c r="I16" s="32"/>
+      <c r="J16" s="38">
         <v>10</v>
       </c>
-      <c r="J16" s="16" t="s">
+      <c r="K16" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="K16" s="40">
+      <c r="L16" s="40">
         <v>314.25976666666668</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="41">
         <v>11</v>
       </c>
@@ -2823,21 +2842,22 @@
       <c r="F17" s="18" t="s">
         <v>317</v>
       </c>
-      <c r="G17" s="43">
+      <c r="G17" s="18"/>
+      <c r="H17" s="43">
         <v>78.673066666666671</v>
       </c>
-      <c r="H17" s="32"/>
-      <c r="I17" s="41">
+      <c r="I17" s="32"/>
+      <c r="J17" s="41">
         <v>11</v>
       </c>
-      <c r="J17" s="18" t="s">
+      <c r="K17" s="18" t="s">
         <v>318</v>
       </c>
-      <c r="K17" s="43">
+      <c r="L17" s="43">
         <v>303.03643333333332</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="41">
         <v>12</v>
       </c>
@@ -2854,21 +2874,22 @@
       <c r="F18" s="18" t="s">
         <v>319</v>
       </c>
-      <c r="G18" s="43">
+      <c r="G18" s="18"/>
+      <c r="H18" s="43">
         <v>75.114450000000005</v>
       </c>
-      <c r="H18" s="32"/>
-      <c r="I18" s="41">
+      <c r="I18" s="32"/>
+      <c r="J18" s="41">
         <v>12</v>
       </c>
-      <c r="J18" s="18" t="s">
+      <c r="K18" s="18" t="s">
         <v>320</v>
       </c>
-      <c r="K18" s="43">
+      <c r="L18" s="43">
         <v>298.90123333333332</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="41">
         <v>13</v>
       </c>
@@ -2885,21 +2906,22 @@
       <c r="F19" s="18" t="s">
         <v>321</v>
       </c>
-      <c r="G19" s="43">
+      <c r="G19" s="18"/>
+      <c r="H19" s="43">
         <v>75.044650000000004</v>
       </c>
-      <c r="H19" s="32"/>
-      <c r="I19" s="41">
+      <c r="I19" s="32"/>
+      <c r="J19" s="41">
         <v>13</v>
       </c>
-      <c r="J19" s="18" t="s">
+      <c r="K19" s="18" t="s">
         <v>322</v>
       </c>
-      <c r="K19" s="43">
+      <c r="L19" s="43">
         <v>254.97268333333332</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="41">
         <v>14</v>
       </c>
@@ -2916,21 +2938,22 @@
       <c r="F20" s="18" t="s">
         <v>323</v>
       </c>
-      <c r="G20" s="43">
+      <c r="G20" s="18"/>
+      <c r="H20" s="43">
         <v>73.818983333333335</v>
       </c>
-      <c r="H20" s="32"/>
-      <c r="I20" s="41">
+      <c r="I20" s="32"/>
+      <c r="J20" s="41">
         <v>14</v>
       </c>
-      <c r="J20" s="18" t="s">
+      <c r="K20" s="18" t="s">
         <v>324</v>
       </c>
-      <c r="K20" s="43">
+      <c r="L20" s="43">
         <v>246.61775</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="41">
         <v>15</v>
       </c>
@@ -2947,21 +2970,22 @@
       <c r="F21" s="18" t="s">
         <v>325</v>
       </c>
-      <c r="G21" s="43">
+      <c r="G21" s="18"/>
+      <c r="H21" s="43">
         <v>70.979200000000006</v>
       </c>
-      <c r="H21" s="32"/>
-      <c r="I21" s="41">
+      <c r="I21" s="32"/>
+      <c r="J21" s="41">
         <v>15</v>
       </c>
-      <c r="J21" s="18" t="s">
+      <c r="K21" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="K21" s="43">
+      <c r="L21" s="43">
         <v>229.86106666666666</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="41">
         <v>16</v>
       </c>
@@ -2978,21 +3002,22 @@
       <c r="F22" s="18" t="s">
         <v>326</v>
       </c>
-      <c r="G22" s="43">
+      <c r="G22" s="18"/>
+      <c r="H22" s="43">
         <v>69.502650000000003</v>
       </c>
-      <c r="H22" s="32"/>
-      <c r="I22" s="41">
+      <c r="I22" s="32"/>
+      <c r="J22" s="41">
         <v>16</v>
       </c>
-      <c r="J22" s="18" t="s">
+      <c r="K22" s="18" t="s">
         <v>327</v>
       </c>
-      <c r="K22" s="43">
+      <c r="L22" s="43">
         <v>220.91378333333333</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="41">
         <v>17</v>
       </c>
@@ -3009,21 +3034,22 @@
       <c r="F23" s="18" t="s">
         <v>328</v>
       </c>
-      <c r="G23" s="43">
+      <c r="G23" s="18"/>
+      <c r="H23" s="43">
         <v>69.15176666666666</v>
       </c>
-      <c r="H23" s="32"/>
-      <c r="I23" s="41">
+      <c r="I23" s="32"/>
+      <c r="J23" s="41">
         <v>17</v>
       </c>
-      <c r="J23" s="18" t="s">
+      <c r="K23" s="18" t="s">
         <v>329</v>
       </c>
-      <c r="K23" s="43">
+      <c r="L23" s="43">
         <v>214.35374999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="41">
         <v>18</v>
       </c>
@@ -3040,21 +3066,22 @@
       <c r="F24" s="18" t="s">
         <v>330</v>
       </c>
-      <c r="G24" s="43">
+      <c r="G24" s="18"/>
+      <c r="H24" s="43">
         <v>68.841333333333338</v>
       </c>
-      <c r="H24" s="32"/>
-      <c r="I24" s="41">
+      <c r="I24" s="32"/>
+      <c r="J24" s="41">
         <v>18</v>
       </c>
-      <c r="J24" s="18" t="s">
+      <c r="K24" s="18" t="s">
         <v>331</v>
       </c>
-      <c r="K24" s="43">
+      <c r="L24" s="43">
         <v>183.71451666666667</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="41">
         <v>19</v>
       </c>
@@ -3071,21 +3098,22 @@
       <c r="F25" s="18" t="s">
         <v>332</v>
       </c>
-      <c r="G25" s="43">
+      <c r="G25" s="18"/>
+      <c r="H25" s="43">
         <v>68.576466666666661</v>
       </c>
-      <c r="H25" s="32"/>
-      <c r="I25" s="41">
+      <c r="I25" s="32"/>
+      <c r="J25" s="41">
         <v>19</v>
       </c>
-      <c r="J25" s="18" t="s">
+      <c r="K25" s="18" t="s">
         <v>333</v>
       </c>
-      <c r="K25" s="43">
+      <c r="L25" s="43">
         <v>178.04235</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="41">
         <v>20</v>
       </c>
@@ -3102,21 +3130,22 @@
       <c r="F26" s="18" t="s">
         <v>334</v>
       </c>
-      <c r="G26" s="43">
+      <c r="G26" s="18"/>
+      <c r="H26" s="43">
         <v>66.407483333333332</v>
       </c>
-      <c r="H26" s="32"/>
-      <c r="I26" s="41">
+      <c r="I26" s="32"/>
+      <c r="J26" s="41">
         <v>20</v>
       </c>
-      <c r="J26" s="18" t="s">
+      <c r="K26" s="18" t="s">
         <v>335</v>
       </c>
-      <c r="K26" s="43">
+      <c r="L26" s="43">
         <v>168.90061666666668</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="44">
         <v>21</v>
       </c>
@@ -3133,21 +3162,22 @@
       <c r="F27" s="20" t="s">
         <v>336</v>
       </c>
-      <c r="G27" s="46">
+      <c r="G27" s="20"/>
+      <c r="H27" s="46">
         <v>65.699233333333339</v>
       </c>
-      <c r="H27" s="32"/>
-      <c r="I27" s="44">
+      <c r="I27" s="32"/>
+      <c r="J27" s="44">
         <v>21</v>
       </c>
-      <c r="J27" s="20" t="s">
+      <c r="K27" s="20" t="s">
         <v>337</v>
       </c>
-      <c r="K27" s="46">
+      <c r="L27" s="46">
         <v>168.52018333333334</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="44">
         <v>22</v>
       </c>
@@ -3164,21 +3194,22 @@
       <c r="F28" s="20" t="s">
         <v>338</v>
       </c>
-      <c r="G28" s="46">
+      <c r="G28" s="20"/>
+      <c r="H28" s="46">
         <v>64.26421666666667</v>
       </c>
-      <c r="H28" s="32"/>
-      <c r="I28" s="44">
+      <c r="I28" s="32"/>
+      <c r="J28" s="44">
         <v>22</v>
       </c>
-      <c r="J28" s="20" t="s">
+      <c r="K28" s="20" t="s">
         <v>339</v>
       </c>
-      <c r="K28" s="46">
+      <c r="L28" s="46">
         <v>167.96270000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="44">
         <v>23</v>
       </c>
@@ -3195,21 +3226,22 @@
       <c r="F29" s="20" t="s">
         <v>340</v>
       </c>
-      <c r="G29" s="46">
+      <c r="G29" s="20"/>
+      <c r="H29" s="46">
         <v>59.984716666666664</v>
       </c>
-      <c r="H29" s="32"/>
-      <c r="I29" s="44">
+      <c r="I29" s="32"/>
+      <c r="J29" s="44">
         <v>23</v>
       </c>
-      <c r="J29" s="20" t="s">
+      <c r="K29" s="20" t="s">
         <v>341</v>
       </c>
-      <c r="K29" s="46">
+      <c r="L29" s="46">
         <v>162.22446666666667</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="44">
         <v>24</v>
       </c>
@@ -3226,21 +3258,22 @@
       <c r="F30" s="20" t="s">
         <v>342</v>
       </c>
-      <c r="G30" s="46">
+      <c r="G30" s="20"/>
+      <c r="H30" s="46">
         <v>59.591999999999999</v>
       </c>
-      <c r="H30" s="32"/>
-      <c r="I30" s="44">
+      <c r="I30" s="32"/>
+      <c r="J30" s="44">
         <v>24</v>
       </c>
-      <c r="J30" s="20" t="s">
+      <c r="K30" s="20" t="s">
         <v>343</v>
       </c>
-      <c r="K30" s="46">
+      <c r="L30" s="46">
         <v>149.07775000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="44">
         <v>25</v>
       </c>
@@ -3257,21 +3290,22 @@
       <c r="F31" s="20" t="s">
         <v>344</v>
       </c>
-      <c r="G31" s="46">
+      <c r="G31" s="20"/>
+      <c r="H31" s="46">
         <v>59.25685</v>
       </c>
-      <c r="H31" s="32"/>
-      <c r="I31" s="44">
+      <c r="I31" s="32"/>
+      <c r="J31" s="44">
         <v>25</v>
       </c>
-      <c r="J31" s="20" t="s">
+      <c r="K31" s="20" t="s">
         <v>345</v>
       </c>
-      <c r="K31" s="46">
+      <c r="L31" s="46">
         <v>148.14113333333333</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="44">
         <v>26</v>
       </c>
@@ -3288,21 +3322,22 @@
       <c r="F32" s="20" t="s">
         <v>312</v>
       </c>
-      <c r="G32" s="46">
+      <c r="G32" s="20"/>
+      <c r="H32" s="46">
         <v>58.996716666666664</v>
       </c>
-      <c r="H32" s="32"/>
-      <c r="I32" s="44">
+      <c r="I32" s="32"/>
+      <c r="J32" s="44">
         <v>26</v>
       </c>
-      <c r="J32" s="20" t="s">
+      <c r="K32" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="K32" s="46">
+      <c r="L32" s="46">
         <v>145.89376666666666</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="44">
         <v>27</v>
       </c>
@@ -3319,21 +3354,22 @@
       <c r="F33" s="20" t="s">
         <v>346</v>
       </c>
-      <c r="G33" s="46">
+      <c r="G33" s="20"/>
+      <c r="H33" s="46">
         <v>58.030183333333333</v>
       </c>
-      <c r="H33" s="32"/>
-      <c r="I33" s="44">
+      <c r="I33" s="32"/>
+      <c r="J33" s="44">
         <v>27</v>
       </c>
-      <c r="J33" s="20" t="s">
+      <c r="K33" s="20" t="s">
         <v>347</v>
       </c>
-      <c r="K33" s="46">
+      <c r="L33" s="46">
         <v>142.68594999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="44">
         <v>28</v>
       </c>
@@ -3350,21 +3386,22 @@
       <c r="F34" s="20" t="s">
         <v>348</v>
       </c>
-      <c r="G34" s="46">
+      <c r="G34" s="20"/>
+      <c r="H34" s="46">
         <v>56.381383333333332</v>
       </c>
-      <c r="H34" s="32"/>
-      <c r="I34" s="44">
+      <c r="I34" s="32"/>
+      <c r="J34" s="44">
         <v>28</v>
       </c>
-      <c r="J34" s="20" t="s">
+      <c r="K34" s="20" t="s">
         <v>349</v>
       </c>
-      <c r="K34" s="46">
+      <c r="L34" s="46">
         <v>140.49725000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="44">
         <v>29</v>
       </c>
@@ -3381,21 +3418,22 @@
       <c r="F35" s="20" t="s">
         <v>350</v>
       </c>
-      <c r="G35" s="46">
+      <c r="G35" s="20"/>
+      <c r="H35" s="46">
         <v>56.032516666666666</v>
       </c>
-      <c r="H35" s="32"/>
-      <c r="I35" s="44">
+      <c r="I35" s="32"/>
+      <c r="J35" s="44">
         <v>29</v>
       </c>
-      <c r="J35" s="20" t="s">
+      <c r="K35" s="20" t="s">
         <v>351</v>
       </c>
-      <c r="K35" s="46">
+      <c r="L35" s="46">
         <v>138.87733333333333</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="44">
         <v>30</v>
       </c>
@@ -3412,21 +3450,22 @@
       <c r="F36" s="20" t="s">
         <v>352</v>
       </c>
-      <c r="G36" s="46">
+      <c r="G36" s="20"/>
+      <c r="H36" s="46">
         <v>55.678566666666669</v>
       </c>
-      <c r="H36" s="32"/>
-      <c r="I36" s="44">
+      <c r="I36" s="32"/>
+      <c r="J36" s="44">
         <v>30</v>
       </c>
-      <c r="J36" s="20" t="s">
+      <c r="K36" s="20" t="s">
         <v>353</v>
       </c>
-      <c r="K36" s="46">
+      <c r="L36" s="46">
         <v>137.19011666666665</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="44">
         <v>31</v>
       </c>
@@ -3443,21 +3482,22 @@
       <c r="F37" s="20" t="s">
         <v>354</v>
       </c>
-      <c r="G37" s="46">
+      <c r="G37" s="20"/>
+      <c r="H37" s="46">
         <v>55.64071666666667</v>
       </c>
-      <c r="H37" s="32"/>
-      <c r="I37" s="44">
+      <c r="I37" s="32"/>
+      <c r="J37" s="44">
         <v>31</v>
       </c>
-      <c r="J37" s="20" t="s">
+      <c r="K37" s="20" t="s">
         <v>355</v>
       </c>
-      <c r="K37" s="46">
+      <c r="L37" s="46">
         <v>136.6472</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="44">
         <v>32</v>
       </c>
@@ -3474,21 +3514,22 @@
       <c r="F38" s="20" t="s">
         <v>356</v>
       </c>
-      <c r="G38" s="46">
+      <c r="G38" s="20"/>
+      <c r="H38" s="46">
         <v>54.588016666666668</v>
       </c>
-      <c r="H38" s="32"/>
-      <c r="I38" s="44">
+      <c r="I38" s="32"/>
+      <c r="J38" s="44">
         <v>32</v>
       </c>
-      <c r="J38" s="20" t="s">
+      <c r="K38" s="20" t="s">
         <v>357</v>
       </c>
-      <c r="K38" s="46">
+      <c r="L38" s="46">
         <v>134.17878333333334</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="44">
         <v>33</v>
       </c>
@@ -3505,21 +3546,22 @@
       <c r="F39" s="20" t="s">
         <v>358</v>
       </c>
-      <c r="G39" s="46">
+      <c r="G39" s="20"/>
+      <c r="H39" s="46">
         <v>53.564533333333337</v>
       </c>
-      <c r="H39" s="32"/>
-      <c r="I39" s="44">
+      <c r="I39" s="32"/>
+      <c r="J39" s="44">
         <v>33</v>
       </c>
-      <c r="J39" s="20" t="s">
+      <c r="K39" s="20" t="s">
         <v>359</v>
       </c>
-      <c r="K39" s="46">
+      <c r="L39" s="46">
         <v>130.53331666666668</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="44">
         <v>34</v>
       </c>
@@ -3536,21 +3578,22 @@
       <c r="F40" s="20" t="s">
         <v>360</v>
       </c>
-      <c r="G40" s="46">
+      <c r="G40" s="20"/>
+      <c r="H40" s="46">
         <v>50.267383333333335</v>
       </c>
-      <c r="H40" s="32"/>
-      <c r="I40" s="44">
+      <c r="I40" s="32"/>
+      <c r="J40" s="44">
         <v>34</v>
       </c>
-      <c r="J40" s="20" t="s">
+      <c r="K40" s="20" t="s">
         <v>361</v>
       </c>
-      <c r="K40" s="46">
+      <c r="L40" s="46">
         <v>128.56056666666666</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="44">
         <v>35</v>
       </c>
@@ -3567,21 +3610,22 @@
       <c r="F41" s="20" t="s">
         <v>362</v>
       </c>
-      <c r="G41" s="46">
+      <c r="G41" s="20"/>
+      <c r="H41" s="46">
         <v>50.252816666666668</v>
       </c>
-      <c r="H41" s="32"/>
-      <c r="I41" s="44">
+      <c r="I41" s="32"/>
+      <c r="J41" s="44">
         <v>35</v>
       </c>
-      <c r="J41" s="20" t="s">
+      <c r="K41" s="20" t="s">
         <v>363</v>
       </c>
-      <c r="K41" s="46">
+      <c r="L41" s="46">
         <v>128.45701666666668</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="44">
         <v>36</v>
       </c>
@@ -3598,21 +3642,22 @@
       <c r="F42" s="20" t="s">
         <v>364</v>
       </c>
-      <c r="G42" s="46">
+      <c r="G42" s="20"/>
+      <c r="H42" s="46">
         <v>49.837466666666664</v>
       </c>
-      <c r="H42" s="32"/>
-      <c r="I42" s="44">
+      <c r="I42" s="32"/>
+      <c r="J42" s="44">
         <v>36</v>
       </c>
-      <c r="J42" s="20" t="s">
+      <c r="K42" s="20" t="s">
         <v>365</v>
       </c>
-      <c r="K42" s="46">
+      <c r="L42" s="46">
         <v>128.04665</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="44">
         <v>37</v>
       </c>
@@ -3629,21 +3674,22 @@
       <c r="F43" s="20" t="s">
         <v>366</v>
       </c>
-      <c r="G43" s="46">
+      <c r="G43" s="20"/>
+      <c r="H43" s="46">
         <v>49.572749999999999</v>
       </c>
-      <c r="H43" s="32"/>
-      <c r="I43" s="44">
+      <c r="I43" s="32"/>
+      <c r="J43" s="44">
         <v>37</v>
       </c>
-      <c r="J43" s="20" t="s">
+      <c r="K43" s="20" t="s">
         <v>367</v>
       </c>
-      <c r="K43" s="46">
+      <c r="L43" s="46">
         <v>127.79783333333333</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="44">
         <v>38</v>
       </c>
@@ -3660,21 +3706,22 @@
       <c r="F44" s="20" t="s">
         <v>368</v>
       </c>
-      <c r="G44" s="46">
+      <c r="G44" s="20"/>
+      <c r="H44" s="46">
         <v>49.404616666666669</v>
       </c>
-      <c r="H44" s="32"/>
-      <c r="I44" s="44">
+      <c r="I44" s="32"/>
+      <c r="J44" s="44">
         <v>38</v>
       </c>
-      <c r="J44" s="20" t="s">
+      <c r="K44" s="20" t="s">
         <v>369</v>
       </c>
-      <c r="K44" s="46">
+      <c r="L44" s="46">
         <v>125.76916666666666</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="44">
         <v>39</v>
       </c>
@@ -3691,21 +3738,22 @@
       <c r="F45" s="20" t="s">
         <v>370</v>
       </c>
-      <c r="G45" s="46">
+      <c r="G45" s="20"/>
+      <c r="H45" s="46">
         <v>49.314399999999999</v>
       </c>
-      <c r="H45" s="32"/>
-      <c r="I45" s="44">
+      <c r="I45" s="32"/>
+      <c r="J45" s="44">
         <v>39</v>
       </c>
-      <c r="J45" s="20" t="s">
+      <c r="K45" s="20" t="s">
         <v>371</v>
       </c>
-      <c r="K45" s="46">
+      <c r="L45" s="46">
         <v>120.94031666666666</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="44">
         <v>40</v>
       </c>
@@ -3722,21 +3770,22 @@
       <c r="F46" s="20" t="s">
         <v>347</v>
       </c>
-      <c r="G46" s="46">
+      <c r="G46" s="20"/>
+      <c r="H46" s="46">
         <v>49.160766666666667</v>
       </c>
-      <c r="H46" s="32"/>
-      <c r="I46" s="44">
+      <c r="I46" s="32"/>
+      <c r="J46" s="44">
         <v>40</v>
       </c>
-      <c r="J46" s="20" t="s">
+      <c r="K46" s="20" t="s">
         <v>372</v>
       </c>
-      <c r="K46" s="46">
+      <c r="L46" s="46">
         <v>117.79996666666666</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="44">
         <v>41</v>
       </c>
@@ -3753,21 +3802,22 @@
       <c r="F47" s="20" t="s">
         <v>373</v>
       </c>
-      <c r="G47" s="46">
+      <c r="G47" s="20"/>
+      <c r="H47" s="46">
         <v>48.411149999999999</v>
       </c>
-      <c r="H47" s="32"/>
-      <c r="I47" s="44">
+      <c r="I47" s="32"/>
+      <c r="J47" s="44">
         <v>41</v>
       </c>
-      <c r="J47" s="20" t="s">
+      <c r="K47" s="20" t="s">
         <v>374</v>
       </c>
-      <c r="K47" s="46">
+      <c r="L47" s="46">
         <v>115.82810000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="44">
         <v>42</v>
       </c>
@@ -3784,21 +3834,22 @@
       <c r="F48" s="20" t="s">
         <v>375</v>
       </c>
-      <c r="G48" s="46">
+      <c r="G48" s="20"/>
+      <c r="H48" s="46">
         <v>47.83155</v>
       </c>
-      <c r="H48" s="32"/>
-      <c r="I48" s="44">
+      <c r="I48" s="32"/>
+      <c r="J48" s="44">
         <v>42</v>
       </c>
-      <c r="J48" s="20" t="s">
+      <c r="K48" s="20" t="s">
         <v>376</v>
       </c>
-      <c r="K48" s="46">
+      <c r="L48" s="46">
         <v>109.71169999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="44">
         <v>43</v>
       </c>
@@ -3815,21 +3866,22 @@
       <c r="F49" s="20" t="s">
         <v>377</v>
       </c>
-      <c r="G49" s="46">
+      <c r="G49" s="20"/>
+      <c r="H49" s="46">
         <v>47.251466666666666</v>
       </c>
-      <c r="H49" s="32"/>
-      <c r="I49" s="44">
+      <c r="I49" s="32"/>
+      <c r="J49" s="44">
         <v>43</v>
       </c>
-      <c r="J49" s="20" t="s">
+      <c r="K49" s="20" t="s">
         <v>378</v>
       </c>
-      <c r="K49" s="46">
+      <c r="L49" s="46">
         <v>108.90828333333333</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="44">
         <v>44</v>
       </c>
@@ -3846,21 +3898,22 @@
       <c r="F50" s="20" t="s">
         <v>379</v>
       </c>
-      <c r="G50" s="46">
+      <c r="G50" s="20"/>
+      <c r="H50" s="46">
         <v>46.779366666666668</v>
       </c>
-      <c r="H50" s="32"/>
-      <c r="I50" s="44">
+      <c r="I50" s="32"/>
+      <c r="J50" s="44">
         <v>44</v>
       </c>
-      <c r="J50" s="20" t="s">
+      <c r="K50" s="20" t="s">
         <v>380</v>
       </c>
-      <c r="K50" s="46">
+      <c r="L50" s="46">
         <v>106.99893333333333</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="44">
         <v>45</v>
       </c>
@@ -3877,21 +3930,22 @@
       <c r="F51" s="20" t="s">
         <v>381</v>
       </c>
-      <c r="G51" s="46">
+      <c r="G51" s="20"/>
+      <c r="H51" s="46">
         <v>46.714550000000003</v>
       </c>
-      <c r="H51" s="32"/>
-      <c r="I51" s="44">
+      <c r="I51" s="32"/>
+      <c r="J51" s="44">
         <v>45</v>
       </c>
-      <c r="J51" s="20" t="s">
+      <c r="K51" s="20" t="s">
         <v>382</v>
       </c>
-      <c r="K51" s="46">
+      <c r="L51" s="46">
         <v>106.43083333333334</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="44">
         <v>46</v>
       </c>
@@ -3908,21 +3962,22 @@
       <c r="F52" s="20" t="s">
         <v>383</v>
       </c>
-      <c r="G52" s="46">
+      <c r="G52" s="20"/>
+      <c r="H52" s="46">
         <v>45.705716666666667</v>
       </c>
-      <c r="H52" s="32"/>
-      <c r="I52" s="44">
+      <c r="I52" s="32"/>
+      <c r="J52" s="44">
         <v>46</v>
       </c>
-      <c r="J52" s="20" t="s">
+      <c r="K52" s="20" t="s">
         <v>384</v>
       </c>
-      <c r="K52" s="46">
+      <c r="L52" s="46">
         <v>105.90445</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="44">
         <v>47</v>
       </c>
@@ -3939,21 +3994,22 @@
       <c r="F53" s="20" t="s">
         <v>385</v>
       </c>
-      <c r="G53" s="46">
+      <c r="G53" s="20"/>
+      <c r="H53" s="46">
         <v>45.406366666666663</v>
       </c>
-      <c r="H53" s="32"/>
-      <c r="I53" s="44">
+      <c r="I53" s="32"/>
+      <c r="J53" s="44">
         <v>47</v>
       </c>
-      <c r="J53" s="20" t="s">
+      <c r="K53" s="20" t="s">
         <v>386</v>
       </c>
-      <c r="K53" s="46">
+      <c r="L53" s="46">
         <v>91.269866666666672</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="44">
         <v>48</v>
       </c>
@@ -3970,21 +4026,22 @@
       <c r="F54" s="20" t="s">
         <v>387</v>
       </c>
-      <c r="G54" s="46">
+      <c r="G54" s="20"/>
+      <c r="H54" s="46">
         <v>45.267933333333332</v>
       </c>
-      <c r="H54" s="32"/>
-      <c r="I54" s="44">
+      <c r="I54" s="32"/>
+      <c r="J54" s="44">
         <v>48</v>
       </c>
-      <c r="J54" s="20" t="s">
+      <c r="K54" s="20" t="s">
         <v>388</v>
       </c>
-      <c r="K54" s="46">
+      <c r="L54" s="46">
         <v>88.534833333333339</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="44">
         <v>49</v>
       </c>
@@ -4001,21 +4058,22 @@
       <c r="F55" s="20" t="s">
         <v>389</v>
       </c>
-      <c r="G55" s="46">
+      <c r="G55" s="20"/>
+      <c r="H55" s="46">
         <v>44.662799999999997</v>
       </c>
-      <c r="H55" s="32"/>
-      <c r="I55" s="44">
+      <c r="I55" s="32"/>
+      <c r="J55" s="44">
         <v>49</v>
       </c>
-      <c r="J55" s="20" t="s">
+      <c r="K55" s="20" t="s">
         <v>390</v>
       </c>
-      <c r="K55" s="46">
+      <c r="L55" s="46">
         <v>88.313266666666664</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="44">
         <v>50</v>
       </c>
@@ -4032,21 +4090,22 @@
       <c r="F56" s="20" t="s">
         <v>391</v>
       </c>
-      <c r="G56" s="46">
+      <c r="G56" s="20"/>
+      <c r="H56" s="46">
         <v>44.518883333333335</v>
       </c>
-      <c r="H56" s="32"/>
-      <c r="I56" s="44">
+      <c r="I56" s="32"/>
+      <c r="J56" s="44">
         <v>50</v>
       </c>
-      <c r="J56" s="20" t="s">
+      <c r="K56" s="20" t="s">
         <v>392</v>
       </c>
-      <c r="K56" s="46">
+      <c r="L56" s="46">
         <v>84.480833333333337</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="44">
         <v>51</v>
       </c>
@@ -4063,21 +4122,22 @@
       <c r="F57" s="20" t="s">
         <v>393</v>
       </c>
-      <c r="G57" s="46">
+      <c r="G57" s="20"/>
+      <c r="H57" s="46">
         <v>44.077500000000001</v>
       </c>
-      <c r="H57" s="32"/>
-      <c r="I57" s="44">
+      <c r="I57" s="32"/>
+      <c r="J57" s="44">
         <v>51</v>
       </c>
-      <c r="J57" s="20" t="s">
+      <c r="K57" s="20" t="s">
         <v>394</v>
       </c>
-      <c r="K57" s="46">
+      <c r="L57" s="46">
         <v>82.130449999999996</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="44">
         <v>52</v>
       </c>
@@ -4094,21 +4154,22 @@
       <c r="F58" s="20" t="s">
         <v>395</v>
       </c>
-      <c r="G58" s="46">
+      <c r="G58" s="20"/>
+      <c r="H58" s="46">
         <v>43.632866666666665</v>
       </c>
-      <c r="H58" s="32"/>
-      <c r="I58" s="44">
+      <c r="I58" s="32"/>
+      <c r="J58" s="44">
         <v>52</v>
       </c>
-      <c r="J58" s="20" t="s">
+      <c r="K58" s="20" t="s">
         <v>396</v>
       </c>
-      <c r="K58" s="46">
+      <c r="L58" s="46">
         <v>77.424366666666671</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="44">
         <v>53</v>
       </c>
@@ -4125,21 +4186,22 @@
       <c r="F59" s="20" t="s">
         <v>397</v>
       </c>
-      <c r="G59" s="46">
+      <c r="G59" s="20"/>
+      <c r="H59" s="46">
         <v>43.256316666666663</v>
       </c>
-      <c r="H59" s="32"/>
-      <c r="I59" s="44">
+      <c r="I59" s="32"/>
+      <c r="J59" s="44">
         <v>53</v>
       </c>
-      <c r="J59" s="20" t="s">
+      <c r="K59" s="20" t="s">
         <v>398</v>
       </c>
-      <c r="K59" s="46">
+      <c r="L59" s="46">
         <v>76.042216666666661</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="44">
         <v>54</v>
       </c>
@@ -4156,21 +4218,22 @@
       <c r="F60" s="20" t="s">
         <v>399</v>
       </c>
-      <c r="G60" s="46">
+      <c r="G60" s="20"/>
+      <c r="H60" s="46">
         <v>43.077449999999999</v>
       </c>
-      <c r="H60" s="32"/>
-      <c r="I60" s="44">
+      <c r="I60" s="32"/>
+      <c r="J60" s="44">
         <v>54</v>
       </c>
-      <c r="J60" s="20" t="s">
+      <c r="K60" s="20" t="s">
         <v>400</v>
       </c>
-      <c r="K60" s="46">
+      <c r="L60" s="46">
         <v>73.640483333333336</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="44">
         <v>55</v>
       </c>
@@ -4187,21 +4250,22 @@
       <c r="F61" s="20" t="s">
         <v>401</v>
       </c>
-      <c r="G61" s="46">
+      <c r="G61" s="20"/>
+      <c r="H61" s="46">
         <v>42.818533333333335</v>
       </c>
-      <c r="H61" s="32"/>
-      <c r="I61" s="44">
+      <c r="I61" s="32"/>
+      <c r="J61" s="44">
         <v>55</v>
       </c>
-      <c r="J61" s="20" t="s">
+      <c r="K61" s="20" t="s">
         <v>402</v>
       </c>
-      <c r="K61" s="46">
+      <c r="L61" s="46">
         <v>70.080966666666669</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="44">
         <v>56</v>
       </c>
@@ -4218,21 +4282,22 @@
       <c r="F62" s="20" t="s">
         <v>403</v>
       </c>
-      <c r="G62" s="46">
+      <c r="G62" s="20"/>
+      <c r="H62" s="46">
         <v>42.366599999999998</v>
       </c>
-      <c r="H62" s="32"/>
-      <c r="I62" s="44">
+      <c r="I62" s="32"/>
+      <c r="J62" s="44">
         <v>56</v>
       </c>
-      <c r="J62" s="20" t="s">
+      <c r="K62" s="20" t="s">
         <v>404</v>
       </c>
-      <c r="K62" s="46">
+      <c r="L62" s="46">
         <v>68.235749999999996</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="44">
         <v>57</v>
       </c>
@@ -4249,21 +4314,22 @@
       <c r="F63" s="20" t="s">
         <v>405</v>
       </c>
-      <c r="G63" s="46">
+      <c r="G63" s="20"/>
+      <c r="H63" s="46">
         <v>41.546383333333331</v>
       </c>
-      <c r="H63" s="32"/>
-      <c r="I63" s="44">
+      <c r="I63" s="32"/>
+      <c r="J63" s="44">
         <v>57</v>
       </c>
-      <c r="J63" s="20" t="s">
+      <c r="K63" s="20" t="s">
         <v>406</v>
       </c>
-      <c r="K63" s="46">
+      <c r="L63" s="46">
         <v>66.422200000000004</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="44">
         <v>58</v>
       </c>
@@ -4280,21 +4346,22 @@
       <c r="F64" s="20" t="s">
         <v>407</v>
       </c>
-      <c r="G64" s="46">
+      <c r="G64" s="20"/>
+      <c r="H64" s="46">
         <v>41.501300000000001</v>
       </c>
-      <c r="H64" s="32"/>
-      <c r="I64" s="44">
+      <c r="I64" s="32"/>
+      <c r="J64" s="44">
         <v>58</v>
       </c>
-      <c r="J64" s="20" t="s">
+      <c r="K64" s="20" t="s">
         <v>408</v>
       </c>
-      <c r="K64" s="46">
+      <c r="L64" s="46">
         <v>65.13655</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="44">
         <v>59</v>
       </c>
@@ -4311,21 +4378,22 @@
       <c r="F65" s="20" t="s">
         <v>409</v>
       </c>
-      <c r="G65" s="46">
+      <c r="G65" s="20"/>
+      <c r="H65" s="46">
         <v>41.40956666666667</v>
       </c>
-      <c r="H65" s="32"/>
-      <c r="I65" s="44">
+      <c r="I65" s="32"/>
+      <c r="J65" s="44">
         <v>59</v>
       </c>
-      <c r="J65" s="20" t="s">
+      <c r="K65" s="20" t="s">
         <v>410</v>
       </c>
-      <c r="K65" s="46">
+      <c r="L65" s="46">
         <v>64.994466666666668</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="44">
         <v>60</v>
       </c>
@@ -4342,21 +4410,22 @@
       <c r="F66" s="20" t="s">
         <v>411</v>
       </c>
-      <c r="G66" s="46">
+      <c r="G66" s="20"/>
+      <c r="H66" s="46">
         <v>41.383383333333335</v>
       </c>
-      <c r="H66" s="32"/>
-      <c r="I66" s="44">
+      <c r="I66" s="32"/>
+      <c r="J66" s="44">
         <v>60</v>
       </c>
-      <c r="J66" s="20" t="s">
+      <c r="K66" s="20" t="s">
         <v>412</v>
       </c>
-      <c r="K66" s="46">
+      <c r="L66" s="46">
         <v>64.283183333333326</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="44">
         <v>61</v>
       </c>
@@ -4373,21 +4442,22 @@
       <c r="F67" s="20" t="s">
         <v>413</v>
       </c>
-      <c r="G67" s="46">
+      <c r="G67" s="20"/>
+      <c r="H67" s="46">
         <v>41.209083333333332</v>
       </c>
-      <c r="H67" s="32"/>
-      <c r="I67" s="44">
+      <c r="I67" s="32"/>
+      <c r="J67" s="44">
         <v>61</v>
       </c>
-      <c r="J67" s="20" t="s">
+      <c r="K67" s="20" t="s">
         <v>414</v>
       </c>
-      <c r="K67" s="46">
+      <c r="L67" s="46">
         <v>63.330783333333336</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="44">
         <v>62</v>
       </c>
@@ -4404,21 +4474,22 @@
       <c r="F68" s="20" t="s">
         <v>415</v>
       </c>
-      <c r="G68" s="46">
+      <c r="G68" s="20"/>
+      <c r="H68" s="46">
         <v>40.812216666666664</v>
       </c>
-      <c r="H68" s="32"/>
-      <c r="I68" s="44">
+      <c r="I68" s="32"/>
+      <c r="J68" s="44">
         <v>62</v>
       </c>
-      <c r="J68" s="20" t="s">
+      <c r="K68" s="20" t="s">
         <v>416</v>
       </c>
-      <c r="K68" s="46">
+      <c r="L68" s="46">
         <v>61.830116666666669</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="44">
         <v>63</v>
       </c>
@@ -4435,21 +4506,22 @@
       <c r="F69" s="20" t="s">
         <v>417</v>
       </c>
-      <c r="G69" s="46">
+      <c r="G69" s="20"/>
+      <c r="H69" s="46">
         <v>40.622900000000001</v>
       </c>
-      <c r="H69" s="32"/>
-      <c r="I69" s="44">
+      <c r="I69" s="32"/>
+      <c r="J69" s="44">
         <v>63</v>
       </c>
-      <c r="J69" s="20" t="s">
+      <c r="K69" s="20" t="s">
         <v>418</v>
       </c>
-      <c r="K69" s="46">
+      <c r="L69" s="46">
         <v>61.559150000000002</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="44">
         <v>64</v>
       </c>
@@ -4466,21 +4538,22 @@
       <c r="F70" s="20" t="s">
         <v>419</v>
       </c>
-      <c r="G70" s="46">
+      <c r="G70" s="20"/>
+      <c r="H70" s="46">
         <v>40.49765</v>
       </c>
-      <c r="H70" s="32"/>
-      <c r="I70" s="44">
+      <c r="I70" s="32"/>
+      <c r="J70" s="44">
         <v>64</v>
       </c>
-      <c r="J70" s="20" t="s">
+      <c r="K70" s="20" t="s">
         <v>420</v>
       </c>
-      <c r="K70" s="46">
+      <c r="L70" s="46">
         <v>57.091233333333335</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="44">
         <v>65</v>
       </c>
@@ -4497,21 +4570,22 @@
       <c r="F71" s="20" t="s">
         <v>421</v>
       </c>
-      <c r="G71" s="46">
+      <c r="G71" s="20"/>
+      <c r="H71" s="46">
         <v>40.272616666666664</v>
       </c>
-      <c r="H71" s="32"/>
-      <c r="I71" s="44">
+      <c r="I71" s="32"/>
+      <c r="J71" s="44">
         <v>65</v>
       </c>
-      <c r="J71" s="20" t="s">
+      <c r="K71" s="20" t="s">
         <v>422</v>
       </c>
-      <c r="K71" s="46">
+      <c r="L71" s="46">
         <v>56.603200000000001</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="44">
         <v>66</v>
       </c>
@@ -4528,21 +4602,22 @@
       <c r="F72" s="20" t="s">
         <v>423</v>
       </c>
-      <c r="G72" s="46">
+      <c r="G72" s="20"/>
+      <c r="H72" s="46">
         <v>40.190216666666664</v>
       </c>
-      <c r="H72" s="32"/>
-      <c r="I72" s="44">
+      <c r="I72" s="32"/>
+      <c r="J72" s="44">
         <v>66</v>
       </c>
-      <c r="J72" s="20" t="s">
+      <c r="K72" s="20" t="s">
         <v>424</v>
       </c>
-      <c r="K72" s="46">
+      <c r="L72" s="46">
         <v>56.13368333333333</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="44">
         <v>67</v>
       </c>
@@ -4559,21 +4634,22 @@
       <c r="F73" s="20" t="s">
         <v>425</v>
       </c>
-      <c r="G73" s="46">
+      <c r="G73" s="20"/>
+      <c r="H73" s="46">
         <v>39.674883333333334</v>
       </c>
-      <c r="H73" s="32"/>
-      <c r="I73" s="44">
+      <c r="I73" s="32"/>
+      <c r="J73" s="44">
         <v>67</v>
       </c>
-      <c r="J73" s="20" t="s">
+      <c r="K73" s="20" t="s">
         <v>426</v>
       </c>
-      <c r="K73" s="46">
+      <c r="L73" s="46">
         <v>55.9268</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="44">
         <v>68</v>
       </c>
@@ -4590,21 +4666,22 @@
       <c r="F74" s="20" t="s">
         <v>355</v>
       </c>
-      <c r="G74" s="46">
+      <c r="G74" s="20"/>
+      <c r="H74" s="46">
         <v>39.643000000000001</v>
       </c>
-      <c r="H74" s="32"/>
-      <c r="I74" s="44">
+      <c r="I74" s="32"/>
+      <c r="J74" s="44">
         <v>68</v>
       </c>
-      <c r="J74" s="20" t="s">
+      <c r="K74" s="20" t="s">
         <v>427</v>
       </c>
-      <c r="K74" s="46">
+      <c r="L74" s="46">
         <v>55.613100000000003</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="44">
         <v>69</v>
       </c>
@@ -4621,21 +4698,22 @@
       <c r="F75" s="20" t="s">
         <v>428</v>
       </c>
-      <c r="G75" s="46">
+      <c r="G75" s="20"/>
+      <c r="H75" s="46">
         <v>39.427933333333335</v>
       </c>
-      <c r="H75" s="32"/>
-      <c r="I75" s="44">
+      <c r="I75" s="32"/>
+      <c r="J75" s="44">
         <v>69</v>
       </c>
-      <c r="J75" s="20" t="s">
+      <c r="K75" s="20" t="s">
         <v>429</v>
       </c>
-      <c r="K75" s="46">
+      <c r="L75" s="46">
         <v>54.5002</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="44">
         <v>70</v>
       </c>
@@ -4652,21 +4730,22 @@
       <c r="F76" s="20" t="s">
         <v>430</v>
       </c>
-      <c r="G76" s="46">
+      <c r="G76" s="20"/>
+      <c r="H76" s="46">
         <v>39.401633333333336</v>
       </c>
-      <c r="H76" s="32"/>
-      <c r="I76" s="44">
+      <c r="I76" s="32"/>
+      <c r="J76" s="44">
         <v>70</v>
       </c>
-      <c r="J76" s="20" t="s">
+      <c r="K76" s="20" t="s">
         <v>431</v>
       </c>
-      <c r="K76" s="46">
+      <c r="L76" s="46">
         <v>52.543599999999998</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="44">
         <v>71</v>
       </c>
@@ -4683,21 +4762,22 @@
       <c r="F77" s="20" t="s">
         <v>432</v>
       </c>
-      <c r="G77" s="46">
+      <c r="G77" s="20"/>
+      <c r="H77" s="46">
         <v>39.323016666666668</v>
       </c>
-      <c r="H77" s="32"/>
-      <c r="I77" s="44">
+      <c r="I77" s="32"/>
+      <c r="J77" s="44">
         <v>71</v>
       </c>
-      <c r="J77" s="20" t="s">
+      <c r="K77" s="20" t="s">
         <v>433</v>
       </c>
-      <c r="K77" s="46">
+      <c r="L77" s="46">
         <v>52.16825</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="44">
         <v>72</v>
       </c>
@@ -4714,21 +4794,22 @@
       <c r="F78" s="20" t="s">
         <v>434</v>
       </c>
-      <c r="G78" s="46">
+      <c r="G78" s="20"/>
+      <c r="H78" s="46">
         <v>39.18013333333333</v>
       </c>
-      <c r="H78" s="32"/>
-      <c r="I78" s="44">
+      <c r="I78" s="32"/>
+      <c r="J78" s="44">
         <v>72</v>
       </c>
-      <c r="J78" s="20" t="s">
+      <c r="K78" s="20" t="s">
         <v>435</v>
       </c>
-      <c r="K78" s="46">
+      <c r="L78" s="46">
         <v>51.807549999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="44">
         <v>73</v>
       </c>
@@ -4745,21 +4826,22 @@
       <c r="F79" s="20" t="s">
         <v>436</v>
       </c>
-      <c r="G79" s="46">
+      <c r="G79" s="20"/>
+      <c r="H79" s="46">
         <v>39.129800000000003</v>
       </c>
-      <c r="H79" s="32"/>
-      <c r="I79" s="44">
+      <c r="I79" s="32"/>
+      <c r="J79" s="44">
         <v>73</v>
       </c>
-      <c r="J79" s="20" t="s">
+      <c r="K79" s="20" t="s">
         <v>437</v>
       </c>
-      <c r="K79" s="46">
+      <c r="L79" s="46">
         <v>51.616999999999997</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="44">
         <v>74</v>
       </c>
@@ -4776,21 +4858,22 @@
       <c r="F80" s="20" t="s">
         <v>438</v>
       </c>
-      <c r="G80" s="46">
+      <c r="G80" s="20"/>
+      <c r="H80" s="46">
         <v>39.037999999999997</v>
       </c>
-      <c r="H80" s="32"/>
-      <c r="I80" s="44">
+      <c r="I80" s="32"/>
+      <c r="J80" s="44">
         <v>74</v>
       </c>
-      <c r="J80" s="20" t="s">
+      <c r="K80" s="20" t="s">
         <v>439</v>
       </c>
-      <c r="K80" s="46">
+      <c r="L80" s="46">
         <v>50.596249999999998</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="44">
         <v>75</v>
       </c>
@@ -4807,21 +4890,22 @@
       <c r="F81" s="20" t="s">
         <v>440</v>
       </c>
-      <c r="G81" s="46">
+      <c r="G81" s="20"/>
+      <c r="H81" s="46">
         <v>38.56335</v>
       </c>
-      <c r="H81" s="32"/>
-      <c r="I81" s="44">
+      <c r="I81" s="32"/>
+      <c r="J81" s="44">
         <v>75</v>
       </c>
-      <c r="J81" s="20" t="s">
+      <c r="K81" s="20" t="s">
         <v>441</v>
       </c>
-      <c r="K81" s="46">
+      <c r="L81" s="46">
         <v>50.034050000000001</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="44">
         <v>76</v>
       </c>
@@ -4838,21 +4922,22 @@
       <c r="F82" s="20" t="s">
         <v>310</v>
       </c>
-      <c r="G82" s="46">
+      <c r="G82" s="20"/>
+      <c r="H82" s="46">
         <v>38.457383333333333</v>
       </c>
-      <c r="H82" s="32"/>
-      <c r="I82" s="44">
+      <c r="I82" s="32"/>
+      <c r="J82" s="44">
         <v>76</v>
       </c>
-      <c r="J82" s="20" t="s">
+      <c r="K82" s="20" t="s">
         <v>442</v>
       </c>
-      <c r="K82" s="46">
+      <c r="L82" s="46">
         <v>49.198816666666666</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="44">
         <v>77</v>
       </c>
@@ -4869,21 +4954,22 @@
       <c r="F83" s="20" t="s">
         <v>443</v>
       </c>
-      <c r="G83" s="46">
+      <c r="G83" s="20"/>
+      <c r="H83" s="46">
         <v>38.339849999999998</v>
       </c>
-      <c r="H83" s="32"/>
-      <c r="I83" s="44">
+      <c r="I83" s="32"/>
+      <c r="J83" s="44">
         <v>77</v>
       </c>
-      <c r="J83" s="20" t="s">
+      <c r="K83" s="20" t="s">
         <v>444</v>
       </c>
-      <c r="K83" s="46">
+      <c r="L83" s="46">
         <v>48.018916666666669</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="44">
         <v>78</v>
       </c>
@@ -4900,21 +4986,22 @@
       <c r="F84" s="20" t="s">
         <v>445</v>
       </c>
-      <c r="G84" s="46">
+      <c r="G84" s="20"/>
+      <c r="H84" s="46">
         <v>37.623316666666668</v>
       </c>
-      <c r="H84" s="32"/>
-      <c r="I84" s="44">
+      <c r="I84" s="32"/>
+      <c r="J84" s="44">
         <v>78</v>
       </c>
-      <c r="J84" s="20" t="s">
+      <c r="K84" s="20" t="s">
         <v>446</v>
       </c>
-      <c r="K84" s="46">
+      <c r="L84" s="46">
         <v>46.793799999999997</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="44">
         <v>79</v>
       </c>
@@ -4931,21 +5018,22 @@
       <c r="F85" s="20" t="s">
         <v>447</v>
       </c>
-      <c r="G85" s="46">
+      <c r="G85" s="20"/>
+      <c r="H85" s="46">
         <v>37.274333333333331</v>
       </c>
-      <c r="H85" s="32"/>
-      <c r="I85" s="44">
+      <c r="I85" s="32"/>
+      <c r="J85" s="44">
         <v>79</v>
       </c>
-      <c r="J85" s="20" t="s">
+      <c r="K85" s="20" t="s">
         <v>448</v>
       </c>
-      <c r="K85" s="46">
+      <c r="L85" s="46">
         <v>45.763733333333334</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="44">
         <v>80</v>
       </c>
@@ -4962,21 +5050,22 @@
       <c r="F86" s="20" t="s">
         <v>449</v>
       </c>
-      <c r="G86" s="46">
+      <c r="G86" s="20"/>
+      <c r="H86" s="46">
         <v>36.484450000000002</v>
       </c>
-      <c r="H86" s="32"/>
-      <c r="I86" s="44">
+      <c r="I86" s="32"/>
+      <c r="J86" s="44">
         <v>80</v>
       </c>
-      <c r="J86" s="20" t="s">
+      <c r="K86" s="20" t="s">
         <v>450</v>
       </c>
-      <c r="K86" s="46">
+      <c r="L86" s="46">
         <v>44.04613333333333</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="44">
         <v>81</v>
       </c>
@@ -4993,21 +5082,22 @@
       <c r="F87" s="20" t="s">
         <v>451</v>
       </c>
-      <c r="G87" s="46">
+      <c r="G87" s="20"/>
+      <c r="H87" s="46">
         <v>36.119599999999998</v>
       </c>
-      <c r="H87" s="32"/>
-      <c r="I87" s="44">
+      <c r="I87" s="32"/>
+      <c r="J87" s="44">
         <v>81</v>
       </c>
-      <c r="J87" s="20" t="s">
+      <c r="K87" s="20" t="s">
         <v>452</v>
       </c>
-      <c r="K87" s="46">
+      <c r="L87" s="46">
         <v>43.24346666666667</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="44">
         <v>82</v>
       </c>
@@ -5024,21 +5114,22 @@
       <c r="F88" s="20" t="s">
         <v>453</v>
       </c>
-      <c r="G88" s="46">
+      <c r="G88" s="20"/>
+      <c r="H88" s="46">
         <v>36.028083333333335</v>
       </c>
-      <c r="H88" s="32"/>
-      <c r="I88" s="44">
+      <c r="I88" s="32"/>
+      <c r="J88" s="44">
         <v>82</v>
       </c>
-      <c r="J88" s="20" t="s">
+      <c r="K88" s="20" t="s">
         <v>454</v>
       </c>
-      <c r="K88" s="46">
+      <c r="L88" s="46">
         <v>42.693516666666667</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="44">
         <v>83</v>
       </c>
@@ -5055,21 +5146,22 @@
       <c r="F89" s="20" t="s">
         <v>455</v>
       </c>
-      <c r="G89" s="46">
+      <c r="G89" s="20"/>
+      <c r="H89" s="46">
         <v>35.577716666666667</v>
       </c>
-      <c r="H89" s="32"/>
-      <c r="I89" s="44">
+      <c r="I89" s="32"/>
+      <c r="J89" s="44">
         <v>83</v>
       </c>
-      <c r="J89" s="20" t="s">
+      <c r="K89" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="K89" s="46">
+      <c r="L89" s="46">
         <v>42.150483333333334</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="44">
         <v>84</v>
       </c>
@@ -5086,21 +5178,22 @@
       <c r="F90" s="20" t="s">
         <v>456</v>
       </c>
-      <c r="G90" s="46">
+      <c r="G90" s="20"/>
+      <c r="H90" s="46">
         <v>35.176349999999999</v>
       </c>
-      <c r="H90" s="32"/>
-      <c r="I90" s="44">
+      <c r="I90" s="32"/>
+      <c r="J90" s="44">
         <v>84</v>
       </c>
-      <c r="J90" s="20" t="s">
+      <c r="K90" s="20" t="s">
         <v>457</v>
       </c>
-      <c r="K90" s="46">
+      <c r="L90" s="46">
         <v>40.891950000000001</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="44">
         <v>85</v>
       </c>
@@ -5117,21 +5210,22 @@
       <c r="F91" s="20" t="s">
         <v>458</v>
       </c>
-      <c r="G91" s="46">
+      <c r="G91" s="20"/>
+      <c r="H91" s="46">
         <v>34.761066666666665</v>
       </c>
-      <c r="H91" s="32"/>
-      <c r="I91" s="44">
+      <c r="I91" s="32"/>
+      <c r="J91" s="44">
         <v>85</v>
       </c>
-      <c r="J91" s="20" t="s">
+      <c r="K91" s="20" t="s">
         <v>459</v>
       </c>
-      <c r="K91" s="46">
+      <c r="L91" s="46">
         <v>40.426666666666669</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="44">
         <v>86</v>
       </c>
@@ -5148,21 +5242,22 @@
       <c r="F92" s="20" t="s">
         <v>460</v>
       </c>
-      <c r="G92" s="46">
+      <c r="G92" s="20"/>
+      <c r="H92" s="46">
         <v>34.72358333333333</v>
       </c>
-      <c r="H92" s="32"/>
-      <c r="I92" s="44">
+      <c r="I92" s="32"/>
+      <c r="J92" s="44">
         <v>86</v>
       </c>
-      <c r="J92" s="20" t="s">
+      <c r="K92" s="20" t="s">
         <v>461</v>
       </c>
-      <c r="K92" s="46">
+      <c r="L92" s="46">
         <v>39.444633333333336</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="44">
         <v>87</v>
       </c>
@@ -5179,21 +5274,22 @@
       <c r="F93" s="20" t="s">
         <v>462</v>
       </c>
-      <c r="G93" s="46">
+      <c r="G93" s="20"/>
+      <c r="H93" s="46">
         <v>34.623416666666664</v>
       </c>
-      <c r="H93" s="32"/>
-      <c r="I93" s="44">
+      <c r="I93" s="32"/>
+      <c r="J93" s="44">
         <v>87</v>
       </c>
-      <c r="J93" s="20" t="s">
+      <c r="K93" s="20" t="s">
         <v>463</v>
       </c>
-      <c r="K93" s="46">
+      <c r="L93" s="46">
         <v>38.128</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="44">
         <v>88</v>
       </c>
@@ -5210,21 +5306,22 @@
       <c r="F94" s="20" t="s">
         <v>464</v>
       </c>
-      <c r="G94" s="46">
+      <c r="G94" s="20"/>
+      <c r="H94" s="46">
         <v>34.598750000000003</v>
       </c>
-      <c r="H94" s="32"/>
-      <c r="I94" s="44">
+      <c r="I94" s="32"/>
+      <c r="J94" s="44">
         <v>88</v>
       </c>
-      <c r="J94" s="20" t="s">
+      <c r="K94" s="20" t="s">
         <v>465</v>
       </c>
-      <c r="K94" s="46">
+      <c r="L94" s="46">
         <v>38.073033333333335</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="44">
         <v>89</v>
       </c>
@@ -5241,21 +5338,22 @@
       <c r="F95" s="20" t="s">
         <v>466</v>
       </c>
-      <c r="G95" s="46">
+      <c r="G95" s="20"/>
+      <c r="H95" s="46">
         <v>33.880800000000001</v>
       </c>
-      <c r="H95" s="32"/>
-      <c r="I95" s="44">
+      <c r="I95" s="32"/>
+      <c r="J95" s="44">
         <v>89</v>
       </c>
-      <c r="J95" s="20" t="s">
+      <c r="K95" s="20" t="s">
         <v>467</v>
       </c>
-      <c r="K95" s="46">
+      <c r="L95" s="46">
         <v>37.61215</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="44">
         <v>90</v>
       </c>
@@ -5272,21 +5370,22 @@
       <c r="F96" s="20" t="s">
         <v>468</v>
       </c>
-      <c r="G96" s="46">
+      <c r="G96" s="20"/>
+      <c r="H96" s="46">
         <v>33.819200000000002</v>
       </c>
-      <c r="H96" s="32"/>
-      <c r="I96" s="44">
+      <c r="I96" s="32"/>
+      <c r="J96" s="44">
         <v>90</v>
       </c>
-      <c r="J96" s="20" t="s">
+      <c r="K96" s="20" t="s">
         <v>395</v>
       </c>
-      <c r="K96" s="46">
+      <c r="L96" s="46">
         <v>37.340316666666666</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="44">
         <v>91</v>
       </c>
@@ -5303,21 +5402,22 @@
       <c r="F97" s="20" t="s">
         <v>469</v>
       </c>
-      <c r="G97" s="46">
+      <c r="G97" s="20"/>
+      <c r="H97" s="46">
         <v>33.413649999999997</v>
       </c>
-      <c r="H97" s="32"/>
-      <c r="I97" s="44">
+      <c r="I97" s="32"/>
+      <c r="J97" s="44">
         <v>91</v>
       </c>
-      <c r="J97" s="20" t="s">
+      <c r="K97" s="20" t="s">
         <v>470</v>
       </c>
-      <c r="K97" s="46">
+      <c r="L97" s="46">
         <v>37.040599999999998</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="44">
         <v>92</v>
       </c>
@@ -5334,21 +5434,22 @@
       <c r="F98" s="20" t="s">
         <v>471</v>
       </c>
-      <c r="G98" s="46">
+      <c r="G98" s="20"/>
+      <c r="H98" s="46">
         <v>33.342483333333334</v>
       </c>
-      <c r="H98" s="32"/>
-      <c r="I98" s="44">
+      <c r="I98" s="32"/>
+      <c r="J98" s="44">
         <v>92</v>
       </c>
-      <c r="J98" s="20" t="s">
+      <c r="K98" s="20" t="s">
         <v>472</v>
       </c>
-      <c r="K98" s="46">
+      <c r="L98" s="46">
         <v>36.776383333333335</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="44">
         <v>93</v>
       </c>
@@ -5365,21 +5466,22 @@
       <c r="F99" s="20" t="s">
         <v>473</v>
       </c>
-      <c r="G99" s="46">
+      <c r="G99" s="20"/>
+      <c r="H99" s="46">
         <v>33.120533333333334</v>
       </c>
-      <c r="H99" s="32"/>
-      <c r="I99" s="44">
+      <c r="I99" s="32"/>
+      <c r="J99" s="44">
         <v>93</v>
       </c>
-      <c r="J99" s="20" t="s">
+      <c r="K99" s="20" t="s">
         <v>474</v>
       </c>
-      <c r="K99" s="46">
+      <c r="L99" s="46">
         <v>36.688600000000001</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="44">
         <v>94</v>
       </c>
@@ -5396,21 +5498,22 @@
       <c r="F100" s="20" t="s">
         <v>475</v>
       </c>
-      <c r="G100" s="46">
+      <c r="G100" s="20"/>
+      <c r="H100" s="46">
         <v>32.58271666666667</v>
       </c>
-      <c r="H100" s="32"/>
-      <c r="I100" s="44">
+      <c r="I100" s="32"/>
+      <c r="J100" s="44">
         <v>94</v>
       </c>
-      <c r="J100" s="20" t="s">
+      <c r="K100" s="20" t="s">
         <v>476</v>
       </c>
-      <c r="K100" s="46">
+      <c r="L100" s="46">
         <v>36.542666666666669</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="44">
         <v>95</v>
       </c>
@@ -5427,21 +5530,22 @@
       <c r="F101" s="20" t="s">
         <v>477</v>
       </c>
-      <c r="G101" s="46">
+      <c r="G101" s="20"/>
+      <c r="H101" s="46">
         <v>31.991783333333334</v>
       </c>
-      <c r="H101" s="32"/>
-      <c r="I101" s="44">
+      <c r="I101" s="32"/>
+      <c r="J101" s="44">
         <v>95</v>
       </c>
-      <c r="J101" s="20" t="s">
+      <c r="K101" s="20" t="s">
         <v>478</v>
       </c>
-      <c r="K101" s="46">
+      <c r="L101" s="46">
         <v>35.780799999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="44">
         <v>96</v>
       </c>
@@ -5458,21 +5562,22 @@
       <c r="F102" s="20" t="s">
         <v>479</v>
       </c>
-      <c r="G102" s="46">
+      <c r="G102" s="20"/>
+      <c r="H102" s="46">
         <v>31.932583333333334</v>
       </c>
-      <c r="H102" s="32"/>
-      <c r="I102" s="44">
+      <c r="I102" s="32"/>
+      <c r="J102" s="44">
         <v>96</v>
       </c>
-      <c r="J102" s="20" t="s">
+      <c r="K102" s="20" t="s">
         <v>480</v>
       </c>
-      <c r="K102" s="46">
+      <c r="L102" s="46">
         <v>35.665983333333337</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="44">
         <v>97</v>
       </c>
@@ -5489,21 +5594,22 @@
       <c r="F103" s="20" t="s">
         <v>308</v>
       </c>
-      <c r="G103" s="46">
+      <c r="G103" s="20"/>
+      <c r="H103" s="46">
         <v>31.926766666666666</v>
       </c>
-      <c r="H103" s="32"/>
-      <c r="I103" s="44">
+      <c r="I103" s="32"/>
+      <c r="J103" s="44">
         <v>97</v>
       </c>
-      <c r="J103" s="20" t="s">
+      <c r="K103" s="20" t="s">
         <v>481</v>
       </c>
-      <c r="K103" s="46">
+      <c r="L103" s="46">
         <v>34.720950000000002</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="44">
         <v>98</v>
       </c>
@@ -5520,21 +5626,22 @@
       <c r="F104" s="20" t="s">
         <v>482</v>
       </c>
-      <c r="G104" s="46">
+      <c r="G104" s="20"/>
+      <c r="H104" s="46">
         <v>31.685449999999999</v>
       </c>
-      <c r="H104" s="32"/>
-      <c r="I104" s="44">
+      <c r="I104" s="32"/>
+      <c r="J104" s="44">
         <v>98</v>
       </c>
-      <c r="J104" s="20" t="s">
+      <c r="K104" s="20" t="s">
         <v>483</v>
       </c>
-      <c r="K104" s="46">
+      <c r="L104" s="46">
         <v>33.522950000000002</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="44">
         <v>99</v>
       </c>
@@ -5551,21 +5658,22 @@
       <c r="F105" s="20" t="s">
         <v>484</v>
       </c>
-      <c r="G105" s="46">
+      <c r="G105" s="20"/>
+      <c r="H105" s="46">
         <v>31.426950000000001</v>
       </c>
-      <c r="H105" s="32"/>
-      <c r="I105" s="44">
+      <c r="I105" s="32"/>
+      <c r="J105" s="44">
         <v>99</v>
       </c>
-      <c r="J105" s="20" t="s">
+      <c r="K105" s="20" t="s">
         <v>485</v>
       </c>
-      <c r="K105" s="46">
+      <c r="L105" s="46">
         <v>33.484116666666665</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="47">
         <v>100</v>
       </c>
@@ -5582,28 +5690,29 @@
       <c r="F106" s="48" t="s">
         <v>486</v>
       </c>
-      <c r="G106" s="50">
+      <c r="G106" s="48"/>
+      <c r="H106" s="50">
         <v>30.630600000000001</v>
       </c>
-      <c r="H106" s="32"/>
-      <c r="I106" s="47">
+      <c r="I106" s="32"/>
+      <c r="J106" s="47">
         <v>100</v>
       </c>
-      <c r="J106" s="48" t="s">
+      <c r="K106" s="48" t="s">
         <v>487</v>
       </c>
-      <c r="K106" s="50">
+      <c r="L106" s="50">
         <v>32.550016666666664</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A3:L3"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="J5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6252,10 +6361,10 @@
   </sheetPr>
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G32" sqref="G32"/>
-      <selection pane="bottomLeft" sqref="A1:L1"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update 2025 top tracks sorted by canonical_track
</commit_message>
<xml_diff>
--- a/excel/spotify_listening_report_2025.xlsx
+++ b/excel/spotify_listening_report_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermitchell/Documents/projects/projects_2025/analytics_projects/Spotify_Sandbox/spotify_sandbox_github/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360F54A3-D90D-B748-A0FB-B20AA74B958A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6904BB5-D814-2E48-AC10-7B5F2EE8A004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="-1960" windowWidth="38400" windowHeight="21600" xr2:uid="{02962024-D185-E646-89C4-A67A4B8F8E62}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="526">
   <si>
     <t>Based on Spotify Extended Streaming History Time Listened (Music Only)</t>
   </si>
@@ -1629,8 +1629,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1945,7 +1946,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2031,6 +2032,12 @@
     <xf numFmtId="3" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2373,7 +2380,7 @@
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G32" sqref="G32"/>
-      <selection pane="bottomLeft" activeCell="K28" sqref="K28"/>
+      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2521,8 +2528,10 @@
       <c r="F7" s="30" t="s">
         <v>298</v>
       </c>
-      <c r="G7" s="30"/>
-      <c r="H7" s="33">
+      <c r="G7" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="65">
         <v>162.39576666666667</v>
       </c>
       <c r="I7" s="32"/>
@@ -2553,8 +2562,10 @@
       <c r="F8" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="36">
+      <c r="G8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="66">
         <v>136.98431666666667</v>
       </c>
       <c r="I8" s="32"/>
@@ -2585,8 +2596,10 @@
       <c r="F9" s="10" t="s">
         <v>301</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="36">
+      <c r="G9" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="66">
         <v>129.39758333333333</v>
       </c>
       <c r="I9" s="32"/>
@@ -2617,8 +2630,10 @@
       <c r="F10" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="36">
+      <c r="G10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="66">
         <v>120.67485000000001</v>
       </c>
       <c r="I10" s="32"/>
@@ -2649,8 +2664,10 @@
       <c r="F11" s="10" t="s">
         <v>305</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="36">
+      <c r="G11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="66">
         <v>116.45350000000001</v>
       </c>
       <c r="I11" s="32"/>
@@ -2682,8 +2699,10 @@
       <c r="F12" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="G12" s="16"/>
-      <c r="H12" s="40">
+      <c r="G12" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="67">
         <v>110.51224999999999</v>
       </c>
       <c r="I12" s="32"/>
@@ -2714,8 +2733,10 @@
       <c r="F13" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="40">
+      <c r="G13" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="67">
         <v>110.18210000000001</v>
       </c>
       <c r="I13" s="32"/>
@@ -2744,11 +2765,13 @@
         <v>8</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="40">
-        <v>101.7728</v>
+        <v>313</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="67">
+        <v>88.796733333333336</v>
       </c>
       <c r="I14" s="32"/>
       <c r="J14" s="38">
@@ -2776,11 +2799,13 @@
         <v>9</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>313</v>
-      </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="40">
-        <v>88.796733333333336</v>
+        <v>315</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="67">
+        <v>87.560916666666671</v>
       </c>
       <c r="I15" s="32"/>
       <c r="J15" s="38">
@@ -2808,11 +2833,13 @@
         <v>10</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>315</v>
-      </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="40">
-        <v>87.560916666666671</v>
+        <v>317</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="67">
+        <v>78.673066666666671</v>
       </c>
       <c r="I16" s="32"/>
       <c r="J16" s="38">
@@ -2840,11 +2867,13 @@
         <v>11</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>317</v>
-      </c>
-      <c r="G17" s="18"/>
-      <c r="H17" s="43">
-        <v>78.673066666666671</v>
+        <v>319</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="H17" s="68">
+        <v>75.114450000000005</v>
       </c>
       <c r="I17" s="32"/>
       <c r="J17" s="41">
@@ -2872,11 +2901,13 @@
         <v>12</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>319</v>
-      </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="43">
-        <v>75.114450000000005</v>
+        <v>321</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="68">
+        <v>75.044650000000004</v>
       </c>
       <c r="I18" s="32"/>
       <c r="J18" s="41">
@@ -2904,11 +2935,13 @@
         <v>13</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>321</v>
-      </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="43">
-        <v>75.044650000000004</v>
+        <v>323</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="68">
+        <v>73.818983333333335</v>
       </c>
       <c r="I19" s="32"/>
       <c r="J19" s="41">
@@ -2936,11 +2969,13 @@
         <v>14</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>323</v>
-      </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="43">
-        <v>73.818983333333335</v>
+        <v>325</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="68">
+        <v>70.979200000000006</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20" s="41">
@@ -2968,11 +3003,13 @@
         <v>15</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>325</v>
-      </c>
-      <c r="G21" s="18"/>
-      <c r="H21" s="43">
-        <v>70.979200000000006</v>
+        <v>326</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="68">
+        <v>69.502650000000003</v>
       </c>
       <c r="I21" s="32"/>
       <c r="J21" s="41">
@@ -3000,11 +3037,13 @@
         <v>16</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>326</v>
-      </c>
-      <c r="G22" s="18"/>
-      <c r="H22" s="43">
-        <v>69.502650000000003</v>
+        <v>328</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" s="68">
+        <v>69.15176666666666</v>
       </c>
       <c r="I22" s="32"/>
       <c r="J22" s="41">
@@ -3032,11 +3071,13 @@
         <v>17</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>328</v>
-      </c>
-      <c r="G23" s="18"/>
-      <c r="H23" s="43">
-        <v>69.15176666666666</v>
+        <v>330</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" s="68">
+        <v>68.841333333333338</v>
       </c>
       <c r="I23" s="32"/>
       <c r="J23" s="41">
@@ -3064,11 +3105,13 @@
         <v>18</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>330</v>
-      </c>
-      <c r="G24" s="18"/>
-      <c r="H24" s="43">
-        <v>68.841333333333338</v>
+        <v>332</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="68">
+        <v>68.576466666666661</v>
       </c>
       <c r="I24" s="32"/>
       <c r="J24" s="41">
@@ -3096,11 +3139,13 @@
         <v>19</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>332</v>
-      </c>
-      <c r="G25" s="18"/>
-      <c r="H25" s="43">
-        <v>68.576466666666661</v>
+        <v>334</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="68">
+        <v>66.407483333333332</v>
       </c>
       <c r="I25" s="32"/>
       <c r="J25" s="41">
@@ -3128,11 +3173,13 @@
         <v>20</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>334</v>
-      </c>
-      <c r="G26" s="18"/>
-      <c r="H26" s="43">
-        <v>66.407483333333332</v>
+        <v>336</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="68">
+        <v>65.699233333333339</v>
       </c>
       <c r="I26" s="32"/>
       <c r="J26" s="41">
@@ -3160,11 +3207,13 @@
         <v>21</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>336</v>
-      </c>
-      <c r="G27" s="20"/>
-      <c r="H27" s="46">
-        <v>65.699233333333339</v>
+        <v>311</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="69">
+        <v>65.456116666666674</v>
       </c>
       <c r="I27" s="32"/>
       <c r="J27" s="44">
@@ -3194,8 +3243,10 @@
       <c r="F28" s="20" t="s">
         <v>338</v>
       </c>
-      <c r="G28" s="20"/>
-      <c r="H28" s="46">
+      <c r="G28" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28" s="69">
         <v>64.26421666666667</v>
       </c>
       <c r="I28" s="32"/>
@@ -3226,8 +3277,10 @@
       <c r="F29" s="20" t="s">
         <v>340</v>
       </c>
-      <c r="G29" s="20"/>
-      <c r="H29" s="46">
+      <c r="G29" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="69">
         <v>59.984716666666664</v>
       </c>
       <c r="I29" s="32"/>
@@ -3258,8 +3311,10 @@
       <c r="F30" s="20" t="s">
         <v>342</v>
       </c>
-      <c r="G30" s="20"/>
-      <c r="H30" s="46">
+      <c r="G30" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30" s="69">
         <v>59.591999999999999</v>
       </c>
       <c r="I30" s="32"/>
@@ -3290,8 +3345,10 @@
       <c r="F31" s="20" t="s">
         <v>344</v>
       </c>
-      <c r="G31" s="20"/>
-      <c r="H31" s="46">
+      <c r="G31" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H31" s="69">
         <v>59.25685</v>
       </c>
       <c r="I31" s="32"/>
@@ -3322,8 +3379,10 @@
       <c r="F32" s="20" t="s">
         <v>312</v>
       </c>
-      <c r="G32" s="20"/>
-      <c r="H32" s="46">
+      <c r="G32" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" s="69">
         <v>58.996716666666664</v>
       </c>
       <c r="I32" s="32"/>
@@ -3354,8 +3413,10 @@
       <c r="F33" s="20" t="s">
         <v>346</v>
       </c>
-      <c r="G33" s="20"/>
-      <c r="H33" s="46">
+      <c r="G33" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H33" s="69">
         <v>58.030183333333333</v>
       </c>
       <c r="I33" s="32"/>
@@ -3386,8 +3447,10 @@
       <c r="F34" s="20" t="s">
         <v>348</v>
       </c>
-      <c r="G34" s="20"/>
-      <c r="H34" s="46">
+      <c r="G34" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" s="69">
         <v>56.381383333333332</v>
       </c>
       <c r="I34" s="32"/>
@@ -3418,8 +3481,10 @@
       <c r="F35" s="20" t="s">
         <v>350</v>
       </c>
-      <c r="G35" s="20"/>
-      <c r="H35" s="46">
+      <c r="G35" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="69">
         <v>56.032516666666666</v>
       </c>
       <c r="I35" s="32"/>
@@ -3450,8 +3515,10 @@
       <c r="F36" s="20" t="s">
         <v>352</v>
       </c>
-      <c r="G36" s="20"/>
-      <c r="H36" s="46">
+      <c r="G36" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H36" s="69">
         <v>55.678566666666669</v>
       </c>
       <c r="I36" s="32"/>
@@ -3482,8 +3549,10 @@
       <c r="F37" s="20" t="s">
         <v>354</v>
       </c>
-      <c r="G37" s="20"/>
-      <c r="H37" s="46">
+      <c r="G37" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" s="69">
         <v>55.64071666666667</v>
       </c>
       <c r="I37" s="32"/>
@@ -3514,8 +3583,10 @@
       <c r="F38" s="20" t="s">
         <v>356</v>
       </c>
-      <c r="G38" s="20"/>
-      <c r="H38" s="46">
+      <c r="G38" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" s="69">
         <v>54.588016666666668</v>
       </c>
       <c r="I38" s="32"/>
@@ -3546,8 +3617,10 @@
       <c r="F39" s="20" t="s">
         <v>358</v>
       </c>
-      <c r="G39" s="20"/>
-      <c r="H39" s="46">
+      <c r="G39" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H39" s="69">
         <v>53.564533333333337</v>
       </c>
       <c r="I39" s="32"/>
@@ -3578,8 +3651,10 @@
       <c r="F40" s="20" t="s">
         <v>360</v>
       </c>
-      <c r="G40" s="20"/>
-      <c r="H40" s="46">
+      <c r="G40" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H40" s="69">
         <v>50.267383333333335</v>
       </c>
       <c r="I40" s="32"/>
@@ -3610,8 +3685,10 @@
       <c r="F41" s="20" t="s">
         <v>362</v>
       </c>
-      <c r="G41" s="20"/>
-      <c r="H41" s="46">
+      <c r="G41" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H41" s="69">
         <v>50.252816666666668</v>
       </c>
       <c r="I41" s="32"/>
@@ -3642,8 +3719,10 @@
       <c r="F42" s="20" t="s">
         <v>364</v>
       </c>
-      <c r="G42" s="20"/>
-      <c r="H42" s="46">
+      <c r="G42" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" s="69">
         <v>49.837466666666664</v>
       </c>
       <c r="I42" s="32"/>
@@ -3674,8 +3753,10 @@
       <c r="F43" s="20" t="s">
         <v>366</v>
       </c>
-      <c r="G43" s="20"/>
-      <c r="H43" s="46">
+      <c r="G43" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H43" s="69">
         <v>49.572749999999999</v>
       </c>
       <c r="I43" s="32"/>
@@ -3706,8 +3787,10 @@
       <c r="F44" s="20" t="s">
         <v>368</v>
       </c>
-      <c r="G44" s="20"/>
-      <c r="H44" s="46">
+      <c r="G44" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H44" s="69">
         <v>49.404616666666669</v>
       </c>
       <c r="I44" s="32"/>
@@ -3738,8 +3821,10 @@
       <c r="F45" s="20" t="s">
         <v>370</v>
       </c>
-      <c r="G45" s="20"/>
-      <c r="H45" s="46">
+      <c r="G45" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H45" s="69">
         <v>49.314399999999999</v>
       </c>
       <c r="I45" s="32"/>
@@ -3770,8 +3855,10 @@
       <c r="F46" s="20" t="s">
         <v>347</v>
       </c>
-      <c r="G46" s="20"/>
-      <c r="H46" s="46">
+      <c r="G46" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="69">
         <v>49.160766666666667</v>
       </c>
       <c r="I46" s="32"/>
@@ -3802,8 +3889,10 @@
       <c r="F47" s="20" t="s">
         <v>373</v>
       </c>
-      <c r="G47" s="20"/>
-      <c r="H47" s="46">
+      <c r="G47" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" s="69">
         <v>48.411149999999999</v>
       </c>
       <c r="I47" s="32"/>
@@ -3834,8 +3923,10 @@
       <c r="F48" s="20" t="s">
         <v>375</v>
       </c>
-      <c r="G48" s="20"/>
-      <c r="H48" s="46">
+      <c r="G48" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H48" s="69">
         <v>47.83155</v>
       </c>
       <c r="I48" s="32"/>
@@ -3866,8 +3957,10 @@
       <c r="F49" s="20" t="s">
         <v>377</v>
       </c>
-      <c r="G49" s="20"/>
-      <c r="H49" s="46">
+      <c r="G49" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H49" s="69">
         <v>47.251466666666666</v>
       </c>
       <c r="I49" s="32"/>
@@ -3898,8 +3991,10 @@
       <c r="F50" s="20" t="s">
         <v>379</v>
       </c>
-      <c r="G50" s="20"/>
-      <c r="H50" s="46">
+      <c r="G50" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H50" s="69">
         <v>46.779366666666668</v>
       </c>
       <c r="I50" s="32"/>
@@ -3930,8 +4025,10 @@
       <c r="F51" s="20" t="s">
         <v>381</v>
       </c>
-      <c r="G51" s="20"/>
-      <c r="H51" s="46">
+      <c r="G51" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H51" s="69">
         <v>46.714550000000003</v>
       </c>
       <c r="I51" s="32"/>
@@ -3962,8 +4059,10 @@
       <c r="F52" s="20" t="s">
         <v>383</v>
       </c>
-      <c r="G52" s="20"/>
-      <c r="H52" s="46">
+      <c r="G52" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H52" s="69">
         <v>45.705716666666667</v>
       </c>
       <c r="I52" s="32"/>
@@ -3994,8 +4093,10 @@
       <c r="F53" s="20" t="s">
         <v>385</v>
       </c>
-      <c r="G53" s="20"/>
-      <c r="H53" s="46">
+      <c r="G53" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H53" s="69">
         <v>45.406366666666663</v>
       </c>
       <c r="I53" s="32"/>
@@ -4026,8 +4127,10 @@
       <c r="F54" s="20" t="s">
         <v>387</v>
       </c>
-      <c r="G54" s="20"/>
-      <c r="H54" s="46">
+      <c r="G54" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H54" s="69">
         <v>45.267933333333332</v>
       </c>
       <c r="I54" s="32"/>
@@ -4058,8 +4161,10 @@
       <c r="F55" s="20" t="s">
         <v>389</v>
       </c>
-      <c r="G55" s="20"/>
-      <c r="H55" s="46">
+      <c r="G55" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="H55" s="69">
         <v>44.662799999999997</v>
       </c>
       <c r="I55" s="32"/>
@@ -4090,8 +4195,10 @@
       <c r="F56" s="20" t="s">
         <v>391</v>
       </c>
-      <c r="G56" s="20"/>
-      <c r="H56" s="46">
+      <c r="G56" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H56" s="69">
         <v>44.518883333333335</v>
       </c>
       <c r="I56" s="32"/>
@@ -4122,8 +4229,10 @@
       <c r="F57" s="20" t="s">
         <v>393</v>
       </c>
-      <c r="G57" s="20"/>
-      <c r="H57" s="46">
+      <c r="G57" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H57" s="69">
         <v>44.077500000000001</v>
       </c>
       <c r="I57" s="32"/>
@@ -4154,8 +4263,10 @@
       <c r="F58" s="20" t="s">
         <v>395</v>
       </c>
-      <c r="G58" s="20"/>
-      <c r="H58" s="46">
+      <c r="G58" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H58" s="69">
         <v>43.632866666666665</v>
       </c>
       <c r="I58" s="32"/>
@@ -4186,8 +4297,10 @@
       <c r="F59" s="20" t="s">
         <v>397</v>
       </c>
-      <c r="G59" s="20"/>
-      <c r="H59" s="46">
+      <c r="G59" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H59" s="69">
         <v>43.256316666666663</v>
       </c>
       <c r="I59" s="32"/>
@@ -4218,8 +4331,10 @@
       <c r="F60" s="20" t="s">
         <v>399</v>
       </c>
-      <c r="G60" s="20"/>
-      <c r="H60" s="46">
+      <c r="G60" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H60" s="69">
         <v>43.077449999999999</v>
       </c>
       <c r="I60" s="32"/>
@@ -4250,8 +4365,10 @@
       <c r="F61" s="20" t="s">
         <v>401</v>
       </c>
-      <c r="G61" s="20"/>
-      <c r="H61" s="46">
+      <c r="G61" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H61" s="69">
         <v>42.818533333333335</v>
       </c>
       <c r="I61" s="32"/>
@@ -4282,8 +4399,10 @@
       <c r="F62" s="20" t="s">
         <v>403</v>
       </c>
-      <c r="G62" s="20"/>
-      <c r="H62" s="46">
+      <c r="G62" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H62" s="69">
         <v>42.366599999999998</v>
       </c>
       <c r="I62" s="32"/>
@@ -4314,8 +4433,10 @@
       <c r="F63" s="20" t="s">
         <v>405</v>
       </c>
-      <c r="G63" s="20"/>
-      <c r="H63" s="46">
+      <c r="G63" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H63" s="69">
         <v>41.546383333333331</v>
       </c>
       <c r="I63" s="32"/>
@@ -4346,8 +4467,10 @@
       <c r="F64" s="20" t="s">
         <v>407</v>
       </c>
-      <c r="G64" s="20"/>
-      <c r="H64" s="46">
+      <c r="G64" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H64" s="69">
         <v>41.501300000000001</v>
       </c>
       <c r="I64" s="32"/>
@@ -4378,8 +4501,10 @@
       <c r="F65" s="20" t="s">
         <v>409</v>
       </c>
-      <c r="G65" s="20"/>
-      <c r="H65" s="46">
+      <c r="G65" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H65" s="69">
         <v>41.40956666666667</v>
       </c>
       <c r="I65" s="32"/>
@@ -4410,8 +4535,10 @@
       <c r="F66" s="20" t="s">
         <v>411</v>
       </c>
-      <c r="G66" s="20"/>
-      <c r="H66" s="46">
+      <c r="G66" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H66" s="69">
         <v>41.383383333333335</v>
       </c>
       <c r="I66" s="32"/>
@@ -4442,8 +4569,10 @@
       <c r="F67" s="20" t="s">
         <v>413</v>
       </c>
-      <c r="G67" s="20"/>
-      <c r="H67" s="46">
+      <c r="G67" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H67" s="69">
         <v>41.209083333333332</v>
       </c>
       <c r="I67" s="32"/>
@@ -4474,8 +4603,10 @@
       <c r="F68" s="20" t="s">
         <v>415</v>
       </c>
-      <c r="G68" s="20"/>
-      <c r="H68" s="46">
+      <c r="G68" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H68" s="69">
         <v>40.812216666666664</v>
       </c>
       <c r="I68" s="32"/>
@@ -4506,8 +4637,10 @@
       <c r="F69" s="20" t="s">
         <v>417</v>
       </c>
-      <c r="G69" s="20"/>
-      <c r="H69" s="46">
+      <c r="G69" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H69" s="69">
         <v>40.622900000000001</v>
       </c>
       <c r="I69" s="32"/>
@@ -4536,11 +4669,13 @@
         <v>64</v>
       </c>
       <c r="F70" s="20" t="s">
-        <v>419</v>
-      </c>
-      <c r="G70" s="20"/>
-      <c r="H70" s="46">
-        <v>40.49765</v>
+        <v>421</v>
+      </c>
+      <c r="G70" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H70" s="69">
+        <v>40.272616666666664</v>
       </c>
       <c r="I70" s="32"/>
       <c r="J70" s="44">
@@ -4568,11 +4703,13 @@
         <v>65</v>
       </c>
       <c r="F71" s="20" t="s">
-        <v>421</v>
-      </c>
-      <c r="G71" s="20"/>
-      <c r="H71" s="46">
-        <v>40.272616666666664</v>
+        <v>423</v>
+      </c>
+      <c r="G71" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H71" s="69">
+        <v>40.190216666666664</v>
       </c>
       <c r="I71" s="32"/>
       <c r="J71" s="44">
@@ -4600,11 +4737,13 @@
         <v>66</v>
       </c>
       <c r="F72" s="20" t="s">
-        <v>423</v>
-      </c>
-      <c r="G72" s="20"/>
-      <c r="H72" s="46">
-        <v>40.190216666666664</v>
+        <v>425</v>
+      </c>
+      <c r="G72" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H72" s="69">
+        <v>39.674883333333334</v>
       </c>
       <c r="I72" s="32"/>
       <c r="J72" s="44">
@@ -4632,11 +4771,13 @@
         <v>67</v>
       </c>
       <c r="F73" s="20" t="s">
-        <v>425</v>
-      </c>
-      <c r="G73" s="20"/>
-      <c r="H73" s="46">
-        <v>39.674883333333334</v>
+        <v>355</v>
+      </c>
+      <c r="G73" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="H73" s="69">
+        <v>39.643000000000001</v>
       </c>
       <c r="I73" s="32"/>
       <c r="J73" s="44">
@@ -4664,11 +4805,13 @@
         <v>68</v>
       </c>
       <c r="F74" s="20" t="s">
-        <v>355</v>
-      </c>
-      <c r="G74" s="20"/>
-      <c r="H74" s="46">
-        <v>39.643000000000001</v>
+        <v>428</v>
+      </c>
+      <c r="G74" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H74" s="69">
+        <v>39.427933333333335</v>
       </c>
       <c r="I74" s="32"/>
       <c r="J74" s="44">
@@ -4696,11 +4839,13 @@
         <v>69</v>
       </c>
       <c r="F75" s="20" t="s">
-        <v>428</v>
-      </c>
-      <c r="G75" s="20"/>
-      <c r="H75" s="46">
-        <v>39.427933333333335</v>
+        <v>430</v>
+      </c>
+      <c r="G75" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H75" s="69">
+        <v>39.401633333333336</v>
       </c>
       <c r="I75" s="32"/>
       <c r="J75" s="44">
@@ -4728,11 +4873,13 @@
         <v>70</v>
       </c>
       <c r="F76" s="20" t="s">
-        <v>430</v>
-      </c>
-      <c r="G76" s="20"/>
-      <c r="H76" s="46">
-        <v>39.401633333333336</v>
+        <v>432</v>
+      </c>
+      <c r="G76" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H76" s="69">
+        <v>39.323016666666668</v>
       </c>
       <c r="I76" s="32"/>
       <c r="J76" s="44">
@@ -4760,11 +4907,13 @@
         <v>71</v>
       </c>
       <c r="F77" s="20" t="s">
-        <v>432</v>
-      </c>
-      <c r="G77" s="20"/>
-      <c r="H77" s="46">
-        <v>39.323016666666668</v>
+        <v>434</v>
+      </c>
+      <c r="G77" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H77" s="69">
+        <v>39.18013333333333</v>
       </c>
       <c r="I77" s="32"/>
       <c r="J77" s="44">
@@ -4792,11 +4941,13 @@
         <v>72</v>
       </c>
       <c r="F78" s="20" t="s">
-        <v>434</v>
-      </c>
-      <c r="G78" s="20"/>
-      <c r="H78" s="46">
-        <v>39.18013333333333</v>
+        <v>436</v>
+      </c>
+      <c r="G78" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="H78" s="69">
+        <v>39.129800000000003</v>
       </c>
       <c r="I78" s="32"/>
       <c r="J78" s="44">
@@ -4824,11 +4975,13 @@
         <v>73</v>
       </c>
       <c r="F79" s="20" t="s">
-        <v>436</v>
-      </c>
-      <c r="G79" s="20"/>
-      <c r="H79" s="46">
-        <v>39.129800000000003</v>
+        <v>438</v>
+      </c>
+      <c r="G79" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H79" s="69">
+        <v>39.037999999999997</v>
       </c>
       <c r="I79" s="32"/>
       <c r="J79" s="44">
@@ -4856,11 +5009,13 @@
         <v>74</v>
       </c>
       <c r="F80" s="20" t="s">
-        <v>438</v>
-      </c>
-      <c r="G80" s="20"/>
-      <c r="H80" s="46">
-        <v>39.037999999999997</v>
+        <v>440</v>
+      </c>
+      <c r="G80" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H80" s="69">
+        <v>38.56335</v>
       </c>
       <c r="I80" s="32"/>
       <c r="J80" s="44">
@@ -4888,11 +5043,13 @@
         <v>75</v>
       </c>
       <c r="F81" s="20" t="s">
-        <v>440</v>
-      </c>
-      <c r="G81" s="20"/>
-      <c r="H81" s="46">
-        <v>38.56335</v>
+        <v>310</v>
+      </c>
+      <c r="G81" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H81" s="69">
+        <v>38.457383333333333</v>
       </c>
       <c r="I81" s="32"/>
       <c r="J81" s="44">
@@ -4920,11 +5077,13 @@
         <v>76</v>
       </c>
       <c r="F82" s="20" t="s">
-        <v>310</v>
-      </c>
-      <c r="G82" s="20"/>
-      <c r="H82" s="46">
-        <v>38.457383333333333</v>
+        <v>443</v>
+      </c>
+      <c r="G82" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H82" s="69">
+        <v>38.339849999999998</v>
       </c>
       <c r="I82" s="32"/>
       <c r="J82" s="44">
@@ -4952,11 +5111,13 @@
         <v>77</v>
       </c>
       <c r="F83" s="20" t="s">
-        <v>443</v>
-      </c>
-      <c r="G83" s="20"/>
-      <c r="H83" s="46">
-        <v>38.339849999999998</v>
+        <v>445</v>
+      </c>
+      <c r="G83" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H83" s="69">
+        <v>37.623316666666668</v>
       </c>
       <c r="I83" s="32"/>
       <c r="J83" s="44">
@@ -4984,11 +5145,13 @@
         <v>78</v>
       </c>
       <c r="F84" s="20" t="s">
-        <v>445</v>
-      </c>
-      <c r="G84" s="20"/>
-      <c r="H84" s="46">
-        <v>37.623316666666668</v>
+        <v>447</v>
+      </c>
+      <c r="G84" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H84" s="69">
+        <v>37.274333333333331</v>
       </c>
       <c r="I84" s="32"/>
       <c r="J84" s="44">
@@ -5016,11 +5179,13 @@
         <v>79</v>
       </c>
       <c r="F85" s="20" t="s">
-        <v>447</v>
-      </c>
-      <c r="G85" s="20"/>
-      <c r="H85" s="46">
-        <v>37.274333333333331</v>
+        <v>449</v>
+      </c>
+      <c r="G85" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H85" s="69">
+        <v>36.484450000000002</v>
       </c>
       <c r="I85" s="32"/>
       <c r="J85" s="44">
@@ -5048,11 +5213,13 @@
         <v>80</v>
       </c>
       <c r="F86" s="20" t="s">
-        <v>449</v>
-      </c>
-      <c r="G86" s="20"/>
-      <c r="H86" s="46">
-        <v>36.484450000000002</v>
+        <v>311</v>
+      </c>
+      <c r="G86" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H86" s="69">
+        <v>36.31668333333333</v>
       </c>
       <c r="I86" s="32"/>
       <c r="J86" s="44">
@@ -5080,11 +5247,13 @@
         <v>81</v>
       </c>
       <c r="F87" s="20" t="s">
-        <v>451</v>
-      </c>
-      <c r="G87" s="20"/>
-      <c r="H87" s="46">
-        <v>36.119599999999998</v>
+        <v>453</v>
+      </c>
+      <c r="G87" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H87" s="69">
+        <v>36.028083333333335</v>
       </c>
       <c r="I87" s="32"/>
       <c r="J87" s="44">
@@ -5112,11 +5281,13 @@
         <v>82</v>
       </c>
       <c r="F88" s="20" t="s">
-        <v>453</v>
-      </c>
-      <c r="G88" s="20"/>
-      <c r="H88" s="46">
-        <v>36.028083333333335</v>
+        <v>455</v>
+      </c>
+      <c r="G88" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="H88" s="69">
+        <v>35.577716666666667</v>
       </c>
       <c r="I88" s="32"/>
       <c r="J88" s="44">
@@ -5144,11 +5315,13 @@
         <v>83</v>
       </c>
       <c r="F89" s="20" t="s">
-        <v>455</v>
-      </c>
-      <c r="G89" s="20"/>
-      <c r="H89" s="46">
-        <v>35.577716666666667</v>
+        <v>456</v>
+      </c>
+      <c r="G89" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H89" s="69">
+        <v>35.176349999999999</v>
       </c>
       <c r="I89" s="32"/>
       <c r="J89" s="44">
@@ -5176,11 +5349,13 @@
         <v>84</v>
       </c>
       <c r="F90" s="20" t="s">
-        <v>456</v>
-      </c>
-      <c r="G90" s="20"/>
-      <c r="H90" s="46">
-        <v>35.176349999999999</v>
+        <v>458</v>
+      </c>
+      <c r="G90" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H90" s="69">
+        <v>34.761066666666665</v>
       </c>
       <c r="I90" s="32"/>
       <c r="J90" s="44">
@@ -5208,11 +5383,13 @@
         <v>85</v>
       </c>
       <c r="F91" s="20" t="s">
-        <v>458</v>
-      </c>
-      <c r="G91" s="20"/>
-      <c r="H91" s="46">
-        <v>34.761066666666665</v>
+        <v>460</v>
+      </c>
+      <c r="G91" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H91" s="69">
+        <v>34.72358333333333</v>
       </c>
       <c r="I91" s="32"/>
       <c r="J91" s="44">
@@ -5240,11 +5417,13 @@
         <v>86</v>
       </c>
       <c r="F92" s="20" t="s">
-        <v>460</v>
-      </c>
-      <c r="G92" s="20"/>
-      <c r="H92" s="46">
-        <v>34.72358333333333</v>
+        <v>462</v>
+      </c>
+      <c r="G92" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H92" s="69">
+        <v>34.623416666666664</v>
       </c>
       <c r="I92" s="32"/>
       <c r="J92" s="44">
@@ -5272,11 +5451,13 @@
         <v>87</v>
       </c>
       <c r="F93" s="20" t="s">
-        <v>462</v>
-      </c>
-      <c r="G93" s="20"/>
-      <c r="H93" s="46">
-        <v>34.623416666666664</v>
+        <v>464</v>
+      </c>
+      <c r="G93" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H93" s="69">
+        <v>34.598750000000003</v>
       </c>
       <c r="I93" s="32"/>
       <c r="J93" s="44">
@@ -5304,11 +5485,13 @@
         <v>88</v>
       </c>
       <c r="F94" s="20" t="s">
-        <v>464</v>
-      </c>
-      <c r="G94" s="20"/>
-      <c r="H94" s="46">
-        <v>34.598750000000003</v>
+        <v>466</v>
+      </c>
+      <c r="G94" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H94" s="69">
+        <v>33.880800000000001</v>
       </c>
       <c r="I94" s="32"/>
       <c r="J94" s="44">
@@ -5336,11 +5519,13 @@
         <v>89</v>
       </c>
       <c r="F95" s="20" t="s">
-        <v>466</v>
-      </c>
-      <c r="G95" s="20"/>
-      <c r="H95" s="46">
-        <v>33.880800000000001</v>
+        <v>468</v>
+      </c>
+      <c r="G95" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H95" s="69">
+        <v>33.819200000000002</v>
       </c>
       <c r="I95" s="32"/>
       <c r="J95" s="44">
@@ -5368,11 +5553,13 @@
         <v>90</v>
       </c>
       <c r="F96" s="20" t="s">
-        <v>468</v>
-      </c>
-      <c r="G96" s="20"/>
-      <c r="H96" s="46">
-        <v>33.819200000000002</v>
+        <v>451</v>
+      </c>
+      <c r="G96" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H96" s="69">
+        <v>33.569516666666665</v>
       </c>
       <c r="I96" s="32"/>
       <c r="J96" s="44">
@@ -5402,8 +5589,10 @@
       <c r="F97" s="20" t="s">
         <v>469</v>
       </c>
-      <c r="G97" s="20"/>
-      <c r="H97" s="46">
+      <c r="G97" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H97" s="69">
         <v>33.413649999999997</v>
       </c>
       <c r="I97" s="32"/>
@@ -5434,8 +5623,10 @@
       <c r="F98" s="20" t="s">
         <v>471</v>
       </c>
-      <c r="G98" s="20"/>
-      <c r="H98" s="46">
+      <c r="G98" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H98" s="69">
         <v>33.342483333333334</v>
       </c>
       <c r="I98" s="32"/>
@@ -5466,8 +5657,10 @@
       <c r="F99" s="20" t="s">
         <v>473</v>
       </c>
-      <c r="G99" s="20"/>
-      <c r="H99" s="46">
+      <c r="G99" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H99" s="69">
         <v>33.120533333333334</v>
       </c>
       <c r="I99" s="32"/>
@@ -5498,8 +5691,10 @@
       <c r="F100" s="20" t="s">
         <v>475</v>
       </c>
-      <c r="G100" s="20"/>
-      <c r="H100" s="46">
+      <c r="G100" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H100" s="69">
         <v>32.58271666666667</v>
       </c>
       <c r="I100" s="32"/>
@@ -5528,11 +5723,13 @@
         <v>95</v>
       </c>
       <c r="F101" s="20" t="s">
-        <v>477</v>
-      </c>
-      <c r="G101" s="20"/>
-      <c r="H101" s="46">
-        <v>31.991783333333334</v>
+        <v>419</v>
+      </c>
+      <c r="G101" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H101" s="69">
+        <v>32.281649999999999</v>
       </c>
       <c r="I101" s="32"/>
       <c r="J101" s="44">
@@ -5560,11 +5757,13 @@
         <v>96</v>
       </c>
       <c r="F102" s="20" t="s">
-        <v>479</v>
-      </c>
-      <c r="G102" s="20"/>
-      <c r="H102" s="46">
-        <v>31.932583333333334</v>
+        <v>477</v>
+      </c>
+      <c r="G102" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H102" s="69">
+        <v>31.991783333333334</v>
       </c>
       <c r="I102" s="32"/>
       <c r="J102" s="44">
@@ -5592,11 +5791,13 @@
         <v>97</v>
       </c>
       <c r="F103" s="20" t="s">
-        <v>308</v>
-      </c>
-      <c r="G103" s="20"/>
-      <c r="H103" s="46">
-        <v>31.926766666666666</v>
+        <v>479</v>
+      </c>
+      <c r="G103" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H103" s="69">
+        <v>31.932583333333334</v>
       </c>
       <c r="I103" s="32"/>
       <c r="J103" s="44">
@@ -5624,11 +5825,13 @@
         <v>98</v>
       </c>
       <c r="F104" s="20" t="s">
-        <v>482</v>
-      </c>
-      <c r="G104" s="20"/>
-      <c r="H104" s="46">
-        <v>31.685449999999999</v>
+        <v>308</v>
+      </c>
+      <c r="G104" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H104" s="69">
+        <v>31.926766666666666</v>
       </c>
       <c r="I104" s="32"/>
       <c r="J104" s="44">
@@ -5656,11 +5859,13 @@
         <v>99</v>
       </c>
       <c r="F105" s="20" t="s">
-        <v>484</v>
-      </c>
-      <c r="G105" s="20"/>
-      <c r="H105" s="46">
-        <v>31.426950000000001</v>
+        <v>482</v>
+      </c>
+      <c r="G105" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H105" s="69">
+        <v>31.685449999999999</v>
       </c>
       <c r="I105" s="32"/>
       <c r="J105" s="44">
@@ -5688,11 +5893,13 @@
         <v>100</v>
       </c>
       <c r="F106" s="48" t="s">
-        <v>486</v>
-      </c>
-      <c r="G106" s="48"/>
-      <c r="H106" s="50">
-        <v>30.630600000000001</v>
+        <v>484</v>
+      </c>
+      <c r="G106" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="H106" s="70">
+        <v>31.426950000000001</v>
       </c>
       <c r="I106" s="32"/>
       <c r="J106" s="47">

</xml_diff>

<commit_message>
Update 2025 top albums using album_family and merged query. Add By Artist column.
</commit_message>
<xml_diff>
--- a/excel/spotify_listening_report_2025.xlsx
+++ b/excel/spotify_listening_report_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermitchell/Documents/projects/projects_2025/analytics_projects/Spotify_Sandbox/spotify_sandbox_github/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6904BB5-D814-2E48-AC10-7B5F2EE8A004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6710701E-E459-BD43-81A1-DEE24F198F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="-1960" windowWidth="38400" windowHeight="21600" xr2:uid="{02962024-D185-E646-89C4-A67A4B8F8E62}"/>
   </bookViews>
@@ -24,7 +24,7 @@
     <sheet name="Aug" sheetId="11" r:id="rId9"/>
     <sheet name="Sep" sheetId="12" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="526">
   <si>
     <t>Based on Spotify Extended Streaming History Time Listened (Music Only)</t>
   </si>
@@ -1013,9 +1013,6 @@
     <t>Cecil Taylor</t>
   </si>
   <si>
-    <t>Bark At The Moon (Expanded Edition)</t>
-  </si>
-  <si>
     <t>Ice Cream Piano</t>
   </si>
   <si>
@@ -1241,9 +1238,6 @@
     <t>Jack the Stripper / Fairies Wear Boots - 2012 - Remaster</t>
   </si>
   <si>
-    <t>Loaded: Re-Loaded 45th Anniversary Edition</t>
-  </si>
-  <si>
     <t>Stranger</t>
   </si>
   <si>
@@ -1253,9 +1247,6 @@
     <t>Hope</t>
   </si>
   <si>
-    <t>1989</t>
-  </si>
-  <si>
     <t>Electric Funeral - 2012 - Remaster</t>
   </si>
   <si>
@@ -1319,9 +1310,6 @@
     <t>War Pigs / Luke's Wall - 2012 - Remaster</t>
   </si>
   <si>
-    <t>Diary of a Madman (40th Anniversary Expanded Edition)</t>
-  </si>
-  <si>
     <t>Bark at the Moon</t>
   </si>
   <si>
@@ -1442,15 +1430,9 @@
     <t>Hannah Hunt</t>
   </si>
   <si>
-    <t>The Dark Side Of The Moon (50th Anniversary) [2023 Remaster]</t>
-  </si>
-  <si>
     <t>Nancy From Now On</t>
   </si>
   <si>
-    <t>Wildewoman (Expanded Edition)</t>
-  </si>
-  <si>
     <t>Underground</t>
   </si>
   <si>
@@ -1508,9 +1490,6 @@
     <t>Flyin (like a fast train)</t>
   </si>
   <si>
-    <t>Deeper Well: Deeper into the Well</t>
-  </si>
-  <si>
     <t>Track Name</t>
   </si>
   <si>
@@ -1623,6 +1602,27 @@
   </si>
   <si>
     <t>The Nurse</t>
+  </si>
+  <si>
+    <t>Bark At The Moon</t>
+  </si>
+  <si>
+    <t>1989 (Both Versions)</t>
+  </si>
+  <si>
+    <t>Loaded</t>
+  </si>
+  <si>
+    <t>Deeper Well</t>
+  </si>
+  <si>
+    <t>The Dark Side of the Moon</t>
+  </si>
+  <si>
+    <t>Two Star &amp; The Dream Police</t>
+  </si>
+  <si>
+    <t>Bitte Orca</t>
   </si>
 </sst>
 </file>
@@ -2375,12 +2375,12 @@
   <sheetPr>
     <tabColor rgb="FFCFC7FF"/>
   </sheetPr>
-  <dimension ref="A1:O106"/>
+  <dimension ref="A1:P106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G32" sqref="G32"/>
-      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
+      <selection pane="bottomLeft" activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2395,11 +2395,12 @@
     <col min="8" max="8" width="13.83203125" style="51" customWidth="1"/>
     <col min="9" max="9" width="3" customWidth="1"/>
     <col min="10" max="10" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="51.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" style="51" customWidth="1"/>
+    <col min="11" max="11" width="30.1640625" customWidth="1"/>
+    <col min="12" max="12" width="28.1640625" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" style="51" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="22" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="52" t="s">
         <v>295</v>
       </c>
@@ -2414,8 +2415,9 @@
       <c r="J1" s="52"/>
       <c r="K1" s="52"/>
       <c r="L1" s="52"/>
-    </row>
-    <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M1" s="52"/>
+    </row>
+    <row r="2" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
@@ -2430,8 +2432,9 @@
       <c r="J2" s="53"/>
       <c r="K2" s="53"/>
       <c r="L2" s="53"/>
-    </row>
-    <row r="3" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M2" s="53"/>
+    </row>
+    <row r="3" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="54" t="s">
         <v>1</v>
       </c>
@@ -2446,8 +2449,9 @@
       <c r="J3" s="54"/>
       <c r="K3" s="54"/>
       <c r="L3" s="54"/>
-    </row>
-    <row r="4" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M3" s="54"/>
+    </row>
+    <row r="4" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="22"/>
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
@@ -2459,9 +2463,10 @@
       <c r="I4" s="23"/>
       <c r="J4" s="23"/>
       <c r="K4" s="23"/>
-      <c r="L4" s="24"/>
-    </row>
-    <row r="5" spans="1:15" s="25" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L4" s="23"/>
+      <c r="M4" s="24"/>
+    </row>
+    <row r="5" spans="1:16" s="25" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="55" t="s">
         <v>196</v>
       </c>
@@ -2478,8 +2483,9 @@
       </c>
       <c r="K5" s="55"/>
       <c r="L5" s="55"/>
-    </row>
-    <row r="6" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M5" s="55"/>
+    </row>
+    <row r="6" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
         <v>2</v>
       </c>
@@ -2493,10 +2499,10 @@
         <v>2</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="H6" s="28" t="s">
         <v>197</v>
@@ -2505,13 +2511,16 @@
         <v>2</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>489</v>
-      </c>
-      <c r="L6" s="28" t="s">
+        <v>482</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>486</v>
+      </c>
+      <c r="M6" s="28" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="29">
         <v>1</v>
       </c>
@@ -2541,11 +2550,14 @@
       <c r="K7" s="30" t="s">
         <v>298</v>
       </c>
-      <c r="L7" s="33">
+      <c r="L7" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7" s="33">
         <v>756.05693333333329</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="34">
         <v>2</v>
       </c>
@@ -2575,11 +2587,14 @@
       <c r="K8" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="L8" s="36">
+      <c r="L8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" s="36">
         <v>646.74423333333334</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="34">
         <v>3</v>
       </c>
@@ -2609,11 +2624,14 @@
       <c r="K9" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="L9" s="36">
+      <c r="L9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="M9" s="36">
         <v>534.33128333333332</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="34">
         <v>4</v>
       </c>
@@ -2643,11 +2661,14 @@
       <c r="K10" s="10" t="s">
         <v>304</v>
       </c>
-      <c r="L10" s="36">
+      <c r="L10" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" s="36">
         <v>510.32485000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="34">
         <v>5</v>
       </c>
@@ -2677,12 +2698,15 @@
       <c r="K11" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="L11" s="36">
+      <c r="L11" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="M11" s="36">
         <v>453.36713333333336</v>
       </c>
-      <c r="O11" s="37"/>
-    </row>
-    <row r="12" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P11" s="37"/>
+    </row>
+    <row r="12" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="38">
         <v>6</v>
       </c>
@@ -2712,11 +2736,14 @@
       <c r="K12" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="L12" s="40">
+      <c r="L12" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12" s="40">
         <v>428.76588333333331</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="38">
         <v>7</v>
       </c>
@@ -2746,11 +2773,14 @@
       <c r="K13" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="L13" s="40">
+      <c r="L13" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="M13" s="40">
         <v>370.43581666666665</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="38">
         <v>8</v>
       </c>
@@ -2780,11 +2810,14 @@
       <c r="K14" s="16" t="s">
         <v>312</v>
       </c>
-      <c r="L14" s="40">
+      <c r="L14" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="M14" s="40">
         <v>345.12774999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="38">
         <v>9</v>
       </c>
@@ -2814,11 +2847,14 @@
       <c r="K15" s="16" t="s">
         <v>314</v>
       </c>
-      <c r="L15" s="40">
+      <c r="L15" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="M15" s="40">
         <v>340.55865</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="38">
         <v>10</v>
       </c>
@@ -2848,11 +2884,14 @@
       <c r="K16" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="L16" s="40">
+      <c r="L16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="M16" s="40">
         <v>314.25976666666668</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="41">
         <v>11</v>
       </c>
@@ -2882,11 +2921,14 @@
       <c r="K17" s="18" t="s">
         <v>318</v>
       </c>
-      <c r="L17" s="43">
+      <c r="L17" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="M17" s="43">
         <v>303.03643333333332</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="41">
         <v>12</v>
       </c>
@@ -2916,11 +2958,14 @@
       <c r="K18" s="18" t="s">
         <v>320</v>
       </c>
-      <c r="L18" s="43">
+      <c r="L18" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="M18" s="43">
         <v>298.90123333333332</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="41">
         <v>13</v>
       </c>
@@ -2935,7 +2980,7 @@
         <v>13</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G19" s="18" t="s">
         <v>6</v>
@@ -2948,13 +2993,16 @@
         <v>13</v>
       </c>
       <c r="K19" s="18" t="s">
-        <v>322</v>
-      </c>
-      <c r="L19" s="43">
-        <v>254.97268333333332</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>371</v>
+      </c>
+      <c r="L19" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19" s="43">
+        <v>275.70753333333334</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="41">
         <v>14</v>
       </c>
@@ -2969,7 +3017,7 @@
         <v>14</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G20" s="18" t="s">
         <v>8</v>
@@ -2982,13 +3030,16 @@
         <v>14</v>
       </c>
       <c r="K20" s="18" t="s">
-        <v>324</v>
-      </c>
-      <c r="L20" s="43">
-        <v>246.61775</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>519</v>
+      </c>
+      <c r="L20" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="M20" s="43">
+        <v>254.97268333333332</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="41">
         <v>15</v>
       </c>
@@ -3003,7 +3054,7 @@
         <v>15</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G21" s="18" t="s">
         <v>7</v>
@@ -3016,13 +3067,16 @@
         <v>15</v>
       </c>
       <c r="K21" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="L21" s="43">
-        <v>229.86106666666666</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>323</v>
+      </c>
+      <c r="L21" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="M21" s="43">
+        <v>246.61775</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="41">
         <v>16</v>
       </c>
@@ -3037,7 +3091,7 @@
         <v>16</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G22" s="18" t="s">
         <v>6</v>
@@ -3050,13 +3104,16 @@
         <v>16</v>
       </c>
       <c r="K22" s="18" t="s">
-        <v>327</v>
-      </c>
-      <c r="L22" s="43">
-        <v>220.91378333333333</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="L22" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="M22" s="43">
+        <v>229.86106666666666</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="41">
         <v>17</v>
       </c>
@@ -3071,7 +3128,7 @@
         <v>17</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G23" s="18" t="s">
         <v>5</v>
@@ -3084,13 +3141,16 @@
         <v>17</v>
       </c>
       <c r="K23" s="18" t="s">
-        <v>329</v>
-      </c>
-      <c r="L23" s="43">
-        <v>214.35374999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>326</v>
+      </c>
+      <c r="L23" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="M23" s="43">
+        <v>220.91378333333333</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="41">
         <v>18</v>
       </c>
@@ -3105,7 +3165,7 @@
         <v>18</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G24" s="18" t="s">
         <v>5</v>
@@ -3118,13 +3178,16 @@
         <v>18</v>
       </c>
       <c r="K24" s="18" t="s">
-        <v>331</v>
-      </c>
-      <c r="L24" s="43">
-        <v>183.71451666666667</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>328</v>
+      </c>
+      <c r="L24" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="M24" s="43">
+        <v>214.35374999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="41">
         <v>19</v>
       </c>
@@ -3139,7 +3202,7 @@
         <v>19</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G25" s="18" t="s">
         <v>5</v>
@@ -3152,13 +3215,16 @@
         <v>19</v>
       </c>
       <c r="K25" s="18" t="s">
-        <v>333</v>
-      </c>
-      <c r="L25" s="43">
-        <v>178.04235</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>332</v>
+      </c>
+      <c r="L25" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="M25" s="43">
+        <v>201.23169999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="41">
         <v>20</v>
       </c>
@@ -3173,7 +3239,7 @@
         <v>20</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G26" s="18" t="s">
         <v>7</v>
@@ -3186,13 +3252,16 @@
         <v>20</v>
       </c>
       <c r="K26" s="18" t="s">
-        <v>335</v>
-      </c>
-      <c r="L26" s="43">
-        <v>168.90061666666668</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+      <c r="L26" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="M26" s="43">
+        <v>183.71451666666667</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="44">
         <v>21</v>
       </c>
@@ -3220,13 +3289,16 @@
         <v>21</v>
       </c>
       <c r="K27" s="20" t="s">
-        <v>337</v>
-      </c>
-      <c r="L27" s="46">
-        <v>168.52018333333334</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>334</v>
+      </c>
+      <c r="L27" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="M27" s="46">
+        <v>168.90061666666668</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="44">
         <v>22</v>
       </c>
@@ -3241,7 +3313,7 @@
         <v>22</v>
       </c>
       <c r="F28" s="20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G28" s="20" t="s">
         <v>18</v>
@@ -3254,13 +3326,16 @@
         <v>22</v>
       </c>
       <c r="K28" s="20" t="s">
-        <v>339</v>
-      </c>
-      <c r="L28" s="46">
-        <v>167.96270000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>336</v>
+      </c>
+      <c r="L28" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="M28" s="46">
+        <v>168.52018333333334</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="44">
         <v>23</v>
       </c>
@@ -3275,7 +3350,7 @@
         <v>23</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G29" s="20" t="s">
         <v>8</v>
@@ -3288,13 +3363,16 @@
         <v>23</v>
       </c>
       <c r="K29" s="20" t="s">
-        <v>341</v>
-      </c>
-      <c r="L29" s="46">
-        <v>162.22446666666667</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>338</v>
+      </c>
+      <c r="L29" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="M29" s="46">
+        <v>167.96270000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="44">
         <v>24</v>
       </c>
@@ -3309,7 +3387,7 @@
         <v>24</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G30" s="20" t="s">
         <v>9</v>
@@ -3322,13 +3400,16 @@
         <v>24</v>
       </c>
       <c r="K30" s="20" t="s">
-        <v>343</v>
-      </c>
-      <c r="L30" s="46">
-        <v>149.07775000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>340</v>
+      </c>
+      <c r="L30" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="M30" s="46">
+        <v>162.22446666666667</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="44">
         <v>25</v>
       </c>
@@ -3343,7 +3424,7 @@
         <v>25</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G31" s="20" t="s">
         <v>9</v>
@@ -3356,13 +3437,16 @@
         <v>25</v>
       </c>
       <c r="K31" s="20" t="s">
-        <v>345</v>
-      </c>
-      <c r="L31" s="46">
-        <v>148.14113333333333</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>342</v>
+      </c>
+      <c r="L31" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="M31" s="46">
+        <v>149.07775000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="44">
         <v>26</v>
       </c>
@@ -3390,13 +3474,16 @@
         <v>26</v>
       </c>
       <c r="K32" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="L32" s="46">
-        <v>145.89376666666666</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+      <c r="L32" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="M32" s="46">
+        <v>148.14113333333333</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="44">
         <v>27</v>
       </c>
@@ -3411,7 +3498,7 @@
         <v>27</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G33" s="20" t="s">
         <v>5</v>
@@ -3424,13 +3511,16 @@
         <v>27</v>
       </c>
       <c r="K33" s="20" t="s">
-        <v>347</v>
-      </c>
-      <c r="L33" s="46">
-        <v>142.68594999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="L33" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="M33" s="46">
+        <v>145.89376666666666</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="44">
         <v>28</v>
       </c>
@@ -3445,7 +3535,7 @@
         <v>28</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G34" s="20" t="s">
         <v>6</v>
@@ -3458,13 +3548,16 @@
         <v>28</v>
       </c>
       <c r="K34" s="20" t="s">
-        <v>349</v>
-      </c>
-      <c r="L34" s="46">
-        <v>140.49725000000001</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>346</v>
+      </c>
+      <c r="L34" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="M34" s="46">
+        <v>142.68594999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="44">
         <v>29</v>
       </c>
@@ -3479,7 +3572,7 @@
         <v>29</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G35" s="20" t="s">
         <v>12</v>
@@ -3492,13 +3585,16 @@
         <v>29</v>
       </c>
       <c r="K35" s="20" t="s">
-        <v>351</v>
-      </c>
-      <c r="L35" s="46">
-        <v>138.87733333333333</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>348</v>
+      </c>
+      <c r="L35" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="M35" s="46">
+        <v>140.49725000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="44">
         <v>30</v>
       </c>
@@ -3513,7 +3609,7 @@
         <v>30</v>
       </c>
       <c r="F36" s="20" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G36" s="20" t="s">
         <v>27</v>
@@ -3526,13 +3622,16 @@
         <v>30</v>
       </c>
       <c r="K36" s="20" t="s">
-        <v>353</v>
-      </c>
-      <c r="L36" s="46">
-        <v>137.19011666666665</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>350</v>
+      </c>
+      <c r="L36" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="M36" s="46">
+        <v>138.87733333333333</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="44">
         <v>31</v>
       </c>
@@ -3547,7 +3646,7 @@
         <v>31</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G37" s="20" t="s">
         <v>11</v>
@@ -3560,13 +3659,16 @@
         <v>31</v>
       </c>
       <c r="K37" s="20" t="s">
-        <v>355</v>
-      </c>
-      <c r="L37" s="46">
-        <v>136.6472</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>352</v>
+      </c>
+      <c r="L37" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="M37" s="46">
+        <v>137.19011666666665</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="44">
         <v>32</v>
       </c>
@@ -3581,7 +3683,7 @@
         <v>32</v>
       </c>
       <c r="F38" s="20" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G38" s="20" t="s">
         <v>12</v>
@@ -3594,13 +3696,16 @@
         <v>32</v>
       </c>
       <c r="K38" s="20" t="s">
-        <v>357</v>
-      </c>
-      <c r="L38" s="46">
-        <v>134.17878333333334</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>354</v>
+      </c>
+      <c r="L38" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="M38" s="46">
+        <v>136.6472</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="44">
         <v>33</v>
       </c>
@@ -3615,7 +3720,7 @@
         <v>33</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G39" s="20" t="s">
         <v>5</v>
@@ -3628,13 +3733,16 @@
         <v>33</v>
       </c>
       <c r="K39" s="20" t="s">
-        <v>359</v>
-      </c>
-      <c r="L39" s="46">
-        <v>130.53331666666668</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>356</v>
+      </c>
+      <c r="L39" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="M39" s="46">
+        <v>134.17878333333334</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="44">
         <v>34</v>
       </c>
@@ -3649,7 +3757,7 @@
         <v>34</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G40" s="20" t="s">
         <v>5</v>
@@ -3662,13 +3770,16 @@
         <v>34</v>
       </c>
       <c r="K40" s="20" t="s">
-        <v>361</v>
-      </c>
-      <c r="L40" s="46">
-        <v>128.56056666666666</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>358</v>
+      </c>
+      <c r="L40" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="M40" s="46">
+        <v>130.53331666666668</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="44">
         <v>35</v>
       </c>
@@ -3683,7 +3794,7 @@
         <v>35</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G41" s="20" t="s">
         <v>6</v>
@@ -3696,13 +3807,16 @@
         <v>35</v>
       </c>
       <c r="K41" s="20" t="s">
-        <v>363</v>
-      </c>
-      <c r="L41" s="46">
-        <v>128.45701666666668</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>360</v>
+      </c>
+      <c r="L41" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="M41" s="46">
+        <v>129.04191666666668</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="44">
         <v>36</v>
       </c>
@@ -3717,7 +3831,7 @@
         <v>36</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="G42" s="20" t="s">
         <v>6</v>
@@ -3730,13 +3844,16 @@
         <v>36</v>
       </c>
       <c r="K42" s="20" t="s">
-        <v>365</v>
-      </c>
-      <c r="L42" s="46">
-        <v>128.04665</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>362</v>
+      </c>
+      <c r="L42" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="M42" s="46">
+        <v>128.45701666666668</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="44">
         <v>37</v>
       </c>
@@ -3751,7 +3868,7 @@
         <v>37</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G43" s="20" t="s">
         <v>6</v>
@@ -3764,13 +3881,16 @@
         <v>37</v>
       </c>
       <c r="K43" s="20" t="s">
-        <v>367</v>
-      </c>
-      <c r="L43" s="46">
-        <v>127.79783333333333</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>364</v>
+      </c>
+      <c r="L43" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="M43" s="46">
+        <v>128.04665</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="44">
         <v>38</v>
       </c>
@@ -3785,7 +3905,7 @@
         <v>38</v>
       </c>
       <c r="F44" s="20" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G44" s="20" t="s">
         <v>6</v>
@@ -3798,13 +3918,16 @@
         <v>38</v>
       </c>
       <c r="K44" s="20" t="s">
-        <v>369</v>
-      </c>
-      <c r="L44" s="46">
-        <v>125.76916666666666</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>366</v>
+      </c>
+      <c r="L44" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="M44" s="46">
+        <v>127.79783333333333</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="44">
         <v>39</v>
       </c>
@@ -3819,7 +3942,7 @@
         <v>39</v>
       </c>
       <c r="F45" s="20" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G45" s="20" t="s">
         <v>6</v>
@@ -3832,13 +3955,16 @@
         <v>39</v>
       </c>
       <c r="K45" s="20" t="s">
-        <v>371</v>
-      </c>
-      <c r="L45" s="46">
-        <v>120.94031666666666</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>368</v>
+      </c>
+      <c r="L45" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="M45" s="46">
+        <v>125.76916666666666</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="44">
         <v>40</v>
       </c>
@@ -3853,7 +3979,7 @@
         <v>40</v>
       </c>
       <c r="F46" s="20" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G46" s="20" t="s">
         <v>13</v>
@@ -3866,13 +3992,16 @@
         <v>40</v>
       </c>
       <c r="K46" s="20" t="s">
-        <v>372</v>
-      </c>
-      <c r="L46" s="46">
-        <v>117.79996666666666</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>370</v>
+      </c>
+      <c r="L46" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="M46" s="46">
+        <v>120.94031666666666</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="44">
         <v>41</v>
       </c>
@@ -3887,7 +4016,7 @@
         <v>41</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G47" s="20" t="s">
         <v>11</v>
@@ -3900,13 +4029,16 @@
         <v>41</v>
       </c>
       <c r="K47" s="20" t="s">
-        <v>374</v>
-      </c>
-      <c r="L47" s="46">
-        <v>115.82810000000001</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>409</v>
+      </c>
+      <c r="L47" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="M47" s="46">
+        <v>120.41686666666666</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="44">
         <v>42</v>
       </c>
@@ -3921,7 +4053,7 @@
         <v>42</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G48" s="20" t="s">
         <v>9</v>
@@ -3934,13 +4066,16 @@
         <v>42</v>
       </c>
       <c r="K48" s="20" t="s">
-        <v>376</v>
-      </c>
-      <c r="L48" s="46">
-        <v>109.71169999999999</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>373</v>
+      </c>
+      <c r="L48" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="M48" s="46">
+        <v>115.82810000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="44">
         <v>43</v>
       </c>
@@ -3955,7 +4090,7 @@
         <v>43</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G49" s="20" t="s">
         <v>14</v>
@@ -3968,13 +4103,16 @@
         <v>43</v>
       </c>
       <c r="K49" s="20" t="s">
-        <v>378</v>
-      </c>
-      <c r="L49" s="46">
-        <v>108.90828333333333</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>375</v>
+      </c>
+      <c r="L49" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="M49" s="46">
+        <v>109.71169999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="44">
         <v>44</v>
       </c>
@@ -3989,7 +4127,7 @@
         <v>44</v>
       </c>
       <c r="F50" s="20" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G50" s="20" t="s">
         <v>6</v>
@@ -4002,13 +4140,16 @@
         <v>44</v>
       </c>
       <c r="K50" s="20" t="s">
-        <v>380</v>
-      </c>
-      <c r="L50" s="46">
-        <v>106.99893333333333</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+      <c r="L50" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="M50" s="46">
+        <v>108.90828333333333</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="44">
         <v>45</v>
       </c>
@@ -4023,7 +4164,7 @@
         <v>45</v>
       </c>
       <c r="F51" s="20" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G51" s="20" t="s">
         <v>5</v>
@@ -4036,13 +4177,16 @@
         <v>45</v>
       </c>
       <c r="K51" s="20" t="s">
-        <v>382</v>
-      </c>
-      <c r="L51" s="46">
-        <v>106.43083333333334</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>379</v>
+      </c>
+      <c r="L51" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="M51" s="46">
+        <v>106.99893333333333</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="44">
         <v>46</v>
       </c>
@@ -4057,7 +4201,7 @@
         <v>46</v>
       </c>
       <c r="F52" s="20" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G52" s="20" t="s">
         <v>7</v>
@@ -4070,13 +4214,16 @@
         <v>46</v>
       </c>
       <c r="K52" s="20" t="s">
-        <v>384</v>
-      </c>
-      <c r="L52" s="46">
-        <v>105.90445</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>381</v>
+      </c>
+      <c r="L52" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="M52" s="46">
+        <v>106.43083333333334</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="44">
         <v>47</v>
       </c>
@@ -4091,7 +4238,7 @@
         <v>47</v>
       </c>
       <c r="F53" s="20" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G53" s="20" t="s">
         <v>5</v>
@@ -4104,13 +4251,16 @@
         <v>47</v>
       </c>
       <c r="K53" s="20" t="s">
-        <v>386</v>
-      </c>
-      <c r="L53" s="46">
-        <v>91.269866666666672</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>383</v>
+      </c>
+      <c r="L53" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="M53" s="46">
+        <v>105.90445</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="44">
         <v>48</v>
       </c>
@@ -4125,7 +4275,7 @@
         <v>48</v>
       </c>
       <c r="F54" s="20" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G54" s="20" t="s">
         <v>7</v>
@@ -4138,13 +4288,16 @@
         <v>48</v>
       </c>
       <c r="K54" s="20" t="s">
-        <v>388</v>
-      </c>
-      <c r="L54" s="46">
-        <v>88.534833333333339</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>520</v>
+      </c>
+      <c r="L54" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="M54" s="46">
+        <v>102.5929</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="44">
         <v>49</v>
       </c>
@@ -4159,7 +4312,7 @@
         <v>49</v>
       </c>
       <c r="F55" s="20" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G55" s="20" t="s">
         <v>21</v>
@@ -4172,13 +4325,16 @@
         <v>49</v>
       </c>
       <c r="K55" s="20" t="s">
-        <v>390</v>
-      </c>
-      <c r="L55" s="46">
-        <v>88.313266666666664</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>385</v>
+      </c>
+      <c r="L55" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="M55" s="46">
+        <v>91.269866666666672</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="44">
         <v>50</v>
       </c>
@@ -4193,7 +4349,7 @@
         <v>50</v>
       </c>
       <c r="F56" s="20" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G56" s="20" t="s">
         <v>9</v>
@@ -4206,13 +4362,16 @@
         <v>50</v>
       </c>
       <c r="K56" s="20" t="s">
-        <v>392</v>
-      </c>
-      <c r="L56" s="46">
-        <v>84.480833333333337</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>387</v>
+      </c>
+      <c r="L56" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="M56" s="46">
+        <v>88.534833333333339</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="44">
         <v>51</v>
       </c>
@@ -4227,7 +4386,7 @@
         <v>51</v>
       </c>
       <c r="F57" s="20" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G57" s="20" t="s">
         <v>8</v>
@@ -4240,13 +4399,16 @@
         <v>51</v>
       </c>
       <c r="K57" s="20" t="s">
-        <v>394</v>
-      </c>
-      <c r="L57" s="46">
-        <v>82.130449999999996</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>389</v>
+      </c>
+      <c r="L57" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="M57" s="46">
+        <v>88.313266666666664</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="44">
         <v>52</v>
       </c>
@@ -4261,7 +4423,7 @@
         <v>52</v>
       </c>
       <c r="F58" s="20" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G58" s="20" t="s">
         <v>11</v>
@@ -4274,13 +4436,16 @@
         <v>52</v>
       </c>
       <c r="K58" s="20" t="s">
-        <v>396</v>
-      </c>
-      <c r="L58" s="46">
-        <v>77.424366666666671</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>437</v>
+      </c>
+      <c r="L58" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="M58" s="46">
+        <v>87.646199999999993</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="44">
         <v>53</v>
       </c>
@@ -4295,7 +4460,7 @@
         <v>53</v>
       </c>
       <c r="F59" s="20" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G59" s="20" t="s">
         <v>18</v>
@@ -4308,13 +4473,16 @@
         <v>53</v>
       </c>
       <c r="K59" s="20" t="s">
-        <v>398</v>
-      </c>
-      <c r="L59" s="46">
-        <v>76.042216666666661</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>391</v>
+      </c>
+      <c r="L59" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="M59" s="46">
+        <v>84.480833333333337</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="44">
         <v>54</v>
       </c>
@@ -4329,7 +4497,7 @@
         <v>54</v>
       </c>
       <c r="F60" s="20" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="G60" s="20" t="s">
         <v>6</v>
@@ -4342,13 +4510,16 @@
         <v>54</v>
       </c>
       <c r="K60" s="20" t="s">
-        <v>400</v>
-      </c>
-      <c r="L60" s="46">
-        <v>73.640483333333336</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>393</v>
+      </c>
+      <c r="L60" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="M60" s="46">
+        <v>82.130449999999996</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="44">
         <v>55</v>
       </c>
@@ -4363,7 +4534,7 @@
         <v>55</v>
       </c>
       <c r="F61" s="20" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="G61" s="20" t="s">
         <v>6</v>
@@ -4376,13 +4547,16 @@
         <v>55</v>
       </c>
       <c r="K61" s="20" t="s">
-        <v>402</v>
-      </c>
-      <c r="L61" s="46">
-        <v>70.080966666666669</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>521</v>
+      </c>
+      <c r="L61" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="M61" s="46">
+        <v>79.076499999999996</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="44">
         <v>56</v>
       </c>
@@ -4397,7 +4571,7 @@
         <v>56</v>
       </c>
       <c r="F62" s="20" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="G62" s="20" t="s">
         <v>18</v>
@@ -4410,13 +4584,16 @@
         <v>56</v>
       </c>
       <c r="K62" s="20" t="s">
-        <v>404</v>
-      </c>
-      <c r="L62" s="46">
-        <v>68.235749999999996</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>395</v>
+      </c>
+      <c r="L62" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="M62" s="46">
+        <v>77.424366666666671</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="44">
         <v>57</v>
       </c>
@@ -4431,7 +4608,7 @@
         <v>57</v>
       </c>
       <c r="F63" s="20" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="G63" s="20" t="s">
         <v>9</v>
@@ -4444,13 +4621,16 @@
         <v>57</v>
       </c>
       <c r="K63" s="20" t="s">
-        <v>406</v>
-      </c>
-      <c r="L63" s="46">
-        <v>66.422200000000004</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>398</v>
+      </c>
+      <c r="L63" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="M63" s="46">
+        <v>73.640483333333336</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="44">
         <v>58</v>
       </c>
@@ -4465,7 +4645,7 @@
         <v>58</v>
       </c>
       <c r="F64" s="20" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="G64" s="20" t="s">
         <v>5</v>
@@ -4478,13 +4658,16 @@
         <v>58</v>
       </c>
       <c r="K64" s="20" t="s">
-        <v>408</v>
-      </c>
-      <c r="L64" s="46">
-        <v>65.13655</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>401</v>
+      </c>
+      <c r="L64" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="M64" s="46">
+        <v>68.235749999999996</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="44">
         <v>59</v>
       </c>
@@ -4499,7 +4682,7 @@
         <v>59</v>
       </c>
       <c r="F65" s="20" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="G65" s="20" t="s">
         <v>14</v>
@@ -4512,13 +4695,16 @@
         <v>59</v>
       </c>
       <c r="K65" s="20" t="s">
-        <v>410</v>
-      </c>
-      <c r="L65" s="46">
-        <v>64.994466666666668</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>403</v>
+      </c>
+      <c r="L65" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="M65" s="46">
+        <v>66.422200000000004</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="44">
         <v>60</v>
       </c>
@@ -4533,7 +4719,7 @@
         <v>60</v>
       </c>
       <c r="F66" s="20" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="G66" s="20" t="s">
         <v>8</v>
@@ -4546,13 +4732,16 @@
         <v>60</v>
       </c>
       <c r="K66" s="20" t="s">
-        <v>412</v>
-      </c>
-      <c r="L66" s="46">
-        <v>64.283183333333326</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>405</v>
+      </c>
+      <c r="L66" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="M66" s="46">
+        <v>65.13655</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="44">
         <v>61</v>
       </c>
@@ -4567,7 +4756,7 @@
         <v>61</v>
       </c>
       <c r="F67" s="20" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="G67" s="20" t="s">
         <v>5</v>
@@ -4580,13 +4769,16 @@
         <v>61</v>
       </c>
       <c r="K67" s="20" t="s">
-        <v>414</v>
-      </c>
-      <c r="L67" s="46">
-        <v>63.330783333333336</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>407</v>
+      </c>
+      <c r="L67" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="M67" s="46">
+        <v>64.994466666666668</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="44">
         <v>62</v>
       </c>
@@ -4601,7 +4793,7 @@
         <v>62</v>
       </c>
       <c r="F68" s="20" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="G68" s="20" t="s">
         <v>5</v>
@@ -4614,13 +4806,16 @@
         <v>62</v>
       </c>
       <c r="K68" s="20" t="s">
-        <v>416</v>
-      </c>
-      <c r="L68" s="46">
-        <v>61.830116666666669</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+      <c r="L68" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="M68" s="46">
+        <v>63.330783333333336</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="44">
         <v>63</v>
       </c>
@@ -4635,7 +4830,7 @@
         <v>63</v>
       </c>
       <c r="F69" s="20" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="G69" s="20" t="s">
         <v>18</v>
@@ -4648,13 +4843,16 @@
         <v>63</v>
       </c>
       <c r="K69" s="20" t="s">
-        <v>418</v>
-      </c>
-      <c r="L69" s="46">
-        <v>61.559150000000002</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>413</v>
+      </c>
+      <c r="L69" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="M69" s="46">
+        <v>61.830116666666669</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="44">
         <v>64</v>
       </c>
@@ -4669,7 +4867,7 @@
         <v>64</v>
       </c>
       <c r="F70" s="20" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="G70" s="20" t="s">
         <v>7</v>
@@ -4682,13 +4880,16 @@
         <v>64</v>
       </c>
       <c r="K70" s="20" t="s">
-        <v>420</v>
-      </c>
-      <c r="L70" s="46">
-        <v>57.091233333333335</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>415</v>
+      </c>
+      <c r="L70" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="M70" s="46">
+        <v>61.559150000000002</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="44">
         <v>65</v>
       </c>
@@ -4703,7 +4904,7 @@
         <v>65</v>
       </c>
       <c r="F71" s="20" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="G71" s="20" t="s">
         <v>18</v>
@@ -4716,13 +4917,16 @@
         <v>65</v>
       </c>
       <c r="K71" s="20" t="s">
-        <v>422</v>
-      </c>
-      <c r="L71" s="46">
-        <v>56.603200000000001</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="L71" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="M71" s="46">
+        <v>57.091233333333335</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="44">
         <v>66</v>
       </c>
@@ -4737,7 +4941,7 @@
         <v>66</v>
       </c>
       <c r="F72" s="20" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="G72" s="20" t="s">
         <v>7</v>
@@ -4750,13 +4954,16 @@
         <v>66</v>
       </c>
       <c r="K72" s="20" t="s">
-        <v>424</v>
-      </c>
-      <c r="L72" s="46">
-        <v>56.13368333333333</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="L72" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="M72" s="46">
+        <v>56.603200000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="44">
         <v>67</v>
       </c>
@@ -4771,7 +4978,7 @@
         <v>67</v>
       </c>
       <c r="F73" s="20" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G73" s="20" t="s">
         <v>29</v>
@@ -4784,13 +4991,16 @@
         <v>67</v>
       </c>
       <c r="K73" s="20" t="s">
-        <v>426</v>
-      </c>
-      <c r="L73" s="46">
+        <v>422</v>
+      </c>
+      <c r="L73" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="M73" s="46">
         <v>55.9268</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="44">
         <v>68</v>
       </c>
@@ -4805,7 +5015,7 @@
         <v>68</v>
       </c>
       <c r="F74" s="20" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="G74" s="20" t="s">
         <v>9</v>
@@ -4818,13 +5028,16 @@
         <v>68</v>
       </c>
       <c r="K74" s="20" t="s">
-        <v>427</v>
-      </c>
-      <c r="L74" s="46">
+        <v>423</v>
+      </c>
+      <c r="L74" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="M74" s="46">
         <v>55.613100000000003</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="44">
         <v>69</v>
       </c>
@@ -4839,7 +5052,7 @@
         <v>69</v>
       </c>
       <c r="F75" s="20" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="G75" s="20" t="s">
         <v>6</v>
@@ -4852,13 +5065,16 @@
         <v>69</v>
       </c>
       <c r="K75" s="20" t="s">
-        <v>429</v>
-      </c>
-      <c r="L75" s="46">
-        <v>54.5002</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>435</v>
+      </c>
+      <c r="L75" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="M75" s="46">
+        <v>54.525199999999998</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="44">
         <v>70</v>
       </c>
@@ -4873,7 +5089,7 @@
         <v>70</v>
       </c>
       <c r="F76" s="20" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="G76" s="20" t="s">
         <v>5</v>
@@ -4886,13 +5102,16 @@
         <v>70</v>
       </c>
       <c r="K76" s="20" t="s">
-        <v>431</v>
-      </c>
-      <c r="L76" s="46">
-        <v>52.543599999999998</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="L76" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="M76" s="46">
+        <v>54.5002</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="44">
         <v>71</v>
       </c>
@@ -4907,7 +5126,7 @@
         <v>71</v>
       </c>
       <c r="F77" s="20" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="G77" s="20" t="s">
         <v>6</v>
@@ -4920,13 +5139,16 @@
         <v>71</v>
       </c>
       <c r="K77" s="20" t="s">
-        <v>433</v>
-      </c>
-      <c r="L77" s="46">
-        <v>52.16825</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>427</v>
+      </c>
+      <c r="L77" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="M77" s="46">
+        <v>52.543599999999998</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="44">
         <v>72</v>
       </c>
@@ -4941,7 +5163,7 @@
         <v>72</v>
       </c>
       <c r="F78" s="20" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="G78" s="20" t="s">
         <v>11</v>
@@ -4954,13 +5176,16 @@
         <v>72</v>
       </c>
       <c r="K78" s="20" t="s">
-        <v>435</v>
-      </c>
-      <c r="L78" s="46">
-        <v>51.807549999999999</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>429</v>
+      </c>
+      <c r="L78" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="M78" s="46">
+        <v>52.16825</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="44">
         <v>73</v>
       </c>
@@ -4975,7 +5200,7 @@
         <v>73</v>
       </c>
       <c r="F79" s="20" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="G79" s="20" t="s">
         <v>7</v>
@@ -4988,13 +5213,16 @@
         <v>73</v>
       </c>
       <c r="K79" s="20" t="s">
-        <v>437</v>
-      </c>
-      <c r="L79" s="46">
-        <v>51.616999999999997</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>431</v>
+      </c>
+      <c r="L79" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="M79" s="46">
+        <v>51.807549999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="44">
         <v>74</v>
       </c>
@@ -5009,7 +5237,7 @@
         <v>74</v>
       </c>
       <c r="F80" s="20" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="G80" s="20" t="s">
         <v>6</v>
@@ -5022,13 +5250,16 @@
         <v>74</v>
       </c>
       <c r="K80" s="20" t="s">
-        <v>439</v>
-      </c>
-      <c r="L80" s="46">
-        <v>50.596249999999998</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>433</v>
+      </c>
+      <c r="L80" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="M80" s="46">
+        <v>51.616999999999997</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="44">
         <v>75</v>
       </c>
@@ -5056,13 +5287,16 @@
         <v>75</v>
       </c>
       <c r="K81" s="20" t="s">
-        <v>441</v>
-      </c>
-      <c r="L81" s="46">
-        <v>50.034050000000001</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>450</v>
+      </c>
+      <c r="L81" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="M81" s="46">
+        <v>50.907166666666669</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="44">
         <v>76</v>
       </c>
@@ -5077,7 +5311,7 @@
         <v>76</v>
       </c>
       <c r="F82" s="20" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="G82" s="20" t="s">
         <v>12</v>
@@ -5090,13 +5324,16 @@
         <v>76</v>
       </c>
       <c r="K82" s="20" t="s">
-        <v>442</v>
-      </c>
-      <c r="L82" s="46">
+        <v>438</v>
+      </c>
+      <c r="L82" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="M82" s="46">
         <v>49.198816666666666</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="44">
         <v>77</v>
       </c>
@@ -5111,7 +5348,7 @@
         <v>77</v>
       </c>
       <c r="F83" s="20" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="G83" s="20" t="s">
         <v>12</v>
@@ -5124,13 +5361,16 @@
         <v>77</v>
       </c>
       <c r="K83" s="20" t="s">
-        <v>444</v>
-      </c>
-      <c r="L83" s="46">
+        <v>440</v>
+      </c>
+      <c r="L83" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="M83" s="46">
         <v>48.018916666666669</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="44">
         <v>78</v>
       </c>
@@ -5145,7 +5385,7 @@
         <v>78</v>
       </c>
       <c r="F84" s="20" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="G84" s="20" t="s">
         <v>6</v>
@@ -5158,13 +5398,16 @@
         <v>78</v>
       </c>
       <c r="K84" s="20" t="s">
-        <v>446</v>
-      </c>
-      <c r="L84" s="46">
+        <v>442</v>
+      </c>
+      <c r="L84" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="M84" s="46">
         <v>46.793799999999997</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="44">
         <v>79</v>
       </c>
@@ -5179,7 +5422,7 @@
         <v>79</v>
       </c>
       <c r="F85" s="20" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="G85" s="20" t="s">
         <v>13</v>
@@ -5192,13 +5435,16 @@
         <v>79</v>
       </c>
       <c r="K85" s="20" t="s">
-        <v>448</v>
-      </c>
-      <c r="L85" s="46">
+        <v>444</v>
+      </c>
+      <c r="L85" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="M85" s="46">
         <v>45.763733333333334</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="44">
         <v>80</v>
       </c>
@@ -5226,13 +5472,16 @@
         <v>80</v>
       </c>
       <c r="K86" s="20" t="s">
-        <v>450</v>
-      </c>
-      <c r="L86" s="46">
-        <v>44.04613333333333</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>522</v>
+      </c>
+      <c r="L86" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="M86" s="46">
+        <v>44.403633333333332</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="44">
         <v>81</v>
       </c>
@@ -5247,7 +5496,7 @@
         <v>81</v>
       </c>
       <c r="F87" s="20" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="G87" s="20" t="s">
         <v>7</v>
@@ -5260,13 +5509,16 @@
         <v>81</v>
       </c>
       <c r="K87" s="20" t="s">
-        <v>452</v>
-      </c>
-      <c r="L87" s="46">
-        <v>43.24346666666667</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>446</v>
+      </c>
+      <c r="L87" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="M87" s="46">
+        <v>44.04613333333333</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="44">
         <v>82</v>
       </c>
@@ -5281,7 +5533,7 @@
         <v>82</v>
       </c>
       <c r="F88" s="20" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="G88" s="20" t="s">
         <v>24</v>
@@ -5294,13 +5546,16 @@
         <v>82</v>
       </c>
       <c r="K88" s="20" t="s">
-        <v>454</v>
-      </c>
-      <c r="L88" s="46">
-        <v>42.693516666666667</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>448</v>
+      </c>
+      <c r="L88" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="M88" s="46">
+        <v>43.24346666666667</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="44">
         <v>83</v>
       </c>
@@ -5315,7 +5570,7 @@
         <v>83</v>
       </c>
       <c r="F89" s="20" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="G89" s="20" t="s">
         <v>5</v>
@@ -5330,11 +5585,14 @@
       <c r="K89" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="L89" s="46">
+      <c r="L89" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="M89" s="46">
         <v>42.150483333333334</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="44">
         <v>84</v>
       </c>
@@ -5349,7 +5607,7 @@
         <v>84</v>
       </c>
       <c r="F90" s="20" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="G90" s="20" t="s">
         <v>25</v>
@@ -5362,13 +5620,16 @@
         <v>84</v>
       </c>
       <c r="K90" s="20" t="s">
-        <v>457</v>
-      </c>
-      <c r="L90" s="46">
-        <v>40.891950000000001</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>523</v>
+      </c>
+      <c r="L90" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="M90" s="46">
+        <v>40.898600000000002</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="44">
         <v>85</v>
       </c>
@@ -5383,7 +5644,7 @@
         <v>85</v>
       </c>
       <c r="F91" s="20" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="G91" s="20" t="s">
         <v>5</v>
@@ -5396,13 +5657,16 @@
         <v>85</v>
       </c>
       <c r="K91" s="20" t="s">
-        <v>459</v>
-      </c>
-      <c r="L91" s="46">
-        <v>40.426666666666669</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>453</v>
+      </c>
+      <c r="L91" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="M91" s="46">
+        <v>40.891950000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="44">
         <v>86</v>
       </c>
@@ -5417,7 +5681,7 @@
         <v>86</v>
       </c>
       <c r="F92" s="20" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="G92" s="20" t="s">
         <v>8</v>
@@ -5430,13 +5694,16 @@
         <v>86</v>
       </c>
       <c r="K92" s="20" t="s">
-        <v>461</v>
-      </c>
-      <c r="L92" s="46">
-        <v>39.444633333333336</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>455</v>
+      </c>
+      <c r="L92" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="M92" s="46">
+        <v>40.426666666666669</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="44">
         <v>87</v>
       </c>
@@ -5451,7 +5718,7 @@
         <v>87</v>
       </c>
       <c r="F93" s="20" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="G93" s="20" t="s">
         <v>6</v>
@@ -5464,13 +5731,16 @@
         <v>87</v>
       </c>
       <c r="K93" s="20" t="s">
-        <v>463</v>
-      </c>
-      <c r="L93" s="46">
-        <v>38.128</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>457</v>
+      </c>
+      <c r="L93" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="M93" s="46">
+        <v>39.444633333333336</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="44">
         <v>88</v>
       </c>
@@ -5485,7 +5755,7 @@
         <v>88</v>
       </c>
       <c r="F94" s="20" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="G94" s="20" t="s">
         <v>5</v>
@@ -5498,13 +5768,16 @@
         <v>88</v>
       </c>
       <c r="K94" s="20" t="s">
-        <v>465</v>
-      </c>
-      <c r="L94" s="46">
-        <v>38.073033333333335</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>459</v>
+      </c>
+      <c r="L94" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="M94" s="46">
+        <v>38.128</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="44">
         <v>89</v>
       </c>
@@ -5519,7 +5792,7 @@
         <v>89</v>
       </c>
       <c r="F95" s="20" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="G95" s="20" t="s">
         <v>9</v>
@@ -5532,13 +5805,16 @@
         <v>89</v>
       </c>
       <c r="K95" s="20" t="s">
-        <v>467</v>
-      </c>
-      <c r="L95" s="46">
-        <v>37.61215</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>394</v>
+      </c>
+      <c r="L95" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="M95" s="46">
+        <v>37.340316666666666</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="44">
         <v>90</v>
       </c>
@@ -5553,7 +5829,7 @@
         <v>90</v>
       </c>
       <c r="F96" s="20" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="G96" s="20" t="s">
         <v>14</v>
@@ -5566,13 +5842,16 @@
         <v>90</v>
       </c>
       <c r="K96" s="20" t="s">
-        <v>395</v>
-      </c>
-      <c r="L96" s="46">
-        <v>37.340316666666666</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>464</v>
+      </c>
+      <c r="L96" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="M96" s="46">
+        <v>37.040599999999998</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="44">
         <v>91</v>
       </c>
@@ -5587,7 +5866,7 @@
         <v>91</v>
       </c>
       <c r="F97" s="20" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="G97" s="20" t="s">
         <v>15</v>
@@ -5600,13 +5879,16 @@
         <v>91</v>
       </c>
       <c r="K97" s="20" t="s">
-        <v>470</v>
-      </c>
-      <c r="L97" s="46">
-        <v>37.040599999999998</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>466</v>
+      </c>
+      <c r="L97" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="M97" s="46">
+        <v>36.776383333333335</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="44">
         <v>92</v>
       </c>
@@ -5621,7 +5903,7 @@
         <v>92</v>
       </c>
       <c r="F98" s="20" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="G98" s="20" t="s">
         <v>12</v>
@@ -5634,13 +5916,16 @@
         <v>92</v>
       </c>
       <c r="K98" s="20" t="s">
-        <v>472</v>
-      </c>
-      <c r="L98" s="46">
-        <v>36.776383333333335</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>468</v>
+      </c>
+      <c r="L98" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="M98" s="46">
+        <v>36.688600000000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="44">
         <v>93</v>
       </c>
@@ -5655,7 +5940,7 @@
         <v>93</v>
       </c>
       <c r="F99" s="20" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="G99" s="20" t="s">
         <v>36</v>
@@ -5668,13 +5953,16 @@
         <v>93</v>
       </c>
       <c r="K99" s="20" t="s">
-        <v>474</v>
-      </c>
-      <c r="L99" s="46">
-        <v>36.688600000000001</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>470</v>
+      </c>
+      <c r="L99" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="M99" s="46">
+        <v>36.542666666666669</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="44">
         <v>94</v>
       </c>
@@ -5689,7 +5977,7 @@
         <v>94</v>
       </c>
       <c r="F100" s="20" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="G100" s="20" t="s">
         <v>7</v>
@@ -5702,13 +5990,16 @@
         <v>94</v>
       </c>
       <c r="K100" s="20" t="s">
-        <v>476</v>
-      </c>
-      <c r="L100" s="46">
-        <v>36.542666666666669</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>472</v>
+      </c>
+      <c r="L100" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="M100" s="46">
+        <v>35.780799999999999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="44">
         <v>95</v>
       </c>
@@ -5723,7 +6014,7 @@
         <v>95</v>
       </c>
       <c r="F101" s="20" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="G101" s="20" t="s">
         <v>14</v>
@@ -5736,13 +6027,16 @@
         <v>95</v>
       </c>
       <c r="K101" s="20" t="s">
-        <v>478</v>
-      </c>
-      <c r="L101" s="46">
-        <v>35.780799999999999</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>474</v>
+      </c>
+      <c r="L101" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="M101" s="46">
+        <v>35.665983333333337</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="44">
         <v>96</v>
       </c>
@@ -5757,7 +6051,7 @@
         <v>96</v>
       </c>
       <c r="F102" s="20" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="G102" s="20" t="s">
         <v>5</v>
@@ -5770,13 +6064,16 @@
         <v>96</v>
       </c>
       <c r="K102" s="20" t="s">
-        <v>480</v>
-      </c>
-      <c r="L102" s="46">
-        <v>35.665983333333337</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>475</v>
+      </c>
+      <c r="L102" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="M102" s="46">
+        <v>34.720950000000002</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="44">
         <v>97</v>
       </c>
@@ -5791,7 +6088,7 @@
         <v>97</v>
       </c>
       <c r="F103" s="20" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="G103" s="20" t="s">
         <v>6</v>
@@ -5804,13 +6101,16 @@
         <v>97</v>
       </c>
       <c r="K103" s="20" t="s">
-        <v>481</v>
-      </c>
-      <c r="L103" s="46">
-        <v>34.720950000000002</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>477</v>
+      </c>
+      <c r="L103" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="M103" s="46">
+        <v>33.522950000000002</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="44">
         <v>98</v>
       </c>
@@ -5838,13 +6138,16 @@
         <v>98</v>
       </c>
       <c r="K104" s="20" t="s">
-        <v>483</v>
-      </c>
-      <c r="L104" s="46">
-        <v>33.522950000000002</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>479</v>
+      </c>
+      <c r="L104" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="M104" s="46">
+        <v>33.484116666666665</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="44">
         <v>99</v>
       </c>
@@ -5859,7 +6162,7 @@
         <v>99</v>
       </c>
       <c r="F105" s="20" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="G105" s="20" t="s">
         <v>32</v>
@@ -5872,13 +6175,16 @@
         <v>99</v>
       </c>
       <c r="K105" s="20" t="s">
-        <v>485</v>
-      </c>
-      <c r="L105" s="46">
-        <v>33.484116666666665</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+        <v>524</v>
+      </c>
+      <c r="L105" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="M105" s="46">
+        <v>32.133566666666667</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="47">
         <v>100</v>
       </c>
@@ -5893,7 +6199,7 @@
         <v>100</v>
       </c>
       <c r="F106" s="48" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="G106" s="48" t="s">
         <v>8</v>
@@ -5906,20 +6212,23 @@
         <v>100</v>
       </c>
       <c r="K106" s="48" t="s">
-        <v>487</v>
-      </c>
-      <c r="L106" s="50">
-        <v>32.550016666666664</v>
+        <v>525</v>
+      </c>
+      <c r="L106" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="M106" s="50">
+        <v>31.903949999999998</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="E5:H5"/>
-    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J5:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6592,7 +6901,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="52" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="B1" s="52"/>
       <c r="C1" s="52"/>
@@ -6608,7 +6917,7 @@
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="53" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="B2" s="53"/>
       <c r="C2" s="53"/>
@@ -6624,7 +6933,7 @@
     </row>
     <row r="3" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="54" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="B3" s="54"/>
       <c r="C3" s="54"/>
@@ -6684,10 +6993,10 @@
         <v>2</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="H6" s="28" t="s">
         <v>197</v>
@@ -6696,7 +7005,7 @@
         <v>2</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="L6" s="28" t="s">
         <v>197</v>
@@ -6715,7 +7024,7 @@
       <c r="D7" s="32"/>
       <c r="E7" s="29"/>
       <c r="F7" s="30" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G7" s="30" t="s">
         <v>8</v>
@@ -6767,7 +7076,7 @@
       <c r="D9" s="32"/>
       <c r="E9" s="34"/>
       <c r="F9" s="10" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>21</v>
@@ -6793,7 +7102,7 @@
       <c r="D10" s="32"/>
       <c r="E10" s="34"/>
       <c r="F10" s="10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>5</v>
@@ -6846,7 +7155,7 @@
       <c r="D12" s="32"/>
       <c r="E12" s="38"/>
       <c r="F12" s="16" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="G12" s="16" t="s">
         <v>15</v>
@@ -6872,7 +7181,7 @@
       <c r="D13" s="32"/>
       <c r="E13" s="38"/>
       <c r="F13" s="16" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G13" s="16" t="s">
         <v>6</v>
@@ -6898,7 +7207,7 @@
       <c r="D14" s="32"/>
       <c r="E14" s="38"/>
       <c r="F14" s="16" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="G14" s="16" t="s">
         <v>15</v>
@@ -6924,7 +7233,7 @@
       <c r="D15" s="32"/>
       <c r="E15" s="38"/>
       <c r="F15" s="16" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="G15" s="16" t="s">
         <v>28</v>
@@ -6950,7 +7259,7 @@
       <c r="D16" s="32"/>
       <c r="E16" s="38"/>
       <c r="F16" s="16" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="G16" s="16" t="s">
         <v>8</v>
@@ -6976,7 +7285,7 @@
       <c r="D17" s="32"/>
       <c r="E17" s="41"/>
       <c r="F17" s="18" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="G17" s="18" t="s">
         <v>30</v>
@@ -7002,7 +7311,7 @@
       <c r="D18" s="32"/>
       <c r="E18" s="41"/>
       <c r="F18" s="18" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="G18" s="18" t="s">
         <v>21</v>
@@ -7028,7 +7337,7 @@
       <c r="D19" s="32"/>
       <c r="E19" s="41"/>
       <c r="F19" s="18" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="G19" s="18" t="s">
         <v>15</v>
@@ -7054,7 +7363,7 @@
       <c r="D20" s="32"/>
       <c r="E20" s="41"/>
       <c r="F20" s="18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G20" s="18" t="s">
         <v>6</v>
@@ -7080,7 +7389,7 @@
       <c r="D21" s="32"/>
       <c r="E21" s="41"/>
       <c r="F21" s="18" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="G21" s="18" t="s">
         <v>8</v>
@@ -7106,7 +7415,7 @@
       <c r="D22" s="32"/>
       <c r="E22" s="41"/>
       <c r="F22" s="18" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="G22" s="18" t="s">
         <v>21</v>
@@ -7132,7 +7441,7 @@
       <c r="D23" s="32"/>
       <c r="E23" s="41"/>
       <c r="F23" s="18" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="G23" s="18" t="s">
         <v>21</v>
@@ -7158,7 +7467,7 @@
       <c r="D24" s="32"/>
       <c r="E24" s="41"/>
       <c r="F24" s="18" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="G24" s="18" t="s">
         <v>21</v>
@@ -7184,7 +7493,7 @@
       <c r="D25" s="32"/>
       <c r="E25" s="41"/>
       <c r="F25" s="18" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="G25" s="18" t="s">
         <v>15</v>
@@ -7210,7 +7519,7 @@
       <c r="D26" s="32"/>
       <c r="E26" s="41"/>
       <c r="F26" s="18" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="G26" s="18" t="s">
         <v>21</v>
@@ -7236,7 +7545,7 @@
       <c r="D27" s="32"/>
       <c r="E27" s="44"/>
       <c r="F27" s="20" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="G27" s="20" t="s">
         <v>21</v>
@@ -7262,7 +7571,7 @@
       <c r="D28" s="32"/>
       <c r="E28" s="44"/>
       <c r="F28" s="20" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="G28" s="20" t="s">
         <v>21</v>
@@ -7288,7 +7597,7 @@
       <c r="D29" s="32"/>
       <c r="E29" s="44"/>
       <c r="F29" s="20" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="G29" s="20" t="s">
         <v>28</v>
@@ -7314,7 +7623,7 @@
       <c r="D30" s="32"/>
       <c r="E30" s="44"/>
       <c r="F30" s="20" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="G30" s="20" t="s">
         <v>21</v>
@@ -7340,7 +7649,7 @@
       <c r="D31" s="32"/>
       <c r="E31" s="44"/>
       <c r="F31" s="20" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="G31" s="20" t="s">
         <v>33</v>
@@ -7366,7 +7675,7 @@
       <c r="D32" s="32"/>
       <c r="E32" s="44"/>
       <c r="F32" s="20" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="G32" s="20" t="s">
         <v>8</v>
@@ -7392,7 +7701,7 @@
       <c r="D33" s="32"/>
       <c r="E33" s="44"/>
       <c r="F33" s="20" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G33" s="20" t="s">
         <v>8</v>
@@ -7418,7 +7727,7 @@
       <c r="D34" s="32"/>
       <c r="E34" s="44"/>
       <c r="F34" s="20" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="G34" s="20" t="s">
         <v>5</v>
@@ -7470,7 +7779,7 @@
       <c r="D36" s="32"/>
       <c r="E36" s="44"/>
       <c r="F36" s="20" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
       <c r="G36" s="20" t="s">
         <v>6</v>
@@ -7496,7 +7805,7 @@
       <c r="D37" s="32"/>
       <c r="E37" s="44"/>
       <c r="F37" s="20" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="G37" s="20" t="s">
         <v>5</v>
@@ -7522,7 +7831,7 @@
       <c r="D38" s="32"/>
       <c r="E38" s="44"/>
       <c r="F38" s="20" t="s">
-        <v>514</v>
+        <v>507</v>
       </c>
       <c r="G38" s="20" t="s">
         <v>15</v>
@@ -7548,7 +7857,7 @@
       <c r="D39" s="32"/>
       <c r="E39" s="44"/>
       <c r="F39" s="20" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
       <c r="G39" s="20" t="s">
         <v>23</v>
@@ -7574,7 +7883,7 @@
       <c r="D40" s="32"/>
       <c r="E40" s="44"/>
       <c r="F40" s="20" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
       <c r="G40" s="20" t="s">
         <v>149</v>
@@ -7600,7 +7909,7 @@
       <c r="D41" s="32"/>
       <c r="E41" s="44"/>
       <c r="F41" s="20" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="G41" s="20" t="s">
         <v>8</v>
@@ -7626,7 +7935,7 @@
       <c r="D42" s="32"/>
       <c r="E42" s="44"/>
       <c r="F42" s="20" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="G42" s="20" t="s">
         <v>5</v>
@@ -7652,7 +7961,7 @@
       <c r="D43" s="32"/>
       <c r="E43" s="44"/>
       <c r="F43" s="20" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G43" s="20" t="s">
         <v>5</v>
@@ -7678,7 +7987,7 @@
       <c r="D44" s="32"/>
       <c r="E44" s="44"/>
       <c r="F44" s="20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G44" s="20" t="s">
         <v>5</v>
@@ -7704,7 +8013,7 @@
       <c r="D45" s="32"/>
       <c r="E45" s="44"/>
       <c r="F45" s="20" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="G45" s="20" t="s">
         <v>28</v>
@@ -7730,7 +8039,7 @@
       <c r="D46" s="32"/>
       <c r="E46" s="44"/>
       <c r="F46" s="20" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="G46" s="20" t="s">
         <v>28</v>
@@ -7756,7 +8065,7 @@
       <c r="D47" s="32"/>
       <c r="E47" s="44"/>
       <c r="F47" s="20" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="G47" s="20" t="s">
         <v>139</v>
@@ -7782,7 +8091,7 @@
       <c r="D48" s="32"/>
       <c r="E48" s="44"/>
       <c r="F48" s="20" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="G48" s="20" t="s">
         <v>6</v>
@@ -7808,7 +8117,7 @@
       <c r="D49" s="32"/>
       <c r="E49" s="44"/>
       <c r="F49" s="20" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
       <c r="G49" s="20" t="s">
         <v>20</v>
@@ -7834,7 +8143,7 @@
       <c r="D50" s="32"/>
       <c r="E50" s="44"/>
       <c r="F50" s="20" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
       <c r="G50" s="20" t="s">
         <v>8</v>
@@ -7860,7 +8169,7 @@
       <c r="D51" s="32"/>
       <c r="E51" s="44"/>
       <c r="F51" s="20" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="G51" s="20" t="s">
         <v>6</v>
@@ -7886,7 +8195,7 @@
       <c r="D52" s="32"/>
       <c r="E52" s="44"/>
       <c r="F52" s="20" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
       <c r="G52" s="20" t="s">
         <v>21</v>
@@ -7912,7 +8221,7 @@
       <c r="D53" s="32"/>
       <c r="E53" s="44"/>
       <c r="F53" s="20" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
       <c r="G53" s="20" t="s">
         <v>6</v>
@@ -7938,7 +8247,7 @@
       <c r="D54" s="32"/>
       <c r="E54" s="44"/>
       <c r="F54" s="20" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="G54" s="20" t="s">
         <v>8</v>
@@ -7964,7 +8273,7 @@
       <c r="D55" s="32"/>
       <c r="E55" s="44"/>
       <c r="F55" s="20" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="G55" s="20" t="s">
         <v>8</v>
@@ -7990,7 +8299,7 @@
       <c r="D56" s="32"/>
       <c r="E56" s="47"/>
       <c r="F56" s="48" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="G56" s="48" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Update January 2025 tab with new fact table and album_family logic
</commit_message>
<xml_diff>
--- a/excel/spotify_listening_report_2025.xlsx
+++ b/excel/spotify_listening_report_2025.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermitchell/Documents/projects/projects_2025/analytics_projects/Spotify_Sandbox/spotify_sandbox_github/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6710701E-E459-BD43-81A1-DEE24F198F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA13D437-E8A0-5944-854A-913950C14ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="-1960" windowWidth="38400" windowHeight="21600" xr2:uid="{02962024-D185-E646-89C4-A67A4B8F8E62}"/>
+    <workbookView xWindow="30240" yWindow="-1960" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{02962024-D185-E646-89C4-A67A4B8F8E62}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Overview" sheetId="13" r:id="rId1"/>
-    <sheet name="Jan" sheetId="14" r:id="rId2"/>
+    <sheet name="Jan" sheetId="15" r:id="rId2"/>
     <sheet name="Feb" sheetId="5" r:id="rId3"/>
     <sheet name="Mar" sheetId="6" r:id="rId4"/>
     <sheet name="Apr" sheetId="7" r:id="rId5"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1232" uniqueCount="547">
   <si>
     <t>Based on Spotify Extended Streaming History Time Listened (Music Only)</t>
   </si>
@@ -1623,15 +1623,79 @@
   </si>
   <si>
     <t>Bitte Orca</t>
+  </si>
+  <si>
+    <t>High As Hope</t>
+  </si>
+  <si>
+    <t>Girls Can Tell</t>
+  </si>
+  <si>
+    <t>Free Yourself Up</t>
+  </si>
+  <si>
+    <t>Parachutes</t>
+  </si>
+  <si>
+    <t>Fun Machine EP</t>
+  </si>
+  <si>
+    <t>Bad Self Portraits</t>
+  </si>
+  <si>
+    <t>Around the Well</t>
+  </si>
+  <si>
+    <t>Charli</t>
+  </si>
+  <si>
+    <t>A Blessing and a Curse</t>
+  </si>
+  <si>
+    <t>Obviously</t>
+  </si>
+  <si>
+    <t>Hatful of Hollow</t>
+  </si>
+  <si>
+    <t>Doolittle</t>
+  </si>
+  <si>
+    <t>For Emma, Forever Ago</t>
+  </si>
+  <si>
+    <t>Fear Of The Dawn</t>
+  </si>
+  <si>
+    <t>Decoration Day</t>
+  </si>
+  <si>
+    <t>Beautiful Strangers b/w No Place to Fall</t>
+  </si>
+  <si>
+    <t>Tourist History</t>
+  </si>
+  <si>
+    <t>Different Class</t>
+  </si>
+  <si>
+    <t>Shaming Of The Sun</t>
+  </si>
+  <si>
+    <t>Pageant Material</t>
+  </si>
+  <si>
+    <t>Blowin' Your Mind!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0_);\(#,##0.0\)"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -2026,18 +2090,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2377,10 +2441,10 @@
   </sheetPr>
   <dimension ref="A1:P106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G32" sqref="G32"/>
-      <selection pane="bottomLeft" activeCell="N12" sqref="N12"/>
+      <selection pane="bottomLeft" activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2540,7 +2604,7 @@
       <c r="G7" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="65">
+      <c r="H7" s="59">
         <v>162.39576666666667</v>
       </c>
       <c r="I7" s="32"/>
@@ -2577,7 +2641,7 @@
       <c r="G8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="66">
+      <c r="H8" s="60">
         <v>136.98431666666667</v>
       </c>
       <c r="I8" s="32"/>
@@ -2614,7 +2678,7 @@
       <c r="G9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="66">
+      <c r="H9" s="60">
         <v>129.39758333333333</v>
       </c>
       <c r="I9" s="32"/>
@@ -2651,7 +2715,7 @@
       <c r="G10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="66">
+      <c r="H10" s="60">
         <v>120.67485000000001</v>
       </c>
       <c r="I10" s="32"/>
@@ -2688,7 +2752,7 @@
       <c r="G11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="66">
+      <c r="H11" s="60">
         <v>116.45350000000001</v>
       </c>
       <c r="I11" s="32"/>
@@ -2726,7 +2790,7 @@
       <c r="G12" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="67">
+      <c r="H12" s="61">
         <v>110.51224999999999</v>
       </c>
       <c r="I12" s="32"/>
@@ -2763,7 +2827,7 @@
       <c r="G13" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="67">
+      <c r="H13" s="61">
         <v>110.18210000000001</v>
       </c>
       <c r="I13" s="32"/>
@@ -2800,7 +2864,7 @@
       <c r="G14" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="67">
+      <c r="H14" s="61">
         <v>88.796733333333336</v>
       </c>
       <c r="I14" s="32"/>
@@ -2837,7 +2901,7 @@
       <c r="G15" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="67">
+      <c r="H15" s="61">
         <v>87.560916666666671</v>
       </c>
       <c r="I15" s="32"/>
@@ -2874,7 +2938,7 @@
       <c r="G16" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="67">
+      <c r="H16" s="61">
         <v>78.673066666666671</v>
       </c>
       <c r="I16" s="32"/>
@@ -2911,7 +2975,7 @@
       <c r="G17" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="H17" s="68">
+      <c r="H17" s="62">
         <v>75.114450000000005</v>
       </c>
       <c r="I17" s="32"/>
@@ -2948,7 +3012,7 @@
       <c r="G18" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="68">
+      <c r="H18" s="62">
         <v>75.044650000000004</v>
       </c>
       <c r="I18" s="32"/>
@@ -2985,7 +3049,7 @@
       <c r="G19" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H19" s="68">
+      <c r="H19" s="62">
         <v>73.818983333333335</v>
       </c>
       <c r="I19" s="32"/>
@@ -3022,7 +3086,7 @@
       <c r="G20" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="H20" s="68">
+      <c r="H20" s="62">
         <v>70.979200000000006</v>
       </c>
       <c r="I20" s="32"/>
@@ -3059,7 +3123,7 @@
       <c r="G21" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H21" s="68">
+      <c r="H21" s="62">
         <v>69.502650000000003</v>
       </c>
       <c r="I21" s="32"/>
@@ -3096,7 +3160,7 @@
       <c r="G22" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="68">
+      <c r="H22" s="62">
         <v>69.15176666666666</v>
       </c>
       <c r="I22" s="32"/>
@@ -3133,7 +3197,7 @@
       <c r="G23" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H23" s="68">
+      <c r="H23" s="62">
         <v>68.841333333333338</v>
       </c>
       <c r="I23" s="32"/>
@@ -3170,7 +3234,7 @@
       <c r="G24" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H24" s="68">
+      <c r="H24" s="62">
         <v>68.576466666666661</v>
       </c>
       <c r="I24" s="32"/>
@@ -3207,7 +3271,7 @@
       <c r="G25" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H25" s="68">
+      <c r="H25" s="62">
         <v>66.407483333333332</v>
       </c>
       <c r="I25" s="32"/>
@@ -3244,7 +3308,7 @@
       <c r="G26" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H26" s="68">
+      <c r="H26" s="62">
         <v>65.699233333333339</v>
       </c>
       <c r="I26" s="32"/>
@@ -3281,7 +3345,7 @@
       <c r="G27" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="H27" s="69">
+      <c r="H27" s="63">
         <v>65.456116666666674</v>
       </c>
       <c r="I27" s="32"/>
@@ -3318,7 +3382,7 @@
       <c r="G28" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H28" s="69">
+      <c r="H28" s="63">
         <v>64.26421666666667</v>
       </c>
       <c r="I28" s="32"/>
@@ -3355,7 +3419,7 @@
       <c r="G29" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H29" s="69">
+      <c r="H29" s="63">
         <v>59.984716666666664</v>
       </c>
       <c r="I29" s="32"/>
@@ -3392,7 +3456,7 @@
       <c r="G30" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H30" s="69">
+      <c r="H30" s="63">
         <v>59.591999999999999</v>
       </c>
       <c r="I30" s="32"/>
@@ -3429,7 +3493,7 @@
       <c r="G31" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H31" s="69">
+      <c r="H31" s="63">
         <v>59.25685</v>
       </c>
       <c r="I31" s="32"/>
@@ -3466,7 +3530,7 @@
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H32" s="69">
+      <c r="H32" s="63">
         <v>58.996716666666664</v>
       </c>
       <c r="I32" s="32"/>
@@ -3503,7 +3567,7 @@
       <c r="G33" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H33" s="69">
+      <c r="H33" s="63">
         <v>58.030183333333333</v>
       </c>
       <c r="I33" s="32"/>
@@ -3540,7 +3604,7 @@
       <c r="G34" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H34" s="69">
+      <c r="H34" s="63">
         <v>56.381383333333332</v>
       </c>
       <c r="I34" s="32"/>
@@ -3577,7 +3641,7 @@
       <c r="G35" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H35" s="69">
+      <c r="H35" s="63">
         <v>56.032516666666666</v>
       </c>
       <c r="I35" s="32"/>
@@ -3614,7 +3678,7 @@
       <c r="G36" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="H36" s="69">
+      <c r="H36" s="63">
         <v>55.678566666666669</v>
       </c>
       <c r="I36" s="32"/>
@@ -3651,7 +3715,7 @@
       <c r="G37" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="H37" s="69">
+      <c r="H37" s="63">
         <v>55.64071666666667</v>
       </c>
       <c r="I37" s="32"/>
@@ -3688,7 +3752,7 @@
       <c r="G38" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H38" s="69">
+      <c r="H38" s="63">
         <v>54.588016666666668</v>
       </c>
       <c r="I38" s="32"/>
@@ -3725,7 +3789,7 @@
       <c r="G39" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H39" s="69">
+      <c r="H39" s="63">
         <v>53.564533333333337</v>
       </c>
       <c r="I39" s="32"/>
@@ -3762,7 +3826,7 @@
       <c r="G40" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H40" s="69">
+      <c r="H40" s="63">
         <v>50.267383333333335</v>
       </c>
       <c r="I40" s="32"/>
@@ -3799,7 +3863,7 @@
       <c r="G41" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H41" s="69">
+      <c r="H41" s="63">
         <v>50.252816666666668</v>
       </c>
       <c r="I41" s="32"/>
@@ -3836,7 +3900,7 @@
       <c r="G42" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H42" s="69">
+      <c r="H42" s="63">
         <v>49.837466666666664</v>
       </c>
       <c r="I42" s="32"/>
@@ -3873,7 +3937,7 @@
       <c r="G43" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H43" s="69">
+      <c r="H43" s="63">
         <v>49.572749999999999</v>
       </c>
       <c r="I43" s="32"/>
@@ -3910,7 +3974,7 @@
       <c r="G44" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H44" s="69">
+      <c r="H44" s="63">
         <v>49.404616666666669</v>
       </c>
       <c r="I44" s="32"/>
@@ -3947,7 +4011,7 @@
       <c r="G45" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H45" s="69">
+      <c r="H45" s="63">
         <v>49.314399999999999</v>
       </c>
       <c r="I45" s="32"/>
@@ -3984,7 +4048,7 @@
       <c r="G46" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="H46" s="69">
+      <c r="H46" s="63">
         <v>49.160766666666667</v>
       </c>
       <c r="I46" s="32"/>
@@ -4021,7 +4085,7 @@
       <c r="G47" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="H47" s="69">
+      <c r="H47" s="63">
         <v>48.411149999999999</v>
       </c>
       <c r="I47" s="32"/>
@@ -4058,7 +4122,7 @@
       <c r="G48" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H48" s="69">
+      <c r="H48" s="63">
         <v>47.83155</v>
       </c>
       <c r="I48" s="32"/>
@@ -4095,7 +4159,7 @@
       <c r="G49" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="H49" s="69">
+      <c r="H49" s="63">
         <v>47.251466666666666</v>
       </c>
       <c r="I49" s="32"/>
@@ -4132,7 +4196,7 @@
       <c r="G50" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H50" s="69">
+      <c r="H50" s="63">
         <v>46.779366666666668</v>
       </c>
       <c r="I50" s="32"/>
@@ -4169,7 +4233,7 @@
       <c r="G51" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H51" s="69">
+      <c r="H51" s="63">
         <v>46.714550000000003</v>
       </c>
       <c r="I51" s="32"/>
@@ -4206,7 +4270,7 @@
       <c r="G52" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="H52" s="69">
+      <c r="H52" s="63">
         <v>45.705716666666667</v>
       </c>
       <c r="I52" s="32"/>
@@ -4243,7 +4307,7 @@
       <c r="G53" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H53" s="69">
+      <c r="H53" s="63">
         <v>45.406366666666663</v>
       </c>
       <c r="I53" s="32"/>
@@ -4280,7 +4344,7 @@
       <c r="G54" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="H54" s="69">
+      <c r="H54" s="63">
         <v>45.267933333333332</v>
       </c>
       <c r="I54" s="32"/>
@@ -4317,7 +4381,7 @@
       <c r="G55" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="H55" s="69">
+      <c r="H55" s="63">
         <v>44.662799999999997</v>
       </c>
       <c r="I55" s="32"/>
@@ -4354,7 +4418,7 @@
       <c r="G56" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H56" s="69">
+      <c r="H56" s="63">
         <v>44.518883333333335</v>
       </c>
       <c r="I56" s="32"/>
@@ -4391,7 +4455,7 @@
       <c r="G57" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H57" s="69">
+      <c r="H57" s="63">
         <v>44.077500000000001</v>
       </c>
       <c r="I57" s="32"/>
@@ -4428,7 +4492,7 @@
       <c r="G58" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="H58" s="69">
+      <c r="H58" s="63">
         <v>43.632866666666665</v>
       </c>
       <c r="I58" s="32"/>
@@ -4465,7 +4529,7 @@
       <c r="G59" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H59" s="69">
+      <c r="H59" s="63">
         <v>43.256316666666663</v>
       </c>
       <c r="I59" s="32"/>
@@ -4502,7 +4566,7 @@
       <c r="G60" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H60" s="69">
+      <c r="H60" s="63">
         <v>43.077449999999999</v>
       </c>
       <c r="I60" s="32"/>
@@ -4539,7 +4603,7 @@
       <c r="G61" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H61" s="69">
+      <c r="H61" s="63">
         <v>42.818533333333335</v>
       </c>
       <c r="I61" s="32"/>
@@ -4576,7 +4640,7 @@
       <c r="G62" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H62" s="69">
+      <c r="H62" s="63">
         <v>42.366599999999998</v>
       </c>
       <c r="I62" s="32"/>
@@ -4613,7 +4677,7 @@
       <c r="G63" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H63" s="69">
+      <c r="H63" s="63">
         <v>41.546383333333331</v>
       </c>
       <c r="I63" s="32"/>
@@ -4650,7 +4714,7 @@
       <c r="G64" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H64" s="69">
+      <c r="H64" s="63">
         <v>41.501300000000001</v>
       </c>
       <c r="I64" s="32"/>
@@ -4687,7 +4751,7 @@
       <c r="G65" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="H65" s="69">
+      <c r="H65" s="63">
         <v>41.40956666666667</v>
       </c>
       <c r="I65" s="32"/>
@@ -4724,7 +4788,7 @@
       <c r="G66" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H66" s="69">
+      <c r="H66" s="63">
         <v>41.383383333333335</v>
       </c>
       <c r="I66" s="32"/>
@@ -4761,7 +4825,7 @@
       <c r="G67" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H67" s="69">
+      <c r="H67" s="63">
         <v>41.209083333333332</v>
       </c>
       <c r="I67" s="32"/>
@@ -4798,7 +4862,7 @@
       <c r="G68" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H68" s="69">
+      <c r="H68" s="63">
         <v>40.812216666666664</v>
       </c>
       <c r="I68" s="32"/>
@@ -4835,7 +4899,7 @@
       <c r="G69" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H69" s="69">
+      <c r="H69" s="63">
         <v>40.622900000000001</v>
       </c>
       <c r="I69" s="32"/>
@@ -4872,7 +4936,7 @@
       <c r="G70" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="H70" s="69">
+      <c r="H70" s="63">
         <v>40.272616666666664</v>
       </c>
       <c r="I70" s="32"/>
@@ -4909,7 +4973,7 @@
       <c r="G71" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H71" s="69">
+      <c r="H71" s="63">
         <v>40.190216666666664</v>
       </c>
       <c r="I71" s="32"/>
@@ -4946,7 +5010,7 @@
       <c r="G72" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="H72" s="69">
+      <c r="H72" s="63">
         <v>39.674883333333334</v>
       </c>
       <c r="I72" s="32"/>
@@ -4983,7 +5047,7 @@
       <c r="G73" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="H73" s="69">
+      <c r="H73" s="63">
         <v>39.643000000000001</v>
       </c>
       <c r="I73" s="32"/>
@@ -5020,7 +5084,7 @@
       <c r="G74" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H74" s="69">
+      <c r="H74" s="63">
         <v>39.427933333333335</v>
       </c>
       <c r="I74" s="32"/>
@@ -5057,7 +5121,7 @@
       <c r="G75" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H75" s="69">
+      <c r="H75" s="63">
         <v>39.401633333333336</v>
       </c>
       <c r="I75" s="32"/>
@@ -5094,7 +5158,7 @@
       <c r="G76" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H76" s="69">
+      <c r="H76" s="63">
         <v>39.323016666666668</v>
       </c>
       <c r="I76" s="32"/>
@@ -5131,7 +5195,7 @@
       <c r="G77" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H77" s="69">
+      <c r="H77" s="63">
         <v>39.18013333333333</v>
       </c>
       <c r="I77" s="32"/>
@@ -5168,7 +5232,7 @@
       <c r="G78" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="H78" s="69">
+      <c r="H78" s="63">
         <v>39.129800000000003</v>
       </c>
       <c r="I78" s="32"/>
@@ -5205,7 +5269,7 @@
       <c r="G79" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="H79" s="69">
+      <c r="H79" s="63">
         <v>39.037999999999997</v>
       </c>
       <c r="I79" s="32"/>
@@ -5242,7 +5306,7 @@
       <c r="G80" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H80" s="69">
+      <c r="H80" s="63">
         <v>38.56335</v>
       </c>
       <c r="I80" s="32"/>
@@ -5279,7 +5343,7 @@
       <c r="G81" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H81" s="69">
+      <c r="H81" s="63">
         <v>38.457383333333333</v>
       </c>
       <c r="I81" s="32"/>
@@ -5316,7 +5380,7 @@
       <c r="G82" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H82" s="69">
+      <c r="H82" s="63">
         <v>38.339849999999998</v>
       </c>
       <c r="I82" s="32"/>
@@ -5353,7 +5417,7 @@
       <c r="G83" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H83" s="69">
+      <c r="H83" s="63">
         <v>37.623316666666668</v>
       </c>
       <c r="I83" s="32"/>
@@ -5390,7 +5454,7 @@
       <c r="G84" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H84" s="69">
+      <c r="H84" s="63">
         <v>37.274333333333331</v>
       </c>
       <c r="I84" s="32"/>
@@ -5427,7 +5491,7 @@
       <c r="G85" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="H85" s="69">
+      <c r="H85" s="63">
         <v>36.484450000000002</v>
       </c>
       <c r="I85" s="32"/>
@@ -5464,7 +5528,7 @@
       <c r="G86" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="H86" s="69">
+      <c r="H86" s="63">
         <v>36.31668333333333</v>
       </c>
       <c r="I86" s="32"/>
@@ -5501,7 +5565,7 @@
       <c r="G87" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="H87" s="69">
+      <c r="H87" s="63">
         <v>36.028083333333335</v>
       </c>
       <c r="I87" s="32"/>
@@ -5538,7 +5602,7 @@
       <c r="G88" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="H88" s="69">
+      <c r="H88" s="63">
         <v>35.577716666666667</v>
       </c>
       <c r="I88" s="32"/>
@@ -5575,7 +5639,7 @@
       <c r="G89" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H89" s="69">
+      <c r="H89" s="63">
         <v>35.176349999999999</v>
       </c>
       <c r="I89" s="32"/>
@@ -5612,7 +5676,7 @@
       <c r="G90" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="H90" s="69">
+      <c r="H90" s="63">
         <v>34.761066666666665</v>
       </c>
       <c r="I90" s="32"/>
@@ -5649,7 +5713,7 @@
       <c r="G91" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H91" s="69">
+      <c r="H91" s="63">
         <v>34.72358333333333</v>
       </c>
       <c r="I91" s="32"/>
@@ -5686,7 +5750,7 @@
       <c r="G92" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H92" s="69">
+      <c r="H92" s="63">
         <v>34.623416666666664</v>
       </c>
       <c r="I92" s="32"/>
@@ -5723,7 +5787,7 @@
       <c r="G93" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H93" s="69">
+      <c r="H93" s="63">
         <v>34.598750000000003</v>
       </c>
       <c r="I93" s="32"/>
@@ -5760,7 +5824,7 @@
       <c r="G94" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H94" s="69">
+      <c r="H94" s="63">
         <v>33.880800000000001</v>
       </c>
       <c r="I94" s="32"/>
@@ -5797,7 +5861,7 @@
       <c r="G95" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H95" s="69">
+      <c r="H95" s="63">
         <v>33.819200000000002</v>
       </c>
       <c r="I95" s="32"/>
@@ -5834,7 +5898,7 @@
       <c r="G96" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="H96" s="69">
+      <c r="H96" s="63">
         <v>33.569516666666665</v>
       </c>
       <c r="I96" s="32"/>
@@ -5871,7 +5935,7 @@
       <c r="G97" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H97" s="69">
+      <c r="H97" s="63">
         <v>33.413649999999997</v>
       </c>
       <c r="I97" s="32"/>
@@ -5908,7 +5972,7 @@
       <c r="G98" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H98" s="69">
+      <c r="H98" s="63">
         <v>33.342483333333334</v>
       </c>
       <c r="I98" s="32"/>
@@ -5945,7 +6009,7 @@
       <c r="G99" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="H99" s="69">
+      <c r="H99" s="63">
         <v>33.120533333333334</v>
       </c>
       <c r="I99" s="32"/>
@@ -5982,7 +6046,7 @@
       <c r="G100" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="H100" s="69">
+      <c r="H100" s="63">
         <v>32.58271666666667</v>
       </c>
       <c r="I100" s="32"/>
@@ -6019,7 +6083,7 @@
       <c r="G101" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="H101" s="69">
+      <c r="H101" s="63">
         <v>32.281649999999999</v>
       </c>
       <c r="I101" s="32"/>
@@ -6056,7 +6120,7 @@
       <c r="G102" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H102" s="69">
+      <c r="H102" s="63">
         <v>31.991783333333334</v>
       </c>
       <c r="I102" s="32"/>
@@ -6093,7 +6157,7 @@
       <c r="G103" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H103" s="69">
+      <c r="H103" s="63">
         <v>31.932583333333334</v>
       </c>
       <c r="I103" s="32"/>
@@ -6130,7 +6194,7 @@
       <c r="G104" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H104" s="69">
+      <c r="H104" s="63">
         <v>31.926766666666666</v>
       </c>
       <c r="I104" s="32"/>
@@ -6167,7 +6231,7 @@
       <c r="G105" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H105" s="69">
+      <c r="H105" s="63">
         <v>31.685449999999999</v>
       </c>
       <c r="I105" s="32"/>
@@ -6204,7 +6268,7 @@
       <c r="G106" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="H106" s="70">
+      <c r="H106" s="64">
         <v>31.426950000000001</v>
       </c>
       <c r="I106" s="32"/>
@@ -6871,16 +6935,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1083F66-8061-A042-91CB-6DF0947502D8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9671E084-5161-CD4C-8686-5F1F5087756F}">
   <sheetPr>
     <tabColor rgb="FFCFC7FF"/>
   </sheetPr>
-  <dimension ref="A1:O56"/>
+  <dimension ref="A1:P56"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G32" sqref="G32"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomLeft" activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6890,16 +6954,17 @@
     <col min="3" max="3" width="13.83203125" customWidth="1"/>
     <col min="4" max="4" width="3" customWidth="1"/>
     <col min="5" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.1640625" customWidth="1"/>
+    <col min="6" max="6" width="45.5" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" customWidth="1"/>
     <col min="8" max="8" width="13.83203125" style="51" customWidth="1"/>
     <col min="9" max="9" width="3" customWidth="1"/>
     <col min="10" max="10" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="51.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" style="51" customWidth="1"/>
+    <col min="11" max="11" width="36.83203125" customWidth="1"/>
+    <col min="12" max="12" width="26.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" style="51" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="22" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="22" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="52" t="s">
         <v>483</v>
       </c>
@@ -6914,8 +6979,9 @@
       <c r="J1" s="52"/>
       <c r="K1" s="52"/>
       <c r="L1" s="52"/>
-    </row>
-    <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M1" s="52"/>
+    </row>
+    <row r="2" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="53" t="s">
         <v>484</v>
       </c>
@@ -6930,8 +6996,9 @@
       <c r="J2" s="53"/>
       <c r="K2" s="53"/>
       <c r="L2" s="53"/>
-    </row>
-    <row r="3" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M2" s="53"/>
+    </row>
+    <row r="3" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="54" t="s">
         <v>485</v>
       </c>
@@ -6946,8 +7013,9 @@
       <c r="J3" s="54"/>
       <c r="K3" s="54"/>
       <c r="L3" s="54"/>
-    </row>
-    <row r="4" spans="1:15" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M3" s="54"/>
+    </row>
+    <row r="4" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="22"/>
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
@@ -6959,9 +7027,10 @@
       <c r="I4" s="23"/>
       <c r="J4" s="23"/>
       <c r="K4" s="23"/>
-      <c r="L4" s="24"/>
-    </row>
-    <row r="5" spans="1:15" s="25" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L4" s="23"/>
+      <c r="M4" s="24"/>
+    </row>
+    <row r="5" spans="1:16" s="25" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="55" t="s">
         <v>196</v>
       </c>
@@ -6978,8 +7047,9 @@
       </c>
       <c r="K5" s="55"/>
       <c r="L5" s="55"/>
-    </row>
-    <row r="6" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M5" s="55"/>
+    </row>
+    <row r="6" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
         <v>2</v>
       </c>
@@ -7007,1319 +7077,1872 @@
       <c r="K6" s="4" t="s">
         <v>482</v>
       </c>
-      <c r="L6" s="28" t="s">
+      <c r="L6" s="4" t="s">
+        <v>486</v>
+      </c>
+      <c r="M6" s="28" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="29">
         <v>1</v>
       </c>
       <c r="B7" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="65">
         <v>264.58941666666669</v>
       </c>
       <c r="D7" s="32"/>
-      <c r="E7" s="29"/>
+      <c r="E7" s="29">
+        <v>1</v>
+      </c>
       <c r="F7" s="30" t="s">
         <v>324</v>
       </c>
       <c r="G7" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="59">
+      <c r="H7" s="65">
         <v>38.733516666666667</v>
       </c>
       <c r="I7" s="32"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="33"/>
-    </row>
-    <row r="8" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J7" s="29">
+        <v>1</v>
+      </c>
+      <c r="K7" s="30" t="s">
+        <v>302</v>
+      </c>
+      <c r="L7" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" s="65">
+        <v>137.36678333333333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="34">
         <v>2</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="66">
         <v>241.06870000000001</v>
       </c>
       <c r="D8" s="32"/>
-      <c r="E8" s="34"/>
+      <c r="E8" s="34">
+        <v>2</v>
+      </c>
       <c r="F8" s="10" t="s">
         <v>303</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="60">
+      <c r="H8" s="66">
         <v>28.061016666666667</v>
       </c>
       <c r="I8" s="32"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="36"/>
-    </row>
-    <row r="9" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J8" s="34">
+        <v>2</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="66">
+        <v>132.31635</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="34">
         <v>3</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="35">
+      <c r="C9" s="66">
         <v>233.69826666666665</v>
       </c>
       <c r="D9" s="32"/>
-      <c r="E9" s="34"/>
+      <c r="E9" s="34">
+        <v>3</v>
+      </c>
       <c r="F9" s="10" t="s">
         <v>388</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="60">
+      <c r="H9" s="66">
         <v>22.323450000000001</v>
       </c>
       <c r="I9" s="32"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="36"/>
-    </row>
-    <row r="10" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J9" s="34">
+        <v>3</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" s="66">
+        <v>123.38823333333333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="34">
         <v>4</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10" s="66">
         <v>135.68235000000001</v>
       </c>
       <c r="D10" s="32"/>
-      <c r="E10" s="34"/>
+      <c r="E10" s="34">
+        <v>4</v>
+      </c>
       <c r="F10" s="10" t="s">
         <v>380</v>
       </c>
       <c r="G10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="60">
+      <c r="H10" s="66">
         <v>19.705983333333332</v>
       </c>
       <c r="I10" s="32"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="36"/>
-    </row>
-    <row r="11" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J10" s="34">
+        <v>4</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="M10" s="66">
+        <v>120.21013333333333</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="34">
         <v>5</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="66">
         <v>130.97198333333333</v>
       </c>
       <c r="D11" s="32"/>
-      <c r="E11" s="34"/>
+      <c r="E11" s="34">
+        <v>5</v>
+      </c>
       <c r="F11" s="10" t="s">
         <v>309</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="60">
+      <c r="H11" s="66">
         <v>18.794383333333332</v>
       </c>
       <c r="I11" s="32"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="36"/>
-      <c r="O11" s="37"/>
-    </row>
-    <row r="12" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J11" s="34">
+        <v>5</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="M11" s="66">
+        <v>105.75096666666667</v>
+      </c>
+      <c r="P11" s="37"/>
+    </row>
+    <row r="12" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="38">
         <v>6</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="39">
+      <c r="C12" s="67">
         <v>127.02421666666666</v>
       </c>
       <c r="D12" s="32"/>
-      <c r="E12" s="38"/>
+      <c r="E12" s="38">
+        <v>6</v>
+      </c>
       <c r="F12" s="16" t="s">
         <v>487</v>
       </c>
       <c r="G12" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="61">
+      <c r="H12" s="67">
         <v>18.564133333333334</v>
       </c>
       <c r="I12" s="32"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="40"/>
-    </row>
-    <row r="13" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J12" s="38">
+        <v>6</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="L12" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12" s="67">
+        <v>103.40856666666667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="38">
         <v>7</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="39">
+      <c r="C13" s="67">
         <v>81.623166666666663</v>
       </c>
       <c r="D13" s="32"/>
-      <c r="E13" s="38"/>
+      <c r="E13" s="38">
+        <v>7</v>
+      </c>
       <c r="F13" s="16" t="s">
         <v>327</v>
       </c>
       <c r="G13" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="61">
+      <c r="H13" s="67">
         <v>17.858699999999999</v>
       </c>
       <c r="I13" s="32"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="40"/>
-    </row>
-    <row r="14" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J13" s="38">
+        <v>7</v>
+      </c>
+      <c r="K13" s="16" t="s">
+        <v>373</v>
+      </c>
+      <c r="L13" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M13" s="67">
+        <v>83.152850000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="38">
         <v>8</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="39">
+      <c r="C14" s="67">
         <v>57.57586666666667</v>
       </c>
       <c r="D14" s="32"/>
-      <c r="E14" s="38"/>
+      <c r="E14" s="38">
+        <v>8</v>
+      </c>
       <c r="F14" s="16" t="s">
         <v>488</v>
       </c>
       <c r="G14" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="61">
+      <c r="H14" s="67">
         <v>17.284216666666666</v>
       </c>
       <c r="I14" s="32"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="40"/>
-    </row>
-    <row r="15" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J14" s="38">
+        <v>8</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>387</v>
+      </c>
+      <c r="L14" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="M14" s="67">
+        <v>80.058083333333329</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="38">
         <v>9</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="39">
+      <c r="C15" s="67">
         <v>55.518266666666669</v>
       </c>
       <c r="D15" s="32"/>
-      <c r="E15" s="38"/>
+      <c r="E15" s="38">
+        <v>9</v>
+      </c>
       <c r="F15" s="16" t="s">
         <v>489</v>
       </c>
       <c r="G15" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H15" s="61">
+      <c r="H15" s="67">
         <v>16.679966666666665</v>
       </c>
       <c r="I15" s="32"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="40"/>
-    </row>
-    <row r="16" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J15" s="38">
+        <v>9</v>
+      </c>
+      <c r="K15" s="16" t="s">
+        <v>415</v>
+      </c>
+      <c r="L15" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="M15" s="67">
+        <v>61.559150000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="38">
         <v>10</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="39">
+      <c r="C16" s="67">
         <v>48.295400000000001</v>
       </c>
       <c r="D16" s="32"/>
-      <c r="E16" s="38"/>
+      <c r="E16" s="38">
+        <v>10</v>
+      </c>
       <c r="F16" s="16" t="s">
         <v>490</v>
       </c>
       <c r="G16" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="61">
+      <c r="H16" s="67">
         <v>14.8217</v>
       </c>
       <c r="I16" s="32"/>
-      <c r="J16" s="38"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="40"/>
-    </row>
-    <row r="17" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J16" s="38">
+        <v>10</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>385</v>
+      </c>
+      <c r="L16" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="M16" s="67">
+        <v>57.57586666666667</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="41">
         <v>11</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="42">
+      <c r="C17" s="68">
         <v>44.400783333333337</v>
       </c>
       <c r="D17" s="32"/>
-      <c r="E17" s="41"/>
+      <c r="E17" s="41">
+        <v>11</v>
+      </c>
       <c r="F17" s="18" t="s">
         <v>398</v>
       </c>
       <c r="G17" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="H17" s="62">
+      <c r="H17" s="68">
         <v>14.703150000000001</v>
       </c>
       <c r="I17" s="32"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="43"/>
-    </row>
-    <row r="18" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J17" s="41">
+        <v>11</v>
+      </c>
+      <c r="K17" s="18" t="s">
+        <v>450</v>
+      </c>
+      <c r="L17" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="M17" s="68">
+        <v>50.907166666666669</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="41">
         <v>12</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="42">
+      <c r="C18" s="68">
         <v>41.4268</v>
       </c>
       <c r="D18" s="32"/>
-      <c r="E18" s="41"/>
+      <c r="E18" s="41">
+        <v>12</v>
+      </c>
       <c r="F18" s="18" t="s">
         <v>491</v>
       </c>
       <c r="G18" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="62">
+      <c r="H18" s="68">
         <v>14.65865</v>
       </c>
       <c r="I18" s="32"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="43"/>
-    </row>
-    <row r="19" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J18" s="41">
+        <v>12</v>
+      </c>
+      <c r="K18" s="18" t="s">
+        <v>383</v>
+      </c>
+      <c r="L18" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="M18" s="68">
+        <v>48.295400000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="41">
         <v>13</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="42">
+      <c r="C19" s="68">
         <v>40.607216666666666</v>
       </c>
       <c r="D19" s="32"/>
-      <c r="E19" s="41"/>
+      <c r="E19" s="41">
+        <v>13</v>
+      </c>
       <c r="F19" s="18" t="s">
         <v>492</v>
       </c>
       <c r="G19" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="62">
+      <c r="H19" s="68">
         <v>14.6023</v>
       </c>
       <c r="I19" s="32"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="43"/>
-    </row>
-    <row r="20" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J19" s="41">
+        <v>13</v>
+      </c>
+      <c r="K19" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="L19" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="M19" s="68">
+        <v>47.136850000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="41">
         <v>14</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="42">
+      <c r="C20" s="68">
         <v>30.602</v>
       </c>
       <c r="D20" s="32"/>
-      <c r="E20" s="41"/>
+      <c r="E20" s="41">
+        <v>14</v>
+      </c>
       <c r="F20" s="18" t="s">
         <v>347</v>
       </c>
       <c r="G20" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="62">
+      <c r="H20" s="68">
         <v>13.961783333333333</v>
       </c>
       <c r="I20" s="32"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="43"/>
-    </row>
-    <row r="21" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J20" s="41">
+        <v>14</v>
+      </c>
+      <c r="K20" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="L20" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="M20" s="68">
+        <v>47.096550000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="41">
         <v>15</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="42">
+      <c r="C21" s="68">
         <v>29.760116666666665</v>
       </c>
       <c r="D21" s="32"/>
-      <c r="E21" s="41"/>
+      <c r="E21" s="41">
+        <v>15</v>
+      </c>
       <c r="F21" s="18" t="s">
         <v>493</v>
       </c>
       <c r="G21" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="H21" s="62">
+      <c r="H21" s="68">
         <v>13.478633333333333</v>
       </c>
       <c r="I21" s="32"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="43"/>
-    </row>
-    <row r="22" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J21" s="41">
+        <v>15</v>
+      </c>
+      <c r="K21" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="L21" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="M21" s="68">
+        <v>40.962566666666667</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="41">
         <v>16</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="42">
+      <c r="C22" s="68">
         <v>24.136700000000001</v>
       </c>
       <c r="D22" s="32"/>
-      <c r="E22" s="41"/>
+      <c r="E22" s="41">
+        <v>16</v>
+      </c>
       <c r="F22" s="18" t="s">
         <v>494</v>
       </c>
       <c r="G22" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="H22" s="62">
+      <c r="H22" s="68">
         <v>13.429333333333334</v>
       </c>
       <c r="I22" s="32"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="43"/>
-    </row>
-    <row r="23" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J22" s="41">
+        <v>16</v>
+      </c>
+      <c r="K22" s="18" t="s">
+        <v>334</v>
+      </c>
+      <c r="L22" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="M22" s="68">
+        <v>36.593916666666665</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="41">
         <v>17</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="42">
+      <c r="C23" s="68">
         <v>22.285299999999999</v>
       </c>
       <c r="D23" s="32"/>
-      <c r="E23" s="41"/>
+      <c r="E23" s="41">
+        <v>17</v>
+      </c>
       <c r="F23" s="18" t="s">
         <v>495</v>
       </c>
       <c r="G23" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="H23" s="62">
+      <c r="H23" s="68">
         <v>13.334916666666667</v>
       </c>
       <c r="I23" s="32"/>
-      <c r="J23" s="41"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="43"/>
-    </row>
-    <row r="24" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J23" s="41">
+        <v>17</v>
+      </c>
+      <c r="K23" s="18" t="s">
+        <v>522</v>
+      </c>
+      <c r="L23" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="M23" s="68">
+        <v>32.092133333333337</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="41">
         <v>18</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="42">
+      <c r="C24" s="68">
         <v>19.690799999999999</v>
       </c>
       <c r="D24" s="32"/>
-      <c r="E24" s="41"/>
+      <c r="E24" s="41">
+        <v>18</v>
+      </c>
       <c r="F24" s="18" t="s">
         <v>496</v>
       </c>
       <c r="G24" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="H24" s="62">
+      <c r="H24" s="68">
         <v>12.918850000000001</v>
       </c>
       <c r="I24" s="32"/>
-      <c r="J24" s="41"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="43"/>
-    </row>
-    <row r="25" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J24" s="41">
+        <v>18</v>
+      </c>
+      <c r="K24" s="18" t="s">
+        <v>381</v>
+      </c>
+      <c r="L24" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="M24" s="68">
+        <v>30.602</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="41">
         <v>19</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="42">
+      <c r="C25" s="68">
         <v>16.176666666666666</v>
       </c>
       <c r="D25" s="32"/>
-      <c r="E25" s="41"/>
+      <c r="E25" s="41">
+        <v>19</v>
+      </c>
       <c r="F25" s="18" t="s">
         <v>497</v>
       </c>
       <c r="G25" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="H25" s="62">
+      <c r="H25" s="68">
         <v>12.884499999999999</v>
       </c>
       <c r="I25" s="32"/>
-      <c r="J25" s="41"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="43"/>
-    </row>
-    <row r="26" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J25" s="41">
+        <v>19</v>
+      </c>
+      <c r="K25" s="18" t="s">
+        <v>442</v>
+      </c>
+      <c r="L25" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="M25" s="68">
+        <v>29.760116666666665</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="41">
         <v>20</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="42">
+      <c r="C26" s="68">
         <v>15.014533333333333</v>
       </c>
       <c r="D26" s="32"/>
-      <c r="E26" s="41"/>
+      <c r="E26" s="41">
+        <v>20</v>
+      </c>
       <c r="F26" s="18" t="s">
         <v>498</v>
       </c>
       <c r="G26" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="H26" s="62">
+      <c r="H26" s="68">
         <v>12.736666666666666</v>
       </c>
       <c r="I26" s="32"/>
-      <c r="J26" s="41"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="43"/>
-    </row>
-    <row r="27" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J26" s="41">
+        <v>20</v>
+      </c>
+      <c r="K26" s="18" t="s">
+        <v>526</v>
+      </c>
+      <c r="L26" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="M26" s="68">
+        <v>27.915983333333333</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="44">
         <v>21</v>
       </c>
       <c r="B27" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="45">
+      <c r="C27" s="69">
         <v>14.377666666666666</v>
       </c>
       <c r="D27" s="32"/>
-      <c r="E27" s="44"/>
+      <c r="E27" s="44">
+        <v>21</v>
+      </c>
       <c r="F27" s="20" t="s">
         <v>499</v>
       </c>
       <c r="G27" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="H27" s="63">
+      <c r="H27" s="69">
         <v>12.3017</v>
       </c>
       <c r="I27" s="32"/>
-      <c r="J27" s="44"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="46"/>
-    </row>
-    <row r="28" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J27" s="44">
+        <v>21</v>
+      </c>
+      <c r="K27" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="L27" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="M27" s="69">
+        <v>26.039516666666668</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="44">
         <v>22</v>
       </c>
       <c r="B28" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="45">
+      <c r="C28" s="69">
         <v>13.885199999999999</v>
       </c>
       <c r="D28" s="32"/>
-      <c r="E28" s="44"/>
+      <c r="E28" s="44">
+        <v>22</v>
+      </c>
       <c r="F28" s="20" t="s">
         <v>500</v>
       </c>
       <c r="G28" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="H28" s="63">
+      <c r="H28" s="69">
         <v>11.664566666666667</v>
       </c>
       <c r="I28" s="32"/>
-      <c r="J28" s="44"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="46"/>
-    </row>
-    <row r="29" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J28" s="44">
+        <v>22</v>
+      </c>
+      <c r="K28" s="20" t="s">
+        <v>527</v>
+      </c>
+      <c r="L28" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="M28" s="69">
+        <v>17.190616666666667</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="44">
         <v>23</v>
       </c>
       <c r="B29" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="45">
+      <c r="C29" s="69">
         <v>12.404</v>
       </c>
       <c r="D29" s="32"/>
-      <c r="E29" s="44"/>
+      <c r="E29" s="44">
+        <v>23</v>
+      </c>
       <c r="F29" s="20" t="s">
         <v>501</v>
       </c>
       <c r="G29" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H29" s="63">
+      <c r="H29" s="69">
         <v>10.996600000000001</v>
       </c>
       <c r="I29" s="32"/>
-      <c r="J29" s="44"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="46"/>
-    </row>
-    <row r="30" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J29" s="44">
+        <v>23</v>
+      </c>
+      <c r="K29" s="20" t="s">
+        <v>398</v>
+      </c>
+      <c r="L29" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="M29" s="69">
+        <v>14.815149999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="44">
         <v>24</v>
       </c>
       <c r="B30" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="C30" s="45">
+      <c r="C30" s="69">
         <v>11.135983333333334</v>
       </c>
       <c r="D30" s="32"/>
-      <c r="E30" s="44"/>
+      <c r="E30" s="44">
+        <v>24</v>
+      </c>
       <c r="F30" s="20" t="s">
         <v>502</v>
       </c>
       <c r="G30" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="H30" s="63">
+      <c r="H30" s="69">
         <v>10.993616666666666</v>
       </c>
       <c r="I30" s="32"/>
-      <c r="J30" s="44"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="46"/>
-    </row>
-    <row r="31" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J30" s="44">
+        <v>24</v>
+      </c>
+      <c r="K30" s="20" t="s">
+        <v>348</v>
+      </c>
+      <c r="L30" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="M30" s="69">
+        <v>14.5677</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="44">
         <v>25</v>
       </c>
       <c r="B31" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="C31" s="45">
+      <c r="C31" s="69">
         <v>9.5182166666666674</v>
       </c>
       <c r="D31" s="32"/>
-      <c r="E31" s="44"/>
+      <c r="E31" s="44">
+        <v>25</v>
+      </c>
       <c r="F31" s="20" t="s">
         <v>503</v>
       </c>
       <c r="G31" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="H31" s="63">
+      <c r="H31" s="69">
         <v>10.846583333333333</v>
       </c>
       <c r="I31" s="32"/>
-      <c r="J31" s="44"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="46"/>
-    </row>
-    <row r="32" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J31" s="44">
+        <v>25</v>
+      </c>
+      <c r="K31" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="L31" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="M31" s="69">
+        <v>14.012066666666666</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="44">
         <v>26</v>
       </c>
       <c r="B32" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="C32" s="45">
+      <c r="C32" s="69">
         <v>9.5180000000000007</v>
       </c>
       <c r="D32" s="32"/>
-      <c r="E32" s="44"/>
+      <c r="E32" s="44">
+        <v>26</v>
+      </c>
       <c r="F32" s="20" t="s">
         <v>458</v>
       </c>
       <c r="G32" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H32" s="63">
+      <c r="H32" s="69">
         <v>10.729150000000001</v>
       </c>
       <c r="I32" s="32"/>
-      <c r="J32" s="44"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="46"/>
-    </row>
-    <row r="33" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J32" s="44">
+        <v>26</v>
+      </c>
+      <c r="K32" s="20" t="s">
+        <v>453</v>
+      </c>
+      <c r="L32" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="M32" s="69">
+        <v>13.4015</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="44">
         <v>27</v>
       </c>
       <c r="B33" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="C33" s="45">
+      <c r="C33" s="69">
         <v>9.358433333333334</v>
       </c>
       <c r="D33" s="32"/>
-      <c r="E33" s="44"/>
+      <c r="E33" s="44">
+        <v>27</v>
+      </c>
       <c r="F33" s="20" t="s">
         <v>339</v>
       </c>
       <c r="G33" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H33" s="63">
+      <c r="H33" s="69">
         <v>10.672533333333334</v>
       </c>
       <c r="I33" s="32"/>
-      <c r="J33" s="44"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="46"/>
-    </row>
-    <row r="34" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J33" s="44">
+        <v>27</v>
+      </c>
+      <c r="K33" s="20" t="s">
+        <v>463</v>
+      </c>
+      <c r="L33" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="M33" s="69">
+        <v>12.884499999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="44">
         <v>28</v>
       </c>
       <c r="B34" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="C34" s="45">
+      <c r="C34" s="69">
         <v>8.8281166666666664</v>
       </c>
       <c r="D34" s="32"/>
-      <c r="E34" s="44"/>
+      <c r="E34" s="44">
+        <v>28</v>
+      </c>
       <c r="F34" s="20" t="s">
         <v>504</v>
       </c>
       <c r="G34" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H34" s="63">
+      <c r="H34" s="69">
         <v>10.651083333333334</v>
       </c>
       <c r="I34" s="32"/>
-      <c r="J34" s="44"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="46"/>
-    </row>
-    <row r="35" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J34" s="44">
+        <v>28</v>
+      </c>
+      <c r="K34" s="20" t="s">
+        <v>340</v>
+      </c>
+      <c r="L34" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="M34" s="69">
+        <v>11.299666666666667</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="44">
         <v>29</v>
       </c>
       <c r="B35" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="C35" s="45">
+      <c r="C35" s="69">
         <v>8.7695500000000006</v>
       </c>
       <c r="D35" s="32"/>
-      <c r="E35" s="44"/>
+      <c r="E35" s="44">
+        <v>29</v>
+      </c>
       <c r="F35" s="20" t="s">
         <v>308</v>
       </c>
       <c r="G35" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H35" s="63">
+      <c r="H35" s="69">
         <v>10.642733333333334</v>
       </c>
       <c r="I35" s="32"/>
-      <c r="J35" s="44"/>
-      <c r="K35" s="20"/>
-      <c r="L35" s="46"/>
-    </row>
-    <row r="36" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J35" s="44">
+        <v>29</v>
+      </c>
+      <c r="K35" s="20" t="s">
+        <v>528</v>
+      </c>
+      <c r="L35" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="M35" s="69">
+        <v>11.243566666666666</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="44">
         <v>30</v>
       </c>
       <c r="B36" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="C36" s="45">
+      <c r="C36" s="69">
         <v>8.4889500000000009</v>
       </c>
       <c r="D36" s="32"/>
-      <c r="E36" s="44"/>
+      <c r="E36" s="44">
+        <v>30</v>
+      </c>
       <c r="F36" s="20" t="s">
         <v>505</v>
       </c>
       <c r="G36" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H36" s="63">
+      <c r="H36" s="69">
         <v>10.56325</v>
       </c>
       <c r="I36" s="32"/>
-      <c r="J36" s="44"/>
-      <c r="K36" s="20"/>
-      <c r="L36" s="46"/>
-    </row>
-    <row r="37" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J36" s="44">
+        <v>30</v>
+      </c>
+      <c r="K36" s="20" t="s">
+        <v>529</v>
+      </c>
+      <c r="L36" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="M36" s="69">
+        <v>11.135983333333334</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="44">
         <v>31</v>
       </c>
       <c r="B37" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="C37" s="45">
+      <c r="C37" s="69">
         <v>8.2159999999999993</v>
       </c>
       <c r="D37" s="32"/>
-      <c r="E37" s="44"/>
+      <c r="E37" s="44">
+        <v>31</v>
+      </c>
       <c r="F37" s="20" t="s">
         <v>506</v>
       </c>
       <c r="G37" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H37" s="63">
+      <c r="H37" s="69">
         <v>9.7864000000000004</v>
       </c>
       <c r="I37" s="32"/>
-      <c r="J37" s="44"/>
-      <c r="K37" s="20"/>
-      <c r="L37" s="46"/>
-    </row>
-    <row r="38" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J37" s="44">
+        <v>31</v>
+      </c>
+      <c r="K37" s="20" t="s">
+        <v>530</v>
+      </c>
+      <c r="L37" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="M37" s="69">
+        <v>9.9664000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="44">
         <v>32</v>
       </c>
       <c r="B38" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="C38" s="45">
+      <c r="C38" s="69">
         <v>6.8408333333333333</v>
       </c>
       <c r="D38" s="32"/>
-      <c r="E38" s="44"/>
+      <c r="E38" s="44">
+        <v>32</v>
+      </c>
       <c r="F38" s="20" t="s">
         <v>507</v>
       </c>
       <c r="G38" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H38" s="63">
+      <c r="H38" s="69">
         <v>9.6528166666666664</v>
       </c>
       <c r="I38" s="32"/>
-      <c r="J38" s="44"/>
-      <c r="K38" s="20"/>
-      <c r="L38" s="46"/>
-    </row>
-    <row r="39" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J38" s="44">
+        <v>32</v>
+      </c>
+      <c r="K38" s="20" t="s">
+        <v>531</v>
+      </c>
+      <c r="L38" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="M38" s="69">
+        <v>9.7855833333333333</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="44">
         <v>33</v>
       </c>
       <c r="B39" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="45">
+      <c r="C39" s="69">
         <v>6.6478000000000002</v>
       </c>
       <c r="D39" s="32"/>
-      <c r="E39" s="44"/>
+      <c r="E39" s="44">
+        <v>33</v>
+      </c>
       <c r="F39" s="20" t="s">
         <v>508</v>
       </c>
       <c r="G39" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="H39" s="63">
+      <c r="H39" s="69">
         <v>9.6216166666666663</v>
       </c>
       <c r="I39" s="32"/>
-      <c r="J39" s="44"/>
-      <c r="K39" s="20"/>
-      <c r="L39" s="46"/>
-    </row>
-    <row r="40" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J39" s="44">
+        <v>33</v>
+      </c>
+      <c r="K39" s="20" t="s">
+        <v>532</v>
+      </c>
+      <c r="L39" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="M39" s="69">
+        <v>9.5180000000000007</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="44">
         <v>34</v>
       </c>
       <c r="B40" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C40" s="45">
+      <c r="C40" s="69">
         <v>6.3734999999999999</v>
       </c>
       <c r="D40" s="32"/>
-      <c r="E40" s="44"/>
+      <c r="E40" s="44">
+        <v>34</v>
+      </c>
       <c r="F40" s="20" t="s">
         <v>509</v>
       </c>
       <c r="G40" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="H40" s="63">
+      <c r="H40" s="69">
         <v>9.5180000000000007</v>
       </c>
       <c r="I40" s="32"/>
-      <c r="J40" s="44"/>
-      <c r="K40" s="20"/>
-      <c r="L40" s="46"/>
-    </row>
-    <row r="41" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J40" s="44">
+        <v>34</v>
+      </c>
+      <c r="K40" s="20" t="s">
+        <v>521</v>
+      </c>
+      <c r="L40" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="M40" s="69">
+        <v>9.4724500000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="44">
         <v>35</v>
       </c>
       <c r="B41" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="C41" s="45">
+      <c r="C41" s="69">
         <v>5.9540833333333332</v>
       </c>
       <c r="D41" s="32"/>
-      <c r="E41" s="44"/>
+      <c r="E41" s="44">
+        <v>35</v>
+      </c>
       <c r="F41" s="20" t="s">
         <v>510</v>
       </c>
       <c r="G41" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H41" s="63">
+      <c r="H41" s="69">
         <v>9.4505333333333326</v>
       </c>
       <c r="I41" s="32"/>
-      <c r="J41" s="44"/>
-      <c r="K41" s="20"/>
-      <c r="L41" s="46"/>
-    </row>
-    <row r="42" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J41" s="44">
+        <v>35</v>
+      </c>
+      <c r="K41" s="20" t="s">
+        <v>533</v>
+      </c>
+      <c r="L41" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="M41" s="69">
+        <v>8.2159999999999993</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="44">
         <v>36</v>
       </c>
       <c r="B42" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="C42" s="45">
+      <c r="C42" s="69">
         <v>5.8604333333333329</v>
       </c>
       <c r="D42" s="32"/>
-      <c r="E42" s="44"/>
+      <c r="E42" s="44">
+        <v>36</v>
+      </c>
       <c r="F42" s="20" t="s">
         <v>471</v>
       </c>
       <c r="G42" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H42" s="63">
+      <c r="H42" s="69">
         <v>9.1630833333333328</v>
       </c>
       <c r="I42" s="32"/>
-      <c r="J42" s="44"/>
-      <c r="K42" s="20"/>
-      <c r="L42" s="46"/>
-    </row>
-    <row r="43" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J42" s="44">
+        <v>36</v>
+      </c>
+      <c r="K42" s="20" t="s">
+        <v>332</v>
+      </c>
+      <c r="L42" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="M42" s="69">
+        <v>7.8304666666666662</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="44">
         <v>37</v>
       </c>
       <c r="B43" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="C43" s="45">
+      <c r="C43" s="69">
         <v>5.6</v>
       </c>
       <c r="D43" s="32"/>
-      <c r="E43" s="44"/>
+      <c r="E43" s="44">
+        <v>37</v>
+      </c>
       <c r="F43" s="20" t="s">
         <v>384</v>
       </c>
       <c r="G43" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H43" s="63">
+      <c r="H43" s="69">
         <v>9.1441333333333326</v>
       </c>
       <c r="I43" s="32"/>
-      <c r="J43" s="44"/>
-      <c r="K43" s="20"/>
-      <c r="L43" s="46"/>
-    </row>
-    <row r="44" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J43" s="44">
+        <v>37</v>
+      </c>
+      <c r="K43" s="20" t="s">
+        <v>534</v>
+      </c>
+      <c r="L43" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="M43" s="69">
+        <v>7.1057666666666668</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="44">
         <v>38</v>
       </c>
       <c r="B44" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="C44" s="45">
+      <c r="C44" s="69">
         <v>5.5437500000000002</v>
       </c>
       <c r="D44" s="32"/>
-      <c r="E44" s="44"/>
+      <c r="E44" s="44">
+        <v>38</v>
+      </c>
       <c r="F44" s="20" t="s">
         <v>345</v>
       </c>
       <c r="G44" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H44" s="63">
+      <c r="H44" s="69">
         <v>8.6850000000000005</v>
       </c>
       <c r="I44" s="32"/>
-      <c r="J44" s="44"/>
-      <c r="K44" s="20"/>
-      <c r="L44" s="46"/>
-    </row>
-    <row r="45" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J44" s="44">
+        <v>38</v>
+      </c>
+      <c r="K44" s="20" t="s">
+        <v>535</v>
+      </c>
+      <c r="L44" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="M44" s="69">
+        <v>6.9427666666666665</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="44">
         <v>39</v>
       </c>
       <c r="B45" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="45">
+      <c r="C45" s="69">
         <v>5.2590166666666667</v>
       </c>
       <c r="D45" s="32"/>
-      <c r="E45" s="44"/>
+      <c r="E45" s="44">
+        <v>39</v>
+      </c>
       <c r="F45" s="20" t="s">
         <v>511</v>
       </c>
       <c r="G45" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H45" s="63">
+      <c r="H45" s="69">
         <v>8.5350999999999999</v>
       </c>
       <c r="I45" s="32"/>
-      <c r="J45" s="44"/>
-      <c r="K45" s="20"/>
-      <c r="L45" s="46"/>
-    </row>
-    <row r="46" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J45" s="44">
+        <v>39</v>
+      </c>
+      <c r="K45" s="20" t="s">
+        <v>536</v>
+      </c>
+      <c r="L45" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="M45" s="69">
+        <v>6.8028833333333329</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="44">
         <v>40</v>
       </c>
       <c r="B46" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="C46" s="45">
+      <c r="C46" s="69">
         <v>5.0682166666666664</v>
       </c>
       <c r="D46" s="32"/>
-      <c r="E46" s="44"/>
+      <c r="E46" s="44">
+        <v>40</v>
+      </c>
       <c r="F46" s="20" t="s">
         <v>512</v>
       </c>
       <c r="G46" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="H46" s="63">
+      <c r="H46" s="69">
         <v>8.4289666666666658</v>
       </c>
       <c r="I46" s="32"/>
-      <c r="J46" s="44"/>
-      <c r="K46" s="20"/>
-      <c r="L46" s="46"/>
-    </row>
-    <row r="47" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J46" s="44">
+        <v>40</v>
+      </c>
+      <c r="K46" s="20" t="s">
+        <v>537</v>
+      </c>
+      <c r="L46" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="M46" s="69">
+        <v>6.7061999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="44">
         <v>41</v>
       </c>
       <c r="B47" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="C47" s="45">
+      <c r="C47" s="69">
         <v>5.0471000000000004</v>
       </c>
       <c r="D47" s="32"/>
-      <c r="E47" s="44"/>
+      <c r="E47" s="44">
+        <v>41</v>
+      </c>
       <c r="F47" s="20" t="s">
         <v>416</v>
       </c>
       <c r="G47" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="H47" s="63">
+      <c r="H47" s="69">
         <v>8.2159999999999993</v>
       </c>
       <c r="I47" s="32"/>
-      <c r="J47" s="44"/>
-      <c r="K47" s="20"/>
-      <c r="L47" s="46"/>
-    </row>
-    <row r="48" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J47" s="44">
+        <v>41</v>
+      </c>
+      <c r="K47" s="20" t="s">
+        <v>538</v>
+      </c>
+      <c r="L47" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="M47" s="69">
+        <v>6.6902166666666663</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="44">
         <v>42</v>
       </c>
       <c r="B48" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="C48" s="45">
+      <c r="C48" s="69">
         <v>4.9216666666666669</v>
       </c>
       <c r="D48" s="32"/>
-      <c r="E48" s="44"/>
+      <c r="E48" s="44">
+        <v>42</v>
+      </c>
       <c r="F48" s="20" t="s">
         <v>397</v>
       </c>
       <c r="G48" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H48" s="63">
+      <c r="H48" s="69">
         <v>8.1832499999999992</v>
       </c>
       <c r="I48" s="32"/>
-      <c r="J48" s="44"/>
-      <c r="K48" s="20"/>
-      <c r="L48" s="46"/>
-    </row>
-    <row r="49" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J48" s="44">
+        <v>42</v>
+      </c>
+      <c r="K48" s="20" t="s">
+        <v>539</v>
+      </c>
+      <c r="L48" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="M48" s="69">
+        <v>6.6478000000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="44">
         <v>43</v>
       </c>
       <c r="B49" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="C49" s="45">
+      <c r="C49" s="69">
         <v>4.7584499999999998</v>
       </c>
       <c r="D49" s="32"/>
-      <c r="E49" s="44"/>
+      <c r="E49" s="44">
+        <v>43</v>
+      </c>
       <c r="F49" s="20" t="s">
         <v>513</v>
       </c>
       <c r="G49" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="H49" s="63">
+      <c r="H49" s="69">
         <v>8.0293333333333337</v>
       </c>
       <c r="I49" s="32"/>
-      <c r="J49" s="44"/>
-      <c r="K49" s="20"/>
-      <c r="L49" s="46"/>
-    </row>
-    <row r="50" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J49" s="44">
+        <v>43</v>
+      </c>
+      <c r="K49" s="20" t="s">
+        <v>448</v>
+      </c>
+      <c r="L49" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="M49" s="69">
+        <v>6.4262499999999996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="44">
         <v>44</v>
       </c>
       <c r="B50" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="C50" s="45">
+      <c r="C50" s="69">
         <v>4.7210999999999999</v>
       </c>
       <c r="D50" s="32"/>
-      <c r="E50" s="44"/>
+      <c r="E50" s="44">
+        <v>44</v>
+      </c>
       <c r="F50" s="20" t="s">
         <v>514</v>
       </c>
       <c r="G50" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H50" s="63">
+      <c r="H50" s="69">
         <v>7.9660666666666664</v>
       </c>
       <c r="I50" s="32"/>
-      <c r="J50" s="44"/>
-      <c r="K50" s="20"/>
-      <c r="L50" s="46"/>
-    </row>
-    <row r="51" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J50" s="44">
+        <v>44</v>
+      </c>
+      <c r="K50" s="20" t="s">
+        <v>540</v>
+      </c>
+      <c r="L50" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="M50" s="69">
+        <v>6.2958999999999996</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="44">
         <v>45</v>
       </c>
       <c r="B51" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="C51" s="45">
+      <c r="C51" s="69">
         <v>4.6946000000000003</v>
       </c>
       <c r="D51" s="32"/>
-      <c r="E51" s="44"/>
+      <c r="E51" s="44">
+        <v>45</v>
+      </c>
       <c r="F51" s="20" t="s">
         <v>399</v>
       </c>
       <c r="G51" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H51" s="63">
+      <c r="H51" s="69">
         <v>7.964666666666667</v>
       </c>
       <c r="I51" s="32"/>
-      <c r="J51" s="44"/>
-      <c r="K51" s="20"/>
-      <c r="L51" s="46"/>
-    </row>
-    <row r="52" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J51" s="44">
+        <v>45</v>
+      </c>
+      <c r="K51" s="20" t="s">
+        <v>541</v>
+      </c>
+      <c r="L51" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="M51" s="69">
+        <v>6.2650499999999996</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="44">
         <v>46</v>
       </c>
       <c r="B52" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="C52" s="45">
+      <c r="C52" s="69">
         <v>4.4150999999999998</v>
       </c>
       <c r="D52" s="32"/>
-      <c r="E52" s="44"/>
+      <c r="E52" s="44">
+        <v>46</v>
+      </c>
       <c r="F52" s="20" t="s">
         <v>515</v>
       </c>
       <c r="G52" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="H52" s="63">
+      <c r="H52" s="69">
         <v>7.9546000000000001</v>
       </c>
       <c r="I52" s="32"/>
-      <c r="J52" s="44"/>
-      <c r="K52" s="20"/>
-      <c r="L52" s="46"/>
-    </row>
-    <row r="53" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J52" s="44">
+        <v>46</v>
+      </c>
+      <c r="K52" s="20" t="s">
+        <v>542</v>
+      </c>
+      <c r="L52" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="M52" s="69">
+        <v>5.9540833333333332</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="44">
         <v>47</v>
       </c>
       <c r="B53" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="C53" s="45">
+      <c r="C53" s="69">
         <v>4.3005666666666666</v>
       </c>
       <c r="D53" s="32"/>
-      <c r="E53" s="44"/>
+      <c r="E53" s="44">
+        <v>47</v>
+      </c>
       <c r="F53" s="20" t="s">
         <v>516</v>
       </c>
       <c r="G53" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H53" s="63">
+      <c r="H53" s="69">
         <v>7.8794666666666666</v>
       </c>
       <c r="I53" s="32"/>
-      <c r="J53" s="44"/>
-      <c r="K53" s="20"/>
-      <c r="L53" s="46"/>
-    </row>
-    <row r="54" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J53" s="44">
+        <v>47</v>
+      </c>
+      <c r="K53" s="20" t="s">
+        <v>543</v>
+      </c>
+      <c r="L53" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="M53" s="69">
+        <v>5.8604333333333329</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="44">
         <v>48</v>
       </c>
       <c r="B54" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="C54" s="45">
+      <c r="C54" s="69">
         <v>4.2141666666666664</v>
       </c>
       <c r="D54" s="32"/>
-      <c r="E54" s="44"/>
+      <c r="E54" s="44">
+        <v>48</v>
+      </c>
       <c r="F54" s="20" t="s">
         <v>517</v>
       </c>
       <c r="G54" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H54" s="63">
+      <c r="H54" s="69">
         <v>7.8597833333333336</v>
       </c>
       <c r="I54" s="32"/>
-      <c r="J54" s="44"/>
-      <c r="K54" s="20"/>
-      <c r="L54" s="46"/>
-    </row>
-    <row r="55" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J54" s="44">
+        <v>48</v>
+      </c>
+      <c r="K54" s="20" t="s">
+        <v>544</v>
+      </c>
+      <c r="L54" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="M54" s="69">
+        <v>5.5476666666666663</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="44">
         <v>49</v>
       </c>
       <c r="B55" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="C55" s="45">
+      <c r="C55" s="69">
         <v>4.0960000000000001</v>
       </c>
       <c r="D55" s="32"/>
-      <c r="E55" s="44"/>
+      <c r="E55" s="44">
+        <v>49</v>
+      </c>
       <c r="F55" s="20" t="s">
         <v>480</v>
       </c>
       <c r="G55" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="H55" s="63">
+      <c r="H55" s="69">
         <v>7.6649666666666665</v>
       </c>
       <c r="I55" s="32"/>
-      <c r="J55" s="44"/>
-      <c r="K55" s="20"/>
-      <c r="L55" s="46"/>
-    </row>
-    <row r="56" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J55" s="44">
+        <v>49</v>
+      </c>
+      <c r="K55" s="20" t="s">
+        <v>545</v>
+      </c>
+      <c r="L55" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="M55" s="69">
+        <v>5.3366666666666669</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="47">
         <v>50</v>
       </c>
       <c r="B56" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="C56" s="49">
+      <c r="C56" s="70">
         <v>4.064916666666667</v>
       </c>
       <c r="D56" s="32"/>
-      <c r="E56" s="47"/>
+      <c r="E56" s="47">
+        <v>50</v>
+      </c>
       <c r="F56" s="48" t="s">
         <v>518</v>
       </c>
       <c r="G56" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="H56" s="64">
+      <c r="H56" s="70">
         <v>7.5474500000000004</v>
       </c>
       <c r="I56" s="32"/>
-      <c r="J56" s="47"/>
-      <c r="K56" s="48"/>
-      <c r="L56" s="50"/>
+      <c r="J56" s="47">
+        <v>50</v>
+      </c>
+      <c r="K56" s="48" t="s">
+        <v>546</v>
+      </c>
+      <c r="L56" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="M56" s="70">
+        <v>5.2590166666666667</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="E5:H5"/>
-    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J5:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8335,7 +8958,7 @@
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G32" sqref="G32"/>
-      <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomLeft" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add exploratory visualization: Top 5 Artists Monthly Listening (Jan–Oct 2025)
</commit_message>
<xml_diff>
--- a/excel/spotify_listening_report_2025.xlsx
+++ b/excel/spotify_listening_report_2025.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jennifermitchell/Documents/projects/projects_2025/analytics_projects/Spotify_Sandbox/spotify_sandbox_github/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6207D268-129D-774F-BE17-A23BCAA4E399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601AECFD-65A5-B840-BBC2-C1B98DC39ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33980" yWindow="-1460" windowWidth="31440" windowHeight="20400" activeTab="1" xr2:uid="{02962024-D185-E646-89C4-A67A4B8F8E62}"/>
+    <workbookView xWindow="33980" yWindow="-1460" windowWidth="31440" windowHeight="20400" activeTab="2" xr2:uid="{02962024-D185-E646-89C4-A67A4B8F8E62}"/>
   </bookViews>
   <sheets>
     <sheet name="2025 Overview" sheetId="13" r:id="rId1"/>
     <sheet name="Top Artists Over Time" sheetId="32" r:id="rId2"/>
-    <sheet name="Jan" sheetId="23" r:id="rId3"/>
-    <sheet name="Feb" sheetId="24" r:id="rId4"/>
-    <sheet name="Mar" sheetId="25" r:id="rId5"/>
-    <sheet name="Apr" sheetId="26" r:id="rId6"/>
-    <sheet name="May" sheetId="27" r:id="rId7"/>
-    <sheet name="Jun" sheetId="28" r:id="rId8"/>
-    <sheet name="Jul" sheetId="29" r:id="rId9"/>
-    <sheet name="Aug" sheetId="30" r:id="rId10"/>
-    <sheet name="Sep" sheetId="31" r:id="rId11"/>
+    <sheet name="Top 5 Chart" sheetId="33" r:id="rId3"/>
+    <sheet name="Jan" sheetId="23" r:id="rId4"/>
+    <sheet name="Feb" sheetId="24" r:id="rId5"/>
+    <sheet name="Mar" sheetId="25" r:id="rId6"/>
+    <sheet name="Apr" sheetId="26" r:id="rId7"/>
+    <sheet name="May" sheetId="27" r:id="rId8"/>
+    <sheet name="Jun" sheetId="28" r:id="rId9"/>
+    <sheet name="Jul" sheetId="29" r:id="rId10"/>
+    <sheet name="Aug" sheetId="30" r:id="rId11"/>
+    <sheet name="Sep" sheetId="31" r:id="rId12"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId12"/>
+    <externalReference r:id="rId13"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1599" uniqueCount="435">
   <si>
     <t>Based on Spotify Extended Streaming History Time Listened (Music Only)</t>
   </si>
@@ -1351,6 +1352,9 @@
   </si>
   <si>
     <t>2025 Total</t>
+  </si>
+  <si>
+    <t>Source: fact_plays_2025_with_album_family (Jan–Oct 2025)</t>
   </si>
 </sst>
 </file>
@@ -1362,7 +1366,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="#,##0.0_);\(#,##0.0\)"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1428,6 +1432,11 @@
     <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
+      <name val="-webkit-standard"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF777777"/>
       <name val="-webkit-standard"/>
     </font>
   </fonts>
@@ -1702,7 +1711,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1782,6 +1791,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1799,6 +1809,1652 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" cap="none" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Top 5 Artists – Monthly Listening (Jan–Oct 2025)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'[1]Top Artists Over Time'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vampire Weekend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'[1]Top Artists Over Time'!$B$3:$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>January</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>February</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>March</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>April</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>June</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>July</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>August</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>October</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'[1]Top Artists Over Time'!$B$5:$K$5</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0_);\(#,##0.0\)</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>264.58941666666669</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>82.985883333333334</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>73.428849999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>94.33056666666667</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>448.90249999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>251.72315</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>88.191900000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.3228166666666663</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>295.61993333333334</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18.266033333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4C78-E644-B363-A9FD0ACADA1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'[1]Top Artists Over Time'!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Kurt Vile</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'[1]Top Artists Over Time'!$B$3:$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>January</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>February</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>March</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>April</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>June</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>July</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>August</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>October</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'[1]Top Artists Over Time'!$B$7:$K$7</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0_);\(#,##0.0\)</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>233.69826666666665</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>105.74556666666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>111.83578333333334</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8266833333333334</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54.751866666666665</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.585416666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>214.98765</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>34.707616666666667</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.7098499999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4C78-E644-B363-A9FD0ACADA1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'[1]Top Artists Over Time'!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Jack White</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'[1]Top Artists Over Time'!$B$3:$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>January</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>February</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>March</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>April</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>June</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>July</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>August</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>October</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'[1]Top Artists Over Time'!$B$8:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0_);\(#,##0.0\)</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>6.6478000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>493.71803333333332</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.641783333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>99.057183333333327</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>33.958166666666664</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.18975</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4C78-E644-B363-A9FD0ACADA1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="929135567"/>
+        <c:axId val="929137295"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'[1]Top Artists Over Time'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Father John Misty</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'[1]Top Artists Over Time'!$B$3:$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>January</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>February</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>March</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>April</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>June</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>July</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>August</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>October</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'[1]Top Artists Over Time'!$B$4:$K$4</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0_);\(#,##0.0\)</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>130.97198333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1346.1851999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>313.61869999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>96.719149999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>79.266616666666664</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>141.3272</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.726566666666667</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.110749999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4C78-E644-B363-A9FD0ACADA1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'[1]Top Artists Over Time'!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ozzy Osbourne</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'[1]Top Artists Over Time'!$B$3:$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>January</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>February</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>March</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>April</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>May</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>June</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>July</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>August</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>September</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>October</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'[1]Top Artists Over Time'!$B$6:$K$6</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.0_);\(#,##0.0\)</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>221.81710000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>737.94141666666667</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>220.96671666666666</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60.29858333333334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-4C78-E644-B363-A9FD0ACADA1A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="929224735"/>
+        <c:axId val="929221775"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="929135567"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="929137295"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="929137295"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Minutes Played (Other Artists)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.0_);\(#,##0.0\)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="929135567"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="929221775"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Minutes Played (Father John Misty  and Ozzy Osbourne)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.0_);\(#,##0.0\)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="20" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="929224735"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="929224735"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="929221775"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="230">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="0" kern="1200" spc="20" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="2">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="1"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+            <a:alpha val="33000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </cs:spPr>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63327D67-D470-0043-95A2-A1CBE45ABEC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -1809,6 +3465,7 @@
       <sheetName val="2025 Overview"/>
       <sheetName val="Artist &amp; Song Ranking"/>
       <sheetName val="Top Artists Over Time"/>
+      <sheetName val="Top 5 Chart"/>
       <sheetName val="Sheet43"/>
       <sheetName val="oct_raw_plays_2025"/>
       <sheetName val="Artist Ranking"/>
@@ -1833,7 +3490,215 @@
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2">
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>January</v>
+          </cell>
+          <cell r="C3" t="str">
+            <v>February</v>
+          </cell>
+          <cell r="D3" t="str">
+            <v>March</v>
+          </cell>
+          <cell r="E3" t="str">
+            <v>April</v>
+          </cell>
+          <cell r="F3" t="str">
+            <v>May</v>
+          </cell>
+          <cell r="G3" t="str">
+            <v>June</v>
+          </cell>
+          <cell r="H3" t="str">
+            <v>July</v>
+          </cell>
+          <cell r="I3" t="str">
+            <v>August</v>
+          </cell>
+          <cell r="J3" t="str">
+            <v>September</v>
+          </cell>
+          <cell r="K3" t="str">
+            <v>October</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>Father John Misty</v>
+          </cell>
+          <cell r="B4">
+            <v>130.97198333333333</v>
+          </cell>
+          <cell r="C4">
+            <v>1346.1851999999999</v>
+          </cell>
+          <cell r="D4">
+            <v>313.61869999999999</v>
+          </cell>
+          <cell r="E4">
+            <v>96.719149999999999</v>
+          </cell>
+          <cell r="F4">
+            <v>79.266616666666664</v>
+          </cell>
+          <cell r="G4">
+            <v>141.3272</v>
+          </cell>
+          <cell r="H4">
+            <v>11.726566666666667</v>
+          </cell>
+          <cell r="I4">
+            <v>11.110749999999999</v>
+          </cell>
+          <cell r="J4">
+            <v>0</v>
+          </cell>
+          <cell r="K4">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>Vampire Weekend</v>
+          </cell>
+          <cell r="B5">
+            <v>264.58941666666669</v>
+          </cell>
+          <cell r="C5">
+            <v>82.985883333333334</v>
+          </cell>
+          <cell r="D5">
+            <v>73.428849999999997</v>
+          </cell>
+          <cell r="E5">
+            <v>94.33056666666667</v>
+          </cell>
+          <cell r="F5">
+            <v>448.90249999999997</v>
+          </cell>
+          <cell r="G5">
+            <v>251.72315</v>
+          </cell>
+          <cell r="H5">
+            <v>88.191900000000004</v>
+          </cell>
+          <cell r="I5">
+            <v>7.3228166666666663</v>
+          </cell>
+          <cell r="J5">
+            <v>295.61993333333334</v>
+          </cell>
+          <cell r="K5">
+            <v>18.266033333333333</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>Ozzy Osbourne</v>
+          </cell>
+          <cell r="B6">
+            <v>0</v>
+          </cell>
+          <cell r="C6">
+            <v>0</v>
+          </cell>
+          <cell r="D6">
+            <v>0</v>
+          </cell>
+          <cell r="E6">
+            <v>0</v>
+          </cell>
+          <cell r="F6">
+            <v>0</v>
+          </cell>
+          <cell r="G6">
+            <v>0</v>
+          </cell>
+          <cell r="H6">
+            <v>221.81710000000001</v>
+          </cell>
+          <cell r="I6">
+            <v>737.94141666666667</v>
+          </cell>
+          <cell r="J6">
+            <v>220.96671666666666</v>
+          </cell>
+          <cell r="K6">
+            <v>60.29858333333334</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>Kurt Vile</v>
+          </cell>
+          <cell r="B7">
+            <v>233.69826666666665</v>
+          </cell>
+          <cell r="C7">
+            <v>105.74556666666666</v>
+          </cell>
+          <cell r="D7">
+            <v>111.83578333333334</v>
+          </cell>
+          <cell r="E7">
+            <v>2.8266833333333334</v>
+          </cell>
+          <cell r="F7">
+            <v>54.751866666666665</v>
+          </cell>
+          <cell r="G7">
+            <v>22.585416666666667</v>
+          </cell>
+          <cell r="H7">
+            <v>214.98765</v>
+          </cell>
+          <cell r="I7">
+            <v>34.707616666666667</v>
+          </cell>
+          <cell r="J7">
+            <v>3.7098499999999999</v>
+          </cell>
+          <cell r="K7">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>Jack White</v>
+          </cell>
+          <cell r="B8">
+            <v>6.6478000000000002</v>
+          </cell>
+          <cell r="C8">
+            <v>493.71803333333332</v>
+          </cell>
+          <cell r="D8">
+            <v>16.641783333333333</v>
+          </cell>
+          <cell r="E8">
+            <v>0</v>
+          </cell>
+          <cell r="F8">
+            <v>0</v>
+          </cell>
+          <cell r="G8">
+            <v>99.057183333333327</v>
+          </cell>
+          <cell r="H8">
+            <v>0</v>
+          </cell>
+          <cell r="I8">
+            <v>33.958166666666664</v>
+          </cell>
+          <cell r="J8">
+            <v>15.18975</v>
+          </cell>
+          <cell r="K8">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
@@ -1854,6 +3719,7 @@
       <sheetData sheetId="20"/>
       <sheetData sheetId="21"/>
       <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6039,6 +7905,930 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4368EC2C-E0D7-B443-9AD2-CEC35644FA3F}">
+  <sheetPr>
+    <tabColor rgb="FFD0D0E8"/>
+  </sheetPr>
+  <dimension ref="A1:P32"/>
+  <sheetViews>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="F30" sqref="F30"/>
+      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="4" max="4" width="3" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.1640625" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" style="35" customWidth="1"/>
+    <col min="9" max="9" width="3" customWidth="1"/>
+    <col min="10" max="10" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.83203125" customWidth="1"/>
+    <col min="12" max="12" width="26.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" style="35" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="22" customHeight="1">
+      <c r="A1" s="36" t="s">
+        <v>375</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+    </row>
+    <row r="2" spans="1:16" ht="18" customHeight="1">
+      <c r="A2" s="37" t="s">
+        <v>318</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+    </row>
+    <row r="3" spans="1:16" ht="18" customHeight="1">
+      <c r="A3" s="38" t="s">
+        <v>319</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+    </row>
+    <row r="4" spans="1:16" ht="16" customHeight="1">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="8"/>
+    </row>
+    <row r="5" spans="1:16" s="9" customFormat="1" ht="18" customHeight="1">
+      <c r="A5" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="E5" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="J5" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+    </row>
+    <row r="6" spans="1:16" ht="18" customHeight="1">
+      <c r="A6" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="18" customHeight="1">
+      <c r="A7" s="13">
+        <v>1</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="46">
+        <v>280.16663333333332</v>
+      </c>
+      <c r="D7" s="16"/>
+      <c r="E7" s="13">
+        <v>1</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="46">
+        <v>50.24131666666667</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="13">
+        <v>1</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="46">
+        <v>231.46773333333334</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="18" customHeight="1">
+      <c r="A8" s="18">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="47">
+        <v>236.99503333333334</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" s="18">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="47">
+        <v>43.256316666666663</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="18">
+        <v>2</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" s="47">
+        <v>176.28213333333332</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="18" customHeight="1">
+      <c r="A9" s="18">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="47">
+        <v>221.81710000000001</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" s="18">
+        <v>3</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="47">
+        <v>33.327750000000002</v>
+      </c>
+      <c r="I9" s="16"/>
+      <c r="J9" s="18">
+        <v>3</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M9" s="47">
+        <v>161.66909999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="18" customHeight="1">
+      <c r="A10" s="18">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="47">
+        <v>214.98765</v>
+      </c>
+      <c r="D10" s="16"/>
+      <c r="E10" s="18">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="47">
+        <v>33.103883333333336</v>
+      </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="18">
+        <v>4</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10" s="47">
+        <v>92.383766666666673</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="18" customHeight="1">
+      <c r="A11" s="18">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="47">
+        <v>88.191900000000004</v>
+      </c>
+      <c r="D11" s="16"/>
+      <c r="E11" s="18">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="47">
+        <v>30.018733333333333</v>
+      </c>
+      <c r="I11" s="16"/>
+      <c r="J11" s="18">
+        <v>5</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M11" s="47">
+        <v>73.807516666666672</v>
+      </c>
+      <c r="P11" s="21"/>
+    </row>
+    <row r="12" spans="1:16" ht="18" customHeight="1">
+      <c r="A12" s="22">
+        <v>6</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="48">
+        <v>72.265533333333337</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="E12" s="22">
+        <v>6</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="48">
+        <v>29.276833333333332</v>
+      </c>
+      <c r="I12" s="16"/>
+      <c r="J12" s="22">
+        <v>6</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" s="48">
+        <v>60.649433333333334</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="18" customHeight="1">
+      <c r="A13" s="22">
+        <v>7</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="48">
+        <v>49.026116666666667</v>
+      </c>
+      <c r="D13" s="16"/>
+      <c r="E13" s="22">
+        <v>7</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="48">
+        <v>29.21425</v>
+      </c>
+      <c r="I13" s="16"/>
+      <c r="J13" s="22">
+        <v>7</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M13" s="48">
+        <v>50.73296666666667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="18" customHeight="1">
+      <c r="A14" s="22">
+        <v>8</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="48">
+        <v>48.018916666666669</v>
+      </c>
+      <c r="D14" s="16"/>
+      <c r="E14" s="22">
+        <v>8</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="48">
+        <v>24.410716666666666</v>
+      </c>
+      <c r="I14" s="16"/>
+      <c r="J14" s="22">
+        <v>8</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M14" s="48">
+        <v>48.958783333333336</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="18" customHeight="1">
+      <c r="A15" s="22">
+        <v>9</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="48">
+        <v>45.594850000000001</v>
+      </c>
+      <c r="D15" s="16"/>
+      <c r="E15" s="22">
+        <v>9</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" s="48">
+        <v>24.309000000000001</v>
+      </c>
+      <c r="I15" s="16"/>
+      <c r="J15" s="22">
+        <v>9</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M15" s="48">
+        <v>48.18183333333333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="18" customHeight="1">
+      <c r="A16" s="22">
+        <v>10</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="48">
+        <v>40.329816666666666</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="22">
+        <v>10</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="48">
+        <v>24.288583333333332</v>
+      </c>
+      <c r="I16" s="16"/>
+      <c r="J16" s="22">
+        <v>10</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M16" s="48">
+        <v>48.018916666666669</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="18" customHeight="1">
+      <c r="A17" s="25">
+        <v>11</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="49">
+        <v>35.718649999999997</v>
+      </c>
+      <c r="D17" s="16"/>
+      <c r="E17" s="25">
+        <v>11</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="49">
+        <v>22.241250000000001</v>
+      </c>
+      <c r="I17" s="16"/>
+      <c r="J17" s="25">
+        <v>11</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M17" s="49">
+        <v>44.808483333333335</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="18" customHeight="1">
+      <c r="A18" s="25">
+        <v>12</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="49">
+        <v>33.616900000000001</v>
+      </c>
+      <c r="D18" s="16"/>
+      <c r="E18" s="25">
+        <v>12</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="49">
+        <v>20.280999999999999</v>
+      </c>
+      <c r="I18" s="16"/>
+      <c r="J18" s="25">
+        <v>12</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M18" s="49">
+        <v>42.150483333333334</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="18" customHeight="1">
+      <c r="A19" s="25">
+        <v>13</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="49">
+        <v>31.903949999999998</v>
+      </c>
+      <c r="D19" s="16"/>
+      <c r="E19" s="25">
+        <v>13</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="49">
+        <v>19.142949999999999</v>
+      </c>
+      <c r="I19" s="16"/>
+      <c r="J19" s="25">
+        <v>13</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M19" s="49">
+        <v>39.527966666666664</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="18" customHeight="1">
+      <c r="A20" s="25">
+        <v>14</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="49">
+        <v>31.407283333333332</v>
+      </c>
+      <c r="D20" s="16"/>
+      <c r="E20" s="25">
+        <v>14</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="49">
+        <v>18.520233333333334</v>
+      </c>
+      <c r="I20" s="16"/>
+      <c r="J20" s="25">
+        <v>14</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M20" s="49">
+        <v>36.942366666666665</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="18" customHeight="1">
+      <c r="A21" s="25">
+        <v>15</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" s="49">
+        <v>24.309000000000001</v>
+      </c>
+      <c r="D21" s="16"/>
+      <c r="E21" s="25">
+        <v>15</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="49">
+        <v>17.781416666666665</v>
+      </c>
+      <c r="I21" s="16"/>
+      <c r="J21" s="25">
+        <v>15</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M21" s="49">
+        <v>36.817216666666667</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="18" customHeight="1">
+      <c r="A22" s="28">
+        <v>16</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="50">
+        <v>20.972133333333332</v>
+      </c>
+      <c r="D22" s="16"/>
+      <c r="E22" s="28">
+        <v>16</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="50">
+        <v>16.542566666666666</v>
+      </c>
+      <c r="I22" s="16"/>
+      <c r="J22" s="28">
+        <v>16</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M22" s="50">
+        <v>34.338749999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="18" customHeight="1">
+      <c r="A23" s="28">
+        <v>17</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="50">
+        <v>20.461916666666667</v>
+      </c>
+      <c r="D23" s="16"/>
+      <c r="E23" s="28">
+        <v>17</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="50">
+        <v>16.495349999999998</v>
+      </c>
+      <c r="I23" s="16"/>
+      <c r="J23" s="28">
+        <v>17</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M23" s="50">
+        <v>33.616900000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="18" customHeight="1">
+      <c r="A24" s="28">
+        <v>18</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="50">
+        <v>18.325833333333332</v>
+      </c>
+      <c r="D24" s="16"/>
+      <c r="E24" s="28">
+        <v>18</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="50">
+        <v>16.025633333333332</v>
+      </c>
+      <c r="I24" s="16"/>
+      <c r="J24" s="28">
+        <v>18</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="M24" s="50">
+        <v>31.903949999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="18" customHeight="1">
+      <c r="A25" s="28">
+        <v>19</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="50">
+        <v>16.648416666666666</v>
+      </c>
+      <c r="D25" s="16"/>
+      <c r="E25" s="28">
+        <v>19</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="50">
+        <v>15.550466666666667</v>
+      </c>
+      <c r="I25" s="16"/>
+      <c r="J25" s="28">
+        <v>19</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M25" s="50">
+        <v>31.407283333333332</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="18" customHeight="1">
+      <c r="A26" s="31">
+        <v>20</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="51">
+        <v>16.106083333333334</v>
+      </c>
+      <c r="D26" s="16"/>
+      <c r="E26" s="31">
+        <v>20</v>
+      </c>
+      <c r="F26" s="32" t="s">
+        <v>381</v>
+      </c>
+      <c r="G26" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="H26" s="51">
+        <v>15.534866666666666</v>
+      </c>
+      <c r="I26" s="16"/>
+      <c r="J26" s="31">
+        <v>20</v>
+      </c>
+      <c r="K26" s="32" t="s">
+        <v>303</v>
+      </c>
+      <c r="L26" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="M26" s="51">
+        <v>26.335899999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="18" customHeight="1">
+      <c r="H27" s="52"/>
+      <c r="M27" s="52"/>
+    </row>
+    <row r="28" spans="1:13" ht="18" customHeight="1">
+      <c r="H28" s="52"/>
+      <c r="M28" s="52"/>
+    </row>
+    <row r="29" spans="1:13" ht="18" customHeight="1">
+      <c r="M29" s="52"/>
+    </row>
+    <row r="30" spans="1:13" ht="18" customHeight="1">
+      <c r="M30" s="52"/>
+    </row>
+    <row r="31" spans="1:13" ht="18" customHeight="1">
+      <c r="M31" s="52"/>
+    </row>
+    <row r="32" spans="1:13" ht="18" customHeight="1">
+      <c r="M32" s="52"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="J5:M5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78FB15CD-3CF3-D347-AFBE-4687D9C7F7A8}">
   <sheetPr>
     <tabColor rgb="FFD0D0E8"/>
@@ -6962,7 +9752,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78804AC8-ADD7-1C42-ABEA-3F8E47FF4484}">
   <sheetPr>
     <tabColor rgb="FFD0D0E8"/>
@@ -7891,7 +10681,9 @@
   </sheetPr>
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P34" sqref="P34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="1"/>
   <cols>
@@ -9148,6 +11940,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{781C5DFB-F134-0F44-A1B1-2A7DC516B90C}">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
+  <dimension ref="B35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="35" spans="2:2" ht="18">
+      <c r="B35" s="65" t="s">
+        <v>434</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{857B5291-0177-3A46-8D86-45E363EC2EB1}">
   <sheetPr>
     <tabColor rgb="FFD0D0E8"/>
@@ -10051,7 +12867,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F9BBA47-E472-EF40-AA1C-B80F0BA112C1}">
   <sheetPr>
     <tabColor rgb="FFD0D0E8"/>
@@ -10924,7 +13740,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06290B69-AFB4-A54B-9485-72B4D185A557}">
   <sheetPr>
     <tabColor rgb="FFD0D0E8"/>
@@ -11811,7 +14627,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2FF2007-3DBE-964B-A12A-49C62E463CF1}">
   <sheetPr>
     <tabColor rgb="FFD0D0E8"/>
@@ -12735,7 +15551,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C610154A-6CC7-844A-A29C-6C9B36E0A1A6}">
   <sheetPr>
     <tabColor rgb="FFD0D0E8"/>
@@ -13659,7 +16475,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{941B28FC-8DA9-7540-8219-1EC2A1A48579}">
   <sheetPr>
     <tabColor rgb="FFD0D0E8"/>
@@ -14581,928 +17397,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4368EC2C-E0D7-B443-9AD2-CEC35644FA3F}">
-  <sheetPr>
-    <tabColor rgb="FFD0D0E8"/>
-  </sheetPr>
-  <dimension ref="A1:P32"/>
-  <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="F30" sqref="F30"/>
-      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
-    <col min="4" max="4" width="3" customWidth="1"/>
-    <col min="5" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.1640625" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" style="35" customWidth="1"/>
-    <col min="9" max="9" width="3" customWidth="1"/>
-    <col min="10" max="10" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.83203125" customWidth="1"/>
-    <col min="12" max="12" width="26.33203125" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" style="35" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" ht="22" customHeight="1">
-      <c r="A1" s="36" t="s">
-        <v>375</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-    </row>
-    <row r="2" spans="1:16" ht="18" customHeight="1">
-      <c r="A2" s="37" t="s">
-        <v>318</v>
-      </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-    </row>
-    <row r="3" spans="1:16" ht="18" customHeight="1">
-      <c r="A3" s="38" t="s">
-        <v>319</v>
-      </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-    </row>
-    <row r="4" spans="1:16" ht="16" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="8"/>
-    </row>
-    <row r="5" spans="1:16" s="9" customFormat="1" ht="18" customHeight="1">
-      <c r="A5" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="E5" s="39" t="s">
-        <v>131</v>
-      </c>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="J5" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-    </row>
-    <row r="6" spans="1:16" ht="18" customHeight="1">
-      <c r="A6" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="M6" s="12" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="18" customHeight="1">
-      <c r="A7" s="13">
-        <v>1</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="46">
-        <v>280.16663333333332</v>
-      </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="13">
-        <v>1</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="46">
-        <v>50.24131666666667</v>
-      </c>
-      <c r="I7" s="16"/>
-      <c r="J7" s="13">
-        <v>1</v>
-      </c>
-      <c r="K7" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="L7" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="M7" s="46">
-        <v>231.46773333333334</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="18" customHeight="1">
-      <c r="A8" s="18">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="47">
-        <v>236.99503333333334</v>
-      </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="18">
-        <v>2</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="47">
-        <v>43.256316666666663</v>
-      </c>
-      <c r="I8" s="16"/>
-      <c r="J8" s="18">
-        <v>2</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M8" s="47">
-        <v>176.28213333333332</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="18" customHeight="1">
-      <c r="A9" s="18">
-        <v>3</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="47">
-        <v>221.81710000000001</v>
-      </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="18">
-        <v>3</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="47">
-        <v>33.327750000000002</v>
-      </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="18">
-        <v>3</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M9" s="47">
-        <v>161.66909999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="18" customHeight="1">
-      <c r="A10" s="18">
-        <v>4</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="47">
-        <v>214.98765</v>
-      </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="18">
-        <v>4</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="47">
-        <v>33.103883333333336</v>
-      </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="18">
-        <v>4</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M10" s="47">
-        <v>92.383766666666673</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="18" customHeight="1">
-      <c r="A11" s="18">
-        <v>5</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="47">
-        <v>88.191900000000004</v>
-      </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="18">
-        <v>5</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="47">
-        <v>30.018733333333333</v>
-      </c>
-      <c r="I11" s="16"/>
-      <c r="J11" s="18">
-        <v>5</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M11" s="47">
-        <v>73.807516666666672</v>
-      </c>
-      <c r="P11" s="21"/>
-    </row>
-    <row r="12" spans="1:16" ht="18" customHeight="1">
-      <c r="A12" s="22">
-        <v>6</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="48">
-        <v>72.265533333333337</v>
-      </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="22">
-        <v>6</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" s="48">
-        <v>29.276833333333332</v>
-      </c>
-      <c r="I12" s="16"/>
-      <c r="J12" s="22">
-        <v>6</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M12" s="48">
-        <v>60.649433333333334</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="18" customHeight="1">
-      <c r="A13" s="22">
-        <v>7</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="48">
-        <v>49.026116666666667</v>
-      </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="22">
-        <v>7</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="48">
-        <v>29.21425</v>
-      </c>
-      <c r="I13" s="16"/>
-      <c r="J13" s="22">
-        <v>7</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M13" s="48">
-        <v>50.73296666666667</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="18" customHeight="1">
-      <c r="A14" s="22">
-        <v>8</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="48">
-        <v>48.018916666666669</v>
-      </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="22">
-        <v>8</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="48">
-        <v>24.410716666666666</v>
-      </c>
-      <c r="I14" s="16"/>
-      <c r="J14" s="22">
-        <v>8</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M14" s="48">
-        <v>48.958783333333336</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="18" customHeight="1">
-      <c r="A15" s="22">
-        <v>9</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="48">
-        <v>45.594850000000001</v>
-      </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="22">
-        <v>9</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="H15" s="48">
-        <v>24.309000000000001</v>
-      </c>
-      <c r="I15" s="16"/>
-      <c r="J15" s="22">
-        <v>9</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="M15" s="48">
-        <v>48.18183333333333</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="18" customHeight="1">
-      <c r="A16" s="22">
-        <v>10</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="48">
-        <v>40.329816666666666</v>
-      </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="22">
-        <v>10</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H16" s="48">
-        <v>24.288583333333332</v>
-      </c>
-      <c r="I16" s="16"/>
-      <c r="J16" s="22">
-        <v>10</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="M16" s="48">
-        <v>48.018916666666669</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="18" customHeight="1">
-      <c r="A17" s="25">
-        <v>11</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="49">
-        <v>35.718649999999997</v>
-      </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="25">
-        <v>11</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H17" s="49">
-        <v>22.241250000000001</v>
-      </c>
-      <c r="I17" s="16"/>
-      <c r="J17" s="25">
-        <v>11</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M17" s="49">
-        <v>44.808483333333335</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="18" customHeight="1">
-      <c r="A18" s="25">
-        <v>12</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="49">
-        <v>33.616900000000001</v>
-      </c>
-      <c r="D18" s="16"/>
-      <c r="E18" s="25">
-        <v>12</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" s="49">
-        <v>20.280999999999999</v>
-      </c>
-      <c r="I18" s="16"/>
-      <c r="J18" s="25">
-        <v>12</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M18" s="49">
-        <v>42.150483333333334</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="18" customHeight="1">
-      <c r="A19" s="25">
-        <v>13</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" s="49">
-        <v>31.903949999999998</v>
-      </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="25">
-        <v>13</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="49">
-        <v>19.142949999999999</v>
-      </c>
-      <c r="I19" s="16"/>
-      <c r="J19" s="25">
-        <v>13</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="M19" s="49">
-        <v>39.527966666666664</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="18" customHeight="1">
-      <c r="A20" s="25">
-        <v>14</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20" s="49">
-        <v>31.407283333333332</v>
-      </c>
-      <c r="D20" s="16"/>
-      <c r="E20" s="25">
-        <v>14</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="49">
-        <v>18.520233333333334</v>
-      </c>
-      <c r="I20" s="16"/>
-      <c r="J20" s="25">
-        <v>14</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M20" s="49">
-        <v>36.942366666666665</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="18" customHeight="1">
-      <c r="A21" s="25">
-        <v>15</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C21" s="49">
-        <v>24.309000000000001</v>
-      </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="25">
-        <v>15</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>378</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" s="49">
-        <v>17.781416666666665</v>
-      </c>
-      <c r="I21" s="16"/>
-      <c r="J21" s="25">
-        <v>15</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M21" s="49">
-        <v>36.817216666666667</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="18" customHeight="1">
-      <c r="A22" s="28">
-        <v>16</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="50">
-        <v>20.972133333333332</v>
-      </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="28">
-        <v>16</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="50">
-        <v>16.542566666666666</v>
-      </c>
-      <c r="I22" s="16"/>
-      <c r="J22" s="28">
-        <v>16</v>
-      </c>
-      <c r="K22" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="L22" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="M22" s="50">
-        <v>34.338749999999997</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="18" customHeight="1">
-      <c r="A23" s="28">
-        <v>17</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23" s="50">
-        <v>20.461916666666667</v>
-      </c>
-      <c r="D23" s="16"/>
-      <c r="E23" s="28">
-        <v>17</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H23" s="50">
-        <v>16.495349999999998</v>
-      </c>
-      <c r="I23" s="16"/>
-      <c r="J23" s="28">
-        <v>17</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="M23" s="50">
-        <v>33.616900000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="18" customHeight="1">
-      <c r="A24" s="28">
-        <v>18</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" s="50">
-        <v>18.325833333333332</v>
-      </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="28">
-        <v>18</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H24" s="50">
-        <v>16.025633333333332</v>
-      </c>
-      <c r="I24" s="16"/>
-      <c r="J24" s="28">
-        <v>18</v>
-      </c>
-      <c r="K24" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="M24" s="50">
-        <v>31.903949999999998</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="18" customHeight="1">
-      <c r="A25" s="28">
-        <v>19</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="50">
-        <v>16.648416666666666</v>
-      </c>
-      <c r="D25" s="16"/>
-      <c r="E25" s="28">
-        <v>19</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>379</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H25" s="50">
-        <v>15.550466666666667</v>
-      </c>
-      <c r="I25" s="16"/>
-      <c r="J25" s="28">
-        <v>19</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="L25" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="M25" s="50">
-        <v>31.407283333333332</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="18" customHeight="1">
-      <c r="A26" s="31">
-        <v>20</v>
-      </c>
-      <c r="B26" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="51">
-        <v>16.106083333333334</v>
-      </c>
-      <c r="D26" s="16"/>
-      <c r="E26" s="31">
-        <v>20</v>
-      </c>
-      <c r="F26" s="32" t="s">
-        <v>381</v>
-      </c>
-      <c r="G26" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" s="51">
-        <v>15.534866666666666</v>
-      </c>
-      <c r="I26" s="16"/>
-      <c r="J26" s="31">
-        <v>20</v>
-      </c>
-      <c r="K26" s="32" t="s">
-        <v>303</v>
-      </c>
-      <c r="L26" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="M26" s="51">
-        <v>26.335899999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="18" customHeight="1">
-      <c r="H27" s="52"/>
-      <c r="M27" s="52"/>
-    </row>
-    <row r="28" spans="1:13" ht="18" customHeight="1">
-      <c r="H28" s="52"/>
-      <c r="M28" s="52"/>
-    </row>
-    <row r="29" spans="1:13" ht="18" customHeight="1">
-      <c r="M29" s="52"/>
-    </row>
-    <row r="30" spans="1:13" ht="18" customHeight="1">
-      <c r="M30" s="52"/>
-    </row>
-    <row r="31" spans="1:13" ht="18" customHeight="1">
-      <c r="M31" s="52"/>
-    </row>
-    <row r="32" spans="1:13" ht="18" customHeight="1">
-      <c r="M32" s="52"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="J5:M5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>